<commit_message>
I added combine redux and usage in the thunk module, and connected to Firestore Firebase
</commit_message>
<xml_diff>
--- a/Final-React-Project-Design.xlsx
+++ b/Final-React-Project-Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basheer\Desktop\בשיר\Full Stack Work\Full Stack Cors - YanivArad\Projects\React-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DA398C-38D8-4E14-B055-5BDDE4DACE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E34C06-E911-4347-827F-1F5AE30041F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="238">
   <si>
     <t>Num</t>
   </si>
@@ -5019,9 +5019,6 @@
     <t>18/11/23</t>
   </si>
   <si>
-    <t>18-19/11/23</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -5079,12 +5076,224 @@
   <si>
     <t>28/11/23</t>
   </si>
+  <si>
+    <t>18-20/11/23</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">npm install </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Univers"/>
+        <family val="2"/>
+      </rPr>
+      <t>redux-thunk</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>import</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> { createStore, applyMiddleware } </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFD73A49"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF032F62"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'redux'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>import</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> thunk </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFD73A49"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF032F62"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'redux-thunk'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>import</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> rootReducer </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFD73A49"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF032F62"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'./reducers/index'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>const</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> store </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF005CC5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>createStore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(rootReducer, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF6F42C1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>applyMiddleware</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(thunk))</t>
+    </r>
+  </si>
+  <si>
+    <t>src/redux/store.js</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="59">
+  <fonts count="64">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5477,6 +5686,36 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFD73A49"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF032F62"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF005CC5"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF6F42C1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -5558,7 +5797,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -6057,12 +6296,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -6339,6 +6617,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6348,13 +6650,34 @@
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6411,9 +6734,6 @@
     <xf numFmtId="0" fontId="19" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6425,51 +6745,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6483,16 +6758,19 @@
     <xf numFmtId="0" fontId="25" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6535,6 +6813,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -38841,7 +39155,7 @@
   <dimension ref="B3:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15"/>
@@ -38990,9 +39304,11 @@
         <v>143</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="46">
@@ -39005,9 +39321,11 @@
         <v>144</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="46">
@@ -39020,9 +39338,11 @@
         <v>145</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="46">
@@ -39035,9 +39355,11 @@
         <v>142</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="46">
@@ -39125,7 +39447,7 @@
         <v>161</v>
       </c>
       <c r="E22" s="46" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -39134,13 +39456,13 @@
         <v>15</v>
       </c>
       <c r="C23" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="D23" s="46" t="s">
         <v>227</v>
       </c>
-      <c r="D23" s="46" t="s">
-        <v>228</v>
-      </c>
       <c r="E23" s="46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F23" s="1"/>
     </row>
@@ -39149,13 +39471,13 @@
         <v>16</v>
       </c>
       <c r="C24" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D24" s="46" t="s">
         <v>163</v>
       </c>
       <c r="E24" s="46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -39246,10 +39568,10 @@
     <tabColor rgb="FF00B0F0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G79"/>
+  <dimension ref="A2:G89"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52:G53"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39263,36 +39585,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="51.75" customHeight="1">
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="121" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" thickBot="1">
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B4" s="133" t="s">
+      <c r="B4" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="100" t="s">
+      <c r="C4" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="100" t="s">
+      <c r="D4" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="100" t="s">
+      <c r="E4" s="108" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="141"/>
+      <c r="F4" s="119"/>
     </row>
     <row r="5" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B5" s="134"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
       <c r="E5" s="31" t="s">
         <v>9</v>
       </c>
@@ -39300,658 +39622,750 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B6" s="33">
+    <row r="6" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B6" s="126">
         <v>1</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="72" t="s">
+      <c r="D6" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="171" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="22.5">
-      <c r="B7" s="129">
+    <row r="7" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B7" s="127"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="102" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="136" t="s">
+        <v>237</v>
+      </c>
+      <c r="F7" s="172" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B8" s="127"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="139"/>
+      <c r="E8" s="137"/>
+      <c r="F8" s="172" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B9" s="127"/>
+      <c r="C9" s="124"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="172" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B10" s="127"/>
+      <c r="C10" s="124"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="173"/>
+    </row>
+    <row r="11" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
+      <c r="B11" s="175"/>
+      <c r="C11" s="170"/>
+      <c r="D11" s="176"/>
+      <c r="E11" s="177"/>
+      <c r="F11" s="174" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="22.5">
+      <c r="B12" s="115">
         <v>2</v>
       </c>
-      <c r="C7" s="135" t="s">
+      <c r="C12" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="103" t="s">
+      <c r="D12" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="131" t="s">
+      <c r="E12" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F12" s="38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="22.5">
-      <c r="B8" s="130"/>
-      <c r="C8" s="136"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="20" t="s">
+    <row r="13" spans="2:6" ht="22.5">
+      <c r="B13" s="116"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="107"/>
+      <c r="F13" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="22.5">
-      <c r="B9" s="130"/>
-      <c r="C9" s="136"/>
-      <c r="D9" s="104"/>
-      <c r="E9" s="132"/>
-      <c r="F9" s="21" t="s">
+    <row r="14" spans="2:6" ht="22.5">
+      <c r="B14" s="116"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="107"/>
+      <c r="F14" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="22.5">
-      <c r="B10" s="130"/>
-      <c r="C10" s="136"/>
-      <c r="D10" s="104"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="22" t="s">
+    <row r="15" spans="2:6" ht="22.5">
+      <c r="B15" s="116"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="101"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="22.5">
-      <c r="B11" s="130"/>
-      <c r="C11" s="136"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="132"/>
-      <c r="F11" s="23" t="s">
+    <row r="16" spans="2:6" ht="22.5">
+      <c r="B16" s="116"/>
+      <c r="C16" s="104"/>
+      <c r="D16" s="101"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="22.5">
-      <c r="B12" s="130"/>
-      <c r="C12" s="136"/>
-      <c r="D12" s="104"/>
-      <c r="E12" s="132"/>
-      <c r="F12" s="23" t="s">
+    <row r="17" spans="2:6" ht="22.5">
+      <c r="B17" s="116"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="22.5">
-      <c r="B13" s="130"/>
-      <c r="C13" s="136"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="132"/>
-      <c r="F13" s="23" t="s">
+    <row r="18" spans="2:6" ht="22.5">
+      <c r="B18" s="116"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="101"/>
+      <c r="E18" s="107"/>
+      <c r="F18" s="23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B14" s="140"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="40" t="s">
+    <row r="19" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
+      <c r="B19" s="117"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F19" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B15" s="129">
+    <row r="20" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B20" s="115">
         <v>3</v>
       </c>
-      <c r="C15" s="135" t="s">
+      <c r="C20" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="103" t="s">
+      <c r="D20" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="131" t="s">
+      <c r="E20" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="41" t="s">
+      <c r="F20" s="41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B16" s="130"/>
-      <c r="C16" s="136"/>
-      <c r="D16" s="104"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="25" t="s">
+    <row r="21" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B21" s="116"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="101"/>
+      <c r="E21" s="107"/>
+      <c r="F21" s="25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B17" s="130"/>
-      <c r="C17" s="136"/>
-      <c r="D17" s="104"/>
-      <c r="E17" s="132"/>
-      <c r="F17" s="26" t="s">
+    <row r="22" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B22" s="116"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="101"/>
+      <c r="E22" s="107"/>
+      <c r="F22" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B18" s="130"/>
-      <c r="C18" s="136"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="132"/>
-      <c r="F18" s="26" t="s">
+    <row r="23" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B23" s="116"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="101"/>
+      <c r="E23" s="107"/>
+      <c r="F23" s="26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B19" s="130"/>
-      <c r="C19" s="136"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="132"/>
-      <c r="F19" s="27" t="s">
+    <row r="24" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B24" s="116"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="101"/>
+      <c r="E24" s="107"/>
+      <c r="F24" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B20" s="140"/>
-      <c r="C20" s="137"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="40" t="s">
+    <row r="25" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
+      <c r="B25" s="117"/>
+      <c r="C25" s="105"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="42" t="s">
+      <c r="F25" s="42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="22.5">
-      <c r="B21" s="129">
+    <row r="26" spans="2:6" ht="22.5">
+      <c r="B26" s="115">
         <v>4</v>
       </c>
-      <c r="C21" s="135" t="s">
+      <c r="C26" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="103" t="s">
+      <c r="D26" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="131" t="s">
+      <c r="E26" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="41" t="s">
+      <c r="F26" s="41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="22.5">
-      <c r="B22" s="130"/>
-      <c r="C22" s="136"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="132"/>
-      <c r="F22" s="28" t="s">
+    <row r="27" spans="2:6" ht="22.5">
+      <c r="B27" s="116"/>
+      <c r="C27" s="104"/>
+      <c r="D27" s="101"/>
+      <c r="E27" s="107"/>
+      <c r="F27" s="28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="22.5">
-      <c r="B23" s="130"/>
-      <c r="C23" s="136"/>
-      <c r="D23" s="104"/>
-      <c r="E23" s="132"/>
-      <c r="F23" s="29" t="s">
+    <row r="28" spans="2:6" ht="22.5">
+      <c r="B28" s="116"/>
+      <c r="C28" s="104"/>
+      <c r="D28" s="101"/>
+      <c r="E28" s="107"/>
+      <c r="F28" s="29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="42" customHeight="1" thickBot="1">
-      <c r="B24" s="120"/>
-      <c r="C24" s="142"/>
-      <c r="D24" s="124"/>
-      <c r="E24" s="12" t="s">
+    <row r="29" spans="2:6" ht="42" customHeight="1" thickBot="1">
+      <c r="B29" s="135"/>
+      <c r="C29" s="120"/>
+      <c r="D29" s="102"/>
+      <c r="E29" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="24" t="s">
+      <c r="F29" s="24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B25" s="33">
+    <row r="30" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
+      <c r="B30" s="33">
         <v>5</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C30" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="72" t="s">
+      <c r="D30" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="36" t="s">
+      <c r="E30" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="43" t="s">
+      <c r="F30" s="43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B26" s="129">
+    <row r="31" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B31" s="115">
         <v>6</v>
       </c>
-      <c r="C26" s="135" t="s">
+      <c r="C31" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="138" t="s">
+      <c r="D31" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="131" t="s">
+      <c r="E31" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="41" t="s">
+      <c r="F31" s="41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B27" s="130"/>
-      <c r="C27" s="136"/>
-      <c r="D27" s="139"/>
-      <c r="E27" s="132"/>
-      <c r="F27" s="30" t="s">
+    <row r="32" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B32" s="116"/>
+      <c r="C32" s="104"/>
+      <c r="D32" s="114"/>
+      <c r="E32" s="107"/>
+      <c r="F32" s="30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B28" s="140"/>
-      <c r="C28" s="137"/>
-      <c r="D28" s="39" t="s">
+    <row r="33" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
+      <c r="B33" s="117"/>
+      <c r="C33" s="105"/>
+      <c r="D33" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="40" t="s">
+      <c r="E33" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="44"/>
+      <c r="F33" s="44"/>
     </row>
-    <row r="29" spans="2:6" ht="45" customHeight="1" thickBot="1">
-      <c r="B29" s="33">
+    <row r="34" spans="2:6" ht="45" customHeight="1" thickBot="1">
+      <c r="B34" s="33">
         <v>7</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C34" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D34" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="36" t="s">
+      <c r="E34" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="43" t="s">
+      <c r="F34" s="43" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B30" s="33">
+    <row r="35" spans="2:6" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B35" s="33">
         <v>8</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C35" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="72" t="s">
+      <c r="D35" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="E30" s="36" t="s">
+      <c r="E35" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="F30" s="37" t="s">
+      <c r="F35" s="37" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B31" s="111">
+    <row r="36" spans="2:6" ht="42.75" customHeight="1">
+      <c r="B36" s="126">
         <v>9</v>
       </c>
-      <c r="C31" s="108" t="s">
+      <c r="C36" s="123" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="73" t="s">
+      <c r="D36" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E36" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="F31" s="38" t="s">
+      <c r="F36" s="38" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B32" s="112"/>
-      <c r="C32" s="109"/>
-      <c r="D32" s="124" t="s">
+    <row r="37" spans="2:6" ht="42.75" customHeight="1">
+      <c r="B37" s="127"/>
+      <c r="C37" s="124"/>
+      <c r="D37" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="E32" s="121" t="s">
+      <c r="E37" s="136" t="s">
         <v>96</v>
       </c>
-      <c r="F32" s="55" t="s">
+      <c r="F37" s="55" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B33" s="112"/>
-      <c r="C33" s="109"/>
-      <c r="D33" s="125"/>
-      <c r="E33" s="122"/>
-      <c r="F33" s="51" t="s">
+    <row r="38" spans="2:6" ht="42.75" customHeight="1">
+      <c r="B38" s="127"/>
+      <c r="C38" s="124"/>
+      <c r="D38" s="139"/>
+      <c r="E38" s="137"/>
+      <c r="F38" s="51" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B34" s="112"/>
-      <c r="C34" s="109"/>
-      <c r="D34" s="125"/>
-      <c r="E34" s="122"/>
-      <c r="F34" s="51" t="s">
+    <row r="39" spans="2:6" ht="42.75" customHeight="1">
+      <c r="B39" s="127"/>
+      <c r="C39" s="124"/>
+      <c r="D39" s="139"/>
+      <c r="E39" s="137"/>
+      <c r="F39" s="51" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B35" s="112"/>
-      <c r="C35" s="109"/>
-      <c r="D35" s="125"/>
-      <c r="E35" s="123"/>
-      <c r="F35" s="56" t="s">
+    <row r="40" spans="2:6" ht="42.75" customHeight="1">
+      <c r="B40" s="127"/>
+      <c r="C40" s="124"/>
+      <c r="D40" s="139"/>
+      <c r="E40" s="138"/>
+      <c r="F40" s="56" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B36" s="112"/>
-      <c r="C36" s="109"/>
-      <c r="D36" s="125"/>
-      <c r="E36" s="121" t="s">
+    <row r="41" spans="2:6" ht="42.75" customHeight="1">
+      <c r="B41" s="127"/>
+      <c r="C41" s="124"/>
+      <c r="D41" s="139"/>
+      <c r="E41" s="136" t="s">
         <v>98</v>
       </c>
-      <c r="F36" s="57" t="s">
+      <c r="F41" s="57" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B37" s="112"/>
-      <c r="C37" s="109"/>
-      <c r="D37" s="125"/>
-      <c r="E37" s="122"/>
-      <c r="F37" s="58" t="s">
+    <row r="42" spans="2:6" ht="42.75" customHeight="1">
+      <c r="B42" s="127"/>
+      <c r="C42" s="124"/>
+      <c r="D42" s="139"/>
+      <c r="E42" s="137"/>
+      <c r="F42" s="58" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B38" s="112"/>
-      <c r="C38" s="109"/>
-      <c r="D38" s="125"/>
-      <c r="E38" s="122"/>
-      <c r="F38" s="58" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B39" s="112"/>
-      <c r="C39" s="109"/>
-      <c r="D39" s="125"/>
-      <c r="E39" s="122"/>
-      <c r="F39" s="59" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B40" s="112"/>
-      <c r="C40" s="109"/>
-      <c r="D40" s="125"/>
-      <c r="E40" s="122"/>
-      <c r="F40" s="59" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B41" s="112"/>
-      <c r="C41" s="109"/>
-      <c r="D41" s="126"/>
-      <c r="E41" s="123"/>
-      <c r="F41" s="60" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" ht="75">
-      <c r="B42" s="112"/>
-      <c r="C42" s="109"/>
-      <c r="D42" s="124" t="s">
-        <v>97</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F42" s="61" t="s">
-        <v>107</v>
-      </c>
-    </row>
     <row r="43" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B43" s="112"/>
-      <c r="C43" s="109"/>
-      <c r="D43" s="125"/>
-      <c r="E43" s="127" t="s">
-        <v>109</v>
-      </c>
+      <c r="B43" s="127"/>
+      <c r="C43" s="124"/>
+      <c r="D43" s="139"/>
+      <c r="E43" s="137"/>
       <c r="F43" s="58" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B44" s="112"/>
-      <c r="C44" s="109"/>
-      <c r="D44" s="125"/>
-      <c r="E44" s="127"/>
+      <c r="B44" s="127"/>
+      <c r="C44" s="124"/>
+      <c r="D44" s="139"/>
+      <c r="E44" s="137"/>
       <c r="F44" s="59" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B45" s="112"/>
-      <c r="C45" s="109"/>
-      <c r="D45" s="125"/>
-      <c r="E45" s="127"/>
+      <c r="B45" s="127"/>
+      <c r="C45" s="124"/>
+      <c r="D45" s="139"/>
+      <c r="E45" s="137"/>
       <c r="F45" s="59" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B46" s="113"/>
-      <c r="C46" s="110"/>
-      <c r="D46" s="126"/>
-      <c r="E46" s="128"/>
+      <c r="B46" s="127"/>
+      <c r="C46" s="124"/>
+      <c r="D46" s="140"/>
+      <c r="E46" s="138"/>
       <c r="F46" s="60" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B47" s="120">
+    <row r="47" spans="2:6" ht="75">
+      <c r="B47" s="127"/>
+      <c r="C47" s="124"/>
+      <c r="D47" s="102" t="s">
+        <v>97</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F47" s="61" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="42.75" customHeight="1">
+      <c r="B48" s="127"/>
+      <c r="C48" s="124"/>
+      <c r="D48" s="139"/>
+      <c r="E48" s="141" t="s">
+        <v>109</v>
+      </c>
+      <c r="F48" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="42.75" customHeight="1">
+      <c r="B49" s="127"/>
+      <c r="C49" s="124"/>
+      <c r="D49" s="139"/>
+      <c r="E49" s="141"/>
+      <c r="F49" s="59" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="42.75" customHeight="1">
+      <c r="B50" s="127"/>
+      <c r="C50" s="124"/>
+      <c r="D50" s="139"/>
+      <c r="E50" s="141"/>
+      <c r="F50" s="59" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="42.75" customHeight="1">
+      <c r="B51" s="128"/>
+      <c r="C51" s="125"/>
+      <c r="D51" s="140"/>
+      <c r="E51" s="142"/>
+      <c r="F51" s="60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="42.75" customHeight="1">
+      <c r="B52" s="135">
         <v>10</v>
       </c>
-      <c r="C47" s="117" t="s">
+      <c r="C52" s="132" t="s">
         <v>117</v>
       </c>
-      <c r="D47" s="114" t="s">
+      <c r="D52" s="129" t="s">
         <v>126</v>
       </c>
-      <c r="E47" s="121" t="s">
+      <c r="E52" s="136" t="s">
         <v>118</v>
       </c>
-      <c r="F47" s="62" t="s">
+      <c r="F52" s="62" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B48" s="112"/>
-      <c r="C48" s="118"/>
-      <c r="D48" s="115"/>
-      <c r="E48" s="122"/>
-      <c r="F48" s="62" t="s">
+    <row r="53" spans="2:7" ht="42.75" customHeight="1">
+      <c r="B53" s="127"/>
+      <c r="C53" s="133"/>
+      <c r="D53" s="130"/>
+      <c r="E53" s="137"/>
+      <c r="F53" s="62" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B49" s="112"/>
-      <c r="C49" s="118"/>
-      <c r="D49" s="115"/>
-      <c r="E49" s="122"/>
-      <c r="F49" s="63" t="s">
+    <row r="54" spans="2:7" ht="42.75" customHeight="1">
+      <c r="B54" s="127"/>
+      <c r="C54" s="133"/>
+      <c r="D54" s="130"/>
+      <c r="E54" s="137"/>
+      <c r="F54" s="63" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B50" s="112"/>
-      <c r="C50" s="118"/>
-      <c r="D50" s="115"/>
-      <c r="E50" s="122"/>
-      <c r="F50" s="62" t="s">
+    <row r="55" spans="2:7" ht="42.75" customHeight="1">
+      <c r="B55" s="127"/>
+      <c r="C55" s="133"/>
+      <c r="D55" s="130"/>
+      <c r="E55" s="137"/>
+      <c r="F55" s="62" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="51" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B51" s="113"/>
-      <c r="C51" s="119"/>
-      <c r="D51" s="116"/>
-      <c r="E51" s="123"/>
-      <c r="F51" s="62" t="s">
+    <row r="56" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B56" s="128"/>
+      <c r="C56" s="134"/>
+      <c r="D56" s="131"/>
+      <c r="E56" s="138"/>
+      <c r="F56" s="62" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B52" s="33"/>
-      <c r="C52" s="34" t="s">
+    <row r="57" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B57" s="33"/>
+      <c r="C57" s="123" t="s">
         <v>211</v>
       </c>
-      <c r="D52" s="72" t="s">
+      <c r="D57" s="72" t="s">
         <v>212</v>
       </c>
-      <c r="E52" s="36" t="s">
+      <c r="E57" s="36" t="s">
         <v>215</v>
       </c>
-      <c r="F52" s="37" t="s">
+      <c r="F57" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="G52" s="102" t="s">
+      <c r="G57" s="110" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B53" s="33"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="72" t="s">
+    <row r="58" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B58" s="33"/>
+      <c r="C58" s="170"/>
+      <c r="D58" s="72" t="s">
         <v>213</v>
       </c>
-      <c r="E53" s="36" t="s">
+      <c r="E58" s="36" t="s">
         <v>216</v>
       </c>
-      <c r="F53" s="37" t="s">
+      <c r="F58" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="G53" s="102"/>
+      <c r="G58" s="110"/>
     </row>
-    <row r="54" spans="2:7" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B54" s="8"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="50"/>
+    <row r="59" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B59" s="166"/>
+      <c r="C59" s="167"/>
+      <c r="D59" s="168"/>
+      <c r="E59" s="169"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="93"/>
     </row>
-    <row r="55" spans="2:7" s="92" customFormat="1" ht="45.75" customHeight="1">
-      <c r="G55" s="102"/>
-    </row>
-    <row r="56" spans="2:7" s="92" customFormat="1" ht="45.75" customHeight="1">
-      <c r="G56" s="102"/>
-    </row>
-    <row r="57" spans="2:7" s="92" customFormat="1" ht="43.5" customHeight="1">
-      <c r="G57" s="93"/>
-    </row>
-    <row r="58" spans="2:7" s="92" customFormat="1" ht="43.5" customHeight="1">
-      <c r="G58" s="93"/>
-    </row>
-    <row r="60" spans="2:7" s="92" customFormat="1" ht="43.5" customHeight="1">
+    <row r="60" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B60" s="166"/>
+      <c r="C60" s="167"/>
+      <c r="D60" s="168"/>
+      <c r="E60" s="169"/>
+      <c r="F60" s="14"/>
       <c r="G60" s="93"/>
     </row>
-    <row r="61" spans="2:7" s="92" customFormat="1" ht="31.5" customHeight="1">
+    <row r="61" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B61" s="166"/>
+      <c r="C61" s="167"/>
+      <c r="D61" s="168"/>
+      <c r="E61" s="169"/>
+      <c r="F61" s="14"/>
       <c r="G61" s="93"/>
     </row>
-    <row r="62" spans="2:7" s="92" customFormat="1" ht="31.5" customHeight="1">
+    <row r="62" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B62" s="166"/>
+      <c r="C62" s="167"/>
+      <c r="D62" s="168"/>
+      <c r="E62" s="169"/>
+      <c r="F62" s="14"/>
       <c r="G62" s="93"/>
     </row>
-    <row r="63" spans="2:7" s="92" customFormat="1" ht="31.5" customHeight="1">
+    <row r="63" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B63" s="166"/>
+      <c r="C63" s="167"/>
+      <c r="D63" s="168"/>
+      <c r="E63" s="169"/>
+      <c r="F63" s="14"/>
       <c r="G63" s="93"/>
     </row>
-    <row r="64" spans="2:7" s="92" customFormat="1" ht="31.5" customHeight="1">
-      <c r="G64" s="93"/>
+    <row r="64" spans="2:7" ht="34.5" customHeight="1" thickBot="1">
+      <c r="B64" s="8"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="50"/>
     </row>
-    <row r="65" spans="6:7" s="92" customFormat="1" ht="20.25">
-      <c r="G65" s="93"/>
+    <row r="65" spans="6:7" s="92" customFormat="1" ht="45.75" customHeight="1">
+      <c r="G65" s="110"/>
     </row>
-    <row r="66" spans="6:7" ht="22.5">
-      <c r="F66" s="11"/>
+    <row r="66" spans="6:7" s="92" customFormat="1" ht="45.75" customHeight="1">
+      <c r="G66" s="110"/>
     </row>
-    <row r="67" spans="6:7" ht="22.5">
-      <c r="F67" s="52"/>
+    <row r="67" spans="6:7" s="92" customFormat="1" ht="43.5" customHeight="1">
+      <c r="G67" s="93"/>
     </row>
-    <row r="68" spans="6:7" ht="22.5">
-      <c r="F68" s="52"/>
+    <row r="68" spans="6:7" s="92" customFormat="1" ht="43.5" customHeight="1">
+      <c r="G68" s="93"/>
     </row>
-    <row r="69" spans="6:7" ht="22.5">
-      <c r="F69" s="52"/>
+    <row r="70" spans="6:7" s="92" customFormat="1" ht="43.5" customHeight="1">
+      <c r="G70" s="93"/>
     </row>
-    <row r="70" spans="6:7" ht="22.5">
-      <c r="F70" s="53"/>
+    <row r="71" spans="6:7" s="92" customFormat="1" ht="31.5" customHeight="1">
+      <c r="G71" s="93"/>
     </row>
-    <row r="71" spans="6:7" ht="22.5">
-      <c r="F71" s="53"/>
+    <row r="72" spans="6:7" s="92" customFormat="1" ht="31.5" customHeight="1">
+      <c r="G72" s="93"/>
     </row>
-    <row r="72" spans="6:7" ht="22.5">
-      <c r="F72" s="54"/>
+    <row r="73" spans="6:7" s="92" customFormat="1" ht="31.5" customHeight="1">
+      <c r="G73" s="93"/>
+    </row>
+    <row r="74" spans="6:7" s="92" customFormat="1" ht="31.5" customHeight="1">
+      <c r="G74" s="93"/>
+    </row>
+    <row r="75" spans="6:7" s="92" customFormat="1" ht="20.25">
+      <c r="G75" s="93"/>
     </row>
     <row r="76" spans="6:7" ht="22.5">
-      <c r="F76" s="52"/>
+      <c r="F76" s="11"/>
     </row>
     <row r="77" spans="6:7" ht="22.5">
-      <c r="F77" s="53"/>
+      <c r="F77" s="52"/>
     </row>
     <row r="78" spans="6:7" ht="22.5">
-      <c r="F78" s="53"/>
+      <c r="F78" s="52"/>
     </row>
     <row r="79" spans="6:7" ht="22.5">
-      <c r="F79" s="54"/>
+      <c r="F79" s="52"/>
+    </row>
+    <row r="80" spans="6:7" ht="22.5">
+      <c r="F80" s="53"/>
+    </row>
+    <row r="81" spans="6:6" ht="22.5">
+      <c r="F81" s="53"/>
+    </row>
+    <row r="82" spans="6:6" ht="22.5">
+      <c r="F82" s="54"/>
+    </row>
+    <row r="86" spans="6:6" ht="22.5">
+      <c r="F86" s="52"/>
+    </row>
+    <row r="87" spans="6:6" ht="22.5">
+      <c r="F87" s="53"/>
+    </row>
+    <row r="88" spans="6:6" ht="22.5">
+      <c r="F88" s="53"/>
+    </row>
+    <row r="89" spans="6:6" ht="22.5">
+      <c r="F89" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="D21:D24"/>
-    <mergeCell ref="C7:C14"/>
-    <mergeCell ref="E21:E23"/>
+  <mergeCells count="39">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="C36:C51"/>
+    <mergeCell ref="B36:B51"/>
+    <mergeCell ref="D52:D56"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="E52:E56"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="D37:D46"/>
+    <mergeCell ref="D47:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="E12:E18"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D12:D19"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="C12:C19"/>
+    <mergeCell ref="E26:E28"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="E15:E19"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="D15:D20"/>
-    <mergeCell ref="B7:B14"/>
-    <mergeCell ref="E7:E13"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="D7:D14"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="C31:C46"/>
-    <mergeCell ref="B31:B46"/>
-    <mergeCell ref="D47:D51"/>
-    <mergeCell ref="C47:C51"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="E47:E51"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="E36:E41"/>
-    <mergeCell ref="D32:D41"/>
-    <mergeCell ref="D42:D46"/>
-    <mergeCell ref="E43:E46"/>
-    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="C57:C58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="28" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -39981,12 +40395,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="30.75">
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="151" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -39997,20 +40411,20 @@
       <c r="M2" s="4"/>
     </row>
     <row r="4" spans="2:13">
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="143" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="146" t="s">
+      <c r="D4" s="145" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="147"/>
+      <c r="E4" s="146"/>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="145"/>
-      <c r="C5" s="145"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="144"/>
       <c r="D5" s="17" t="s">
         <v>54</v>
       </c>
@@ -40025,10 +40439,10 @@
       <c r="C6" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="150" t="s">
+      <c r="D6" s="147" t="s">
         <v>137</v>
       </c>
-      <c r="E6" s="151"/>
+      <c r="E6" s="148"/>
     </row>
     <row r="7" spans="2:13" ht="23.25" customHeight="1">
       <c r="B7" s="152" t="s">
@@ -40098,20 +40512,20 @@
       </c>
     </row>
     <row r="15" spans="2:13">
-      <c r="B15" s="144" t="s">
+      <c r="B15" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="144" t="s">
+      <c r="C15" s="143" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="146" t="s">
+      <c r="D15" s="145" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="147"/>
+      <c r="E15" s="146"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="B16" s="145"/>
-      <c r="C16" s="145"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
       <c r="D16" s="17" t="s">
         <v>54</v>
       </c>
@@ -40126,16 +40540,16 @@
       <c r="C17" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="150" t="s">
+      <c r="D17" s="147" t="s">
         <v>134</v>
       </c>
-      <c r="E17" s="151"/>
+      <c r="E17" s="148"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="148" t="s">
+      <c r="B18" s="149" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="149" t="s">
+      <c r="C18" s="150" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="16" t="s">
@@ -40146,8 +40560,8 @@
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="148"/>
-      <c r="C19" s="149"/>
+      <c r="B19" s="149"/>
+      <c r="C19" s="150"/>
       <c r="D19" s="16" t="s">
         <v>58</v>
       </c>
@@ -40156,8 +40570,8 @@
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="148"/>
-      <c r="C20" s="149"/>
+      <c r="B20" s="149"/>
+      <c r="C20" s="150"/>
       <c r="D20" s="16" t="s">
         <v>59</v>
       </c>
@@ -40166,8 +40580,8 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="148"/>
-      <c r="C21" s="149"/>
+      <c r="B21" s="149"/>
+      <c r="C21" s="150"/>
       <c r="D21" s="16" t="s">
         <v>220</v>
       </c>
@@ -40176,20 +40590,20 @@
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="144" t="s">
+      <c r="B24" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="144" t="s">
+      <c r="C24" s="143" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="146" t="s">
+      <c r="D24" s="145" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="147"/>
+      <c r="E24" s="146"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="145"/>
-      <c r="C25" s="145"/>
+      <c r="B25" s="144"/>
+      <c r="C25" s="144"/>
       <c r="D25" s="17" t="s">
         <v>54</v>
       </c>
@@ -40204,16 +40618,16 @@
       <c r="C26" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="150" t="s">
+      <c r="D26" s="147" t="s">
         <v>140</v>
       </c>
-      <c r="E26" s="151"/>
+      <c r="E26" s="148"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="148" t="s">
+      <c r="B27" s="149" t="s">
         <v>138</v>
       </c>
-      <c r="C27" s="149" t="s">
+      <c r="C27" s="150" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="16" t="s">
@@ -40224,8 +40638,8 @@
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="148"/>
-      <c r="C28" s="149"/>
+      <c r="B28" s="149"/>
+      <c r="C28" s="150"/>
       <c r="D28" s="16" t="s">
         <v>64</v>
       </c>
@@ -40234,16 +40648,16 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="148"/>
-      <c r="C29" s="149"/>
+      <c r="B29" s="149"/>
+      <c r="C29" s="150"/>
       <c r="D29" s="16" t="s">
         <v>223</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="148"/>
-      <c r="C30" s="149"/>
+      <c r="B30" s="149"/>
+      <c r="C30" s="150"/>
       <c r="D30" s="16" t="s">
         <v>65</v>
       </c>
@@ -40252,20 +40666,20 @@
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="144" t="s">
+      <c r="B32" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="144" t="s">
+      <c r="C32" s="143" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="146" t="s">
+      <c r="D32" s="145" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="147"/>
+      <c r="E32" s="146"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="145"/>
-      <c r="C33" s="145"/>
+      <c r="B33" s="144"/>
+      <c r="C33" s="144"/>
       <c r="D33" s="17" t="s">
         <v>54</v>
       </c>
@@ -40280,16 +40694,16 @@
       <c r="C34" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D34" s="150" t="s">
+      <c r="D34" s="147" t="s">
         <v>130</v>
       </c>
-      <c r="E34" s="151"/>
+      <c r="E34" s="148"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="148" t="s">
+      <c r="B35" s="149" t="s">
         <v>128</v>
       </c>
-      <c r="C35" s="149" t="s">
+      <c r="C35" s="150" t="s">
         <v>53</v>
       </c>
       <c r="D35" s="16" t="s">
@@ -40300,8 +40714,8 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="148"/>
-      <c r="C36" s="149"/>
+      <c r="B36" s="149"/>
+      <c r="C36" s="150"/>
       <c r="D36" s="16" t="s">
         <v>58</v>
       </c>
@@ -40310,8 +40724,8 @@
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="148"/>
-      <c r="C37" s="149"/>
+      <c r="B37" s="149"/>
+      <c r="C37" s="150"/>
       <c r="D37" s="16" t="s">
         <v>180</v>
       </c>
@@ -40320,8 +40734,8 @@
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="148"/>
-      <c r="C38" s="149"/>
+      <c r="B38" s="149"/>
+      <c r="C38" s="150"/>
       <c r="D38" s="16" t="s">
         <v>131</v>
       </c>
@@ -40331,18 +40745,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D26:E26"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -40356,6 +40758,18 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="C7:C12"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40370,8 +40784,8 @@
   </sheetPr>
   <dimension ref="A4:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="A24:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40384,21 +40798,21 @@
   <sheetData>
     <row r="4" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="143" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="146" t="s">
+      <c r="D4" s="145" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="147"/>
+      <c r="E4" s="146"/>
     </row>
     <row r="5" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="145"/>
-      <c r="C5" s="145"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="144"/>
       <c r="D5" s="17" t="s">
         <v>54</v>
       </c>
@@ -40556,20 +40970,20 @@
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" ht="23.25">
-      <c r="B25" s="144" t="s">
+      <c r="B25" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="144" t="s">
+      <c r="C25" s="143" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="146" t="s">
+      <c r="D25" s="145" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="147"/>
+      <c r="E25" s="146"/>
     </row>
     <row r="26" spans="1:5" ht="23.25">
-      <c r="B26" s="145"/>
-      <c r="C26" s="145"/>
+      <c r="B26" s="144"/>
+      <c r="C26" s="144"/>
       <c r="D26" s="17" t="s">
         <v>54</v>
       </c>
@@ -40584,16 +40998,16 @@
       <c r="C27" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="150" t="s">
+      <c r="D27" s="147" t="s">
         <v>134</v>
       </c>
-      <c r="E27" s="151"/>
+      <c r="E27" s="148"/>
     </row>
     <row r="28" spans="1:5" ht="23.25" customHeight="1">
-      <c r="B28" s="148" t="s">
+      <c r="B28" s="149" t="s">
         <v>132</v>
       </c>
-      <c r="C28" s="149" t="s">
+      <c r="C28" s="150" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="16" t="s">
@@ -40602,24 +41016,24 @@
       <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:5" ht="23.25">
-      <c r="B29" s="148"/>
-      <c r="C29" s="149"/>
+      <c r="B29" s="149"/>
+      <c r="C29" s="150"/>
       <c r="D29" s="16" t="s">
         <v>58</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:5" ht="23.25">
-      <c r="B30" s="148"/>
-      <c r="C30" s="149"/>
+      <c r="B30" s="149"/>
+      <c r="C30" s="150"/>
       <c r="D30" s="16" t="s">
         <v>59</v>
       </c>
       <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5" ht="23.25">
-      <c r="B31" s="148"/>
-      <c r="C31" s="149"/>
+      <c r="B31" s="149"/>
+      <c r="C31" s="150"/>
       <c r="D31" s="16" t="s">
         <v>220</v>
       </c>
@@ -40627,17 +41041,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="B6:B11"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="C28:C31"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B6:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40652,7 +41066,7 @@
   </sheetPr>
   <dimension ref="A1:Z235"/>
   <sheetViews>
-    <sheetView topLeftCell="B150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AB184" sqref="AB184"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
I built the <Products> <Customers> <Purchases> models without the delete functionality
</commit_message>
<xml_diff>
--- a/Final-React-Project-Design.xlsx
+++ b/Final-React-Project-Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basheer\Desktop\בשיר\Full Stack Work\Full Stack Cors - YanivArad\Projects\React-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E34C06-E911-4347-827F-1F5AE30041F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC355FA-0CE9-4C86-916B-67194A13CA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="240">
   <si>
     <t>Num</t>
   </si>
@@ -4047,21 +4047,6 @@
     <t>Perform tests for the application</t>
   </si>
   <si>
-    <t>20/11/23</t>
-  </si>
-  <si>
-    <t>21/11/23</t>
-  </si>
-  <si>
-    <t>22-23/11/23</t>
-  </si>
-  <si>
-    <t>24/11/23</t>
-  </si>
-  <si>
-    <t>25/11/23</t>
-  </si>
-  <si>
     <t>FireStore DB</t>
   </si>
   <si>
@@ -5068,12 +5053,6 @@
     <t>Improving the efficiency of the application</t>
   </si>
   <si>
-    <t>26/11/23</t>
-  </si>
-  <si>
-    <t>27/11/23</t>
-  </si>
-  <si>
     <t>28/11/23</t>
   </si>
   <si>
@@ -5287,6 +5266,45 @@
   </si>
   <si>
     <t>src/redux/store.js</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">npm install </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Univers"/>
+        <family val="2"/>
+      </rPr>
+      <t>@mui/x-date-pickers</t>
+    </r>
+  </si>
+  <si>
+    <t>react-material-ui-carousel</t>
+  </si>
+  <si>
+    <t>npm i moment</t>
+  </si>
+  <si>
+    <t>A JavaScript date library for parsing, validating, manipulating, and formatting dates</t>
+  </si>
+  <si>
+    <t>Add timestamp date in react</t>
+  </si>
+  <si>
+    <t xml:space="preserve">import moment from 'moment';  </t>
+  </si>
+  <si>
+    <t>20-27/11/23</t>
+  </si>
+  <si>
+    <t>28-29/11/23</t>
+  </si>
+  <si>
+    <t>30/11/23</t>
   </si>
 </sst>
 </file>
@@ -6340,7 +6358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -6605,6 +6623,30 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -6616,69 +6658,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6704,16 +6683,10 @@
     <xf numFmtId="0" fontId="19" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="48" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="47" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6734,6 +6707,9 @@
     <xf numFmtId="0" fontId="19" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6745,6 +6721,81 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6758,19 +6809,16 @@
     <xf numFmtId="0" fontId="25" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6815,41 +6863,17 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -18075,7 +18099,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>"40",</a:t>
+            <a:t>"Tel Aviv",</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -39155,7 +39179,7 @@
   <dimension ref="B3:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15"/>
@@ -39173,44 +39197,44 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="106" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="99" t="s">
+      <c r="C6" s="107" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="99" t="s">
+      <c r="D6" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="99" t="s">
+      <c r="E6" s="107" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="99" t="s">
+      <c r="F6" s="107" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="99"/>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="46">
@@ -39248,7 +39272,7 @@
       <c r="B10" s="46">
         <v>2</v>
       </c>
-      <c r="C10" s="96" t="s">
+      <c r="C10" s="104" t="s">
         <v>68</v>
       </c>
       <c r="D10" s="47" t="s">
@@ -39265,7 +39289,7 @@
       <c r="B11" s="46">
         <v>3</v>
       </c>
-      <c r="C11" s="97"/>
+      <c r="C11" s="105"/>
       <c r="D11" s="46" t="s">
         <v>70</v>
       </c>
@@ -39287,7 +39311,7 @@
         <v>146</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>124</v>
@@ -39304,7 +39328,7 @@
         <v>143</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>124</v>
@@ -39321,7 +39345,7 @@
         <v>144</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>124</v>
@@ -39338,7 +39362,7 @@
         <v>145</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>124</v>
@@ -39355,7 +39379,7 @@
         <v>142</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>124</v>
@@ -39372,9 +39396,11 @@
         <v>151</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>164</v>
+        <v>237</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="46">
@@ -39387,9 +39413,11 @@
         <v>152</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>165</v>
+        <v>237</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" s="46">
@@ -39402,9 +39430,11 @@
         <v>153</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>166</v>
+        <v>237</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" s="46">
@@ -39417,7 +39447,7 @@
         <v>154</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>167</v>
+        <v>223</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -39432,7 +39462,7 @@
         <v>155</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>168</v>
+        <v>238</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -39447,7 +39477,7 @@
         <v>161</v>
       </c>
       <c r="E22" s="46" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -39456,13 +39486,13 @@
         <v>15</v>
       </c>
       <c r="C23" s="46" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
-      <c r="E23" s="46" t="s">
-        <v>229</v>
+      <c r="E23" s="179">
+        <v>44938</v>
       </c>
       <c r="F23" s="1"/>
     </row>
@@ -39471,13 +39501,13 @@
         <v>16</v>
       </c>
       <c r="C24" s="46" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D24" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="E24" s="46" t="s">
-        <v>230</v>
+      <c r="E24" s="179">
+        <v>44938</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -39519,23 +39549,23 @@
     </row>
     <row r="29" spans="2:6" ht="37.5">
       <c r="C29" s="90" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D29" s="91" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="37.5">
       <c r="C31" s="90" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D31" s="91" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="37.5">
       <c r="D33" s="91" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -39568,10 +39598,10 @@
     <tabColor rgb="FF00B0F0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G89"/>
+  <dimension ref="A2:G90"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D5"/>
+    <sheetView topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61:D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39585,36 +39615,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="51.75" customHeight="1">
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" thickBot="1">
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B4" s="111" t="s">
+      <c r="B4" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="C4" s="147" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="108" t="s">
+      <c r="D4" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="108" t="s">
+      <c r="E4" s="147" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="119"/>
+      <c r="F4" s="148"/>
     </row>
     <row r="5" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B5" s="112"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="109"/>
+      <c r="B5" s="135"/>
+      <c r="C5" s="150"/>
+      <c r="D5" s="150"/>
       <c r="E5" s="31" t="s">
         <v>9</v>
       </c>
@@ -39623,10 +39653,10 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B6" s="126">
+      <c r="B6" s="113">
         <v>1</v>
       </c>
-      <c r="C6" s="123" t="s">
+      <c r="C6" s="110" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="73" t="s">
@@ -39635,68 +39665,68 @@
       <c r="E6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="171" t="s">
+      <c r="F6" s="100" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B7" s="127"/>
-      <c r="C7" s="124"/>
-      <c r="D7" s="102" t="s">
-        <v>232</v>
+      <c r="B7" s="114"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="124" t="s">
+        <v>225</v>
       </c>
-      <c r="E7" s="136" t="s">
-        <v>237</v>
+      <c r="E7" s="121" t="s">
+        <v>230</v>
       </c>
-      <c r="F7" s="172" t="s">
-        <v>233</v>
+      <c r="F7" s="101" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B8" s="127"/>
-      <c r="C8" s="124"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="172" t="s">
-        <v>234</v>
+      <c r="B8" s="114"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="101" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B9" s="127"/>
-      <c r="C9" s="124"/>
-      <c r="D9" s="139"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="172" t="s">
-        <v>235</v>
+      <c r="B9" s="114"/>
+      <c r="C9" s="111"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="101" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B10" s="127"/>
-      <c r="C10" s="124"/>
-      <c r="D10" s="139"/>
-      <c r="E10" s="137"/>
-      <c r="F10" s="173"/>
+      <c r="B10" s="114"/>
+      <c r="C10" s="111"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="102"/>
     </row>
     <row r="11" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B11" s="175"/>
-      <c r="C11" s="170"/>
-      <c r="D11" s="176"/>
-      <c r="E11" s="177"/>
-      <c r="F11" s="174" t="s">
-        <v>236</v>
+      <c r="B11" s="132"/>
+      <c r="C11" s="131"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="151"/>
+      <c r="F11" s="103" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="22.5">
-      <c r="B12" s="115">
+      <c r="B12" s="129">
         <v>2</v>
       </c>
-      <c r="C12" s="103" t="s">
+      <c r="C12" s="136" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="100" t="s">
+      <c r="D12" s="144" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="106" t="s">
+      <c r="E12" s="141" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="38" t="s">
@@ -39704,63 +39734,63 @@
       </c>
     </row>
     <row r="13" spans="2:6" ht="22.5">
-      <c r="B13" s="116"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="107"/>
+      <c r="B13" s="130"/>
+      <c r="C13" s="137"/>
+      <c r="D13" s="145"/>
+      <c r="E13" s="142"/>
       <c r="F13" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="22.5">
-      <c r="B14" s="116"/>
-      <c r="C14" s="104"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="107"/>
+      <c r="B14" s="130"/>
+      <c r="C14" s="137"/>
+      <c r="D14" s="145"/>
+      <c r="E14" s="142"/>
       <c r="F14" s="21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="22.5">
-      <c r="B15" s="116"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="107"/>
+      <c r="B15" s="130"/>
+      <c r="C15" s="137"/>
+      <c r="D15" s="145"/>
+      <c r="E15" s="142"/>
       <c r="F15" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="22.5">
-      <c r="B16" s="116"/>
-      <c r="C16" s="104"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="107"/>
+      <c r="B16" s="130"/>
+      <c r="C16" s="137"/>
+      <c r="D16" s="145"/>
+      <c r="E16" s="142"/>
       <c r="F16" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="22.5">
-      <c r="B17" s="116"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="107"/>
+      <c r="B17" s="130"/>
+      <c r="C17" s="137"/>
+      <c r="D17" s="145"/>
+      <c r="E17" s="142"/>
       <c r="F17" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="22.5">
-      <c r="B18" s="116"/>
-      <c r="C18" s="104"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="107"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="145"/>
+      <c r="E18" s="142"/>
       <c r="F18" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B19" s="117"/>
-      <c r="C19" s="105"/>
-      <c r="D19" s="118"/>
+      <c r="B19" s="143"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="146"/>
       <c r="E19" s="40" t="s">
         <v>13</v>
       </c>
@@ -39769,16 +39799,16 @@
       </c>
     </row>
     <row r="20" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B20" s="115">
+      <c r="B20" s="129">
         <v>3</v>
       </c>
-      <c r="C20" s="103" t="s">
+      <c r="C20" s="136" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="100" t="s">
+      <c r="D20" s="144" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="106" t="s">
+      <c r="E20" s="141" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="41" t="s">
@@ -39786,45 +39816,45 @@
       </c>
     </row>
     <row r="21" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B21" s="116"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="107"/>
+      <c r="B21" s="130"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="145"/>
+      <c r="E21" s="142"/>
       <c r="F21" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B22" s="116"/>
-      <c r="C22" s="104"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="107"/>
+      <c r="B22" s="130"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="145"/>
+      <c r="E22" s="142"/>
       <c r="F22" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B23" s="116"/>
-      <c r="C23" s="104"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="107"/>
+      <c r="B23" s="130"/>
+      <c r="C23" s="137"/>
+      <c r="D23" s="145"/>
+      <c r="E23" s="142"/>
       <c r="F23" s="26" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B24" s="116"/>
-      <c r="C24" s="104"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="107"/>
+      <c r="B24" s="130"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="145"/>
+      <c r="E24" s="142"/>
       <c r="F24" s="27" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B25" s="117"/>
-      <c r="C25" s="105"/>
-      <c r="D25" s="118"/>
+      <c r="B25" s="143"/>
+      <c r="C25" s="138"/>
+      <c r="D25" s="146"/>
       <c r="E25" s="40" t="s">
         <v>13</v>
       </c>
@@ -39833,16 +39863,16 @@
       </c>
     </row>
     <row r="26" spans="2:6" ht="22.5">
-      <c r="B26" s="115">
+      <c r="B26" s="129">
         <v>4</v>
       </c>
-      <c r="C26" s="103" t="s">
+      <c r="C26" s="136" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="100" t="s">
+      <c r="D26" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="106" t="s">
+      <c r="E26" s="141" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="41" t="s">
@@ -39850,27 +39880,27 @@
       </c>
     </row>
     <row r="27" spans="2:6" ht="22.5">
-      <c r="B27" s="116"/>
-      <c r="C27" s="104"/>
-      <c r="D27" s="101"/>
-      <c r="E27" s="107"/>
+      <c r="B27" s="130"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="142"/>
       <c r="F27" s="28" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="22.5">
-      <c r="B28" s="116"/>
-      <c r="C28" s="104"/>
-      <c r="D28" s="101"/>
-      <c r="E28" s="107"/>
+      <c r="B28" s="130"/>
+      <c r="C28" s="137"/>
+      <c r="D28" s="145"/>
+      <c r="E28" s="142"/>
       <c r="F28" s="29" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="42" customHeight="1" thickBot="1">
-      <c r="B29" s="135"/>
-      <c r="C29" s="120"/>
-      <c r="D29" s="102"/>
+      <c r="B29" s="120"/>
+      <c r="C29" s="149"/>
+      <c r="D29" s="124"/>
       <c r="E29" s="12" t="s">
         <v>13</v>
       </c>
@@ -39896,16 +39926,16 @@
       </c>
     </row>
     <row r="31" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B31" s="115">
+      <c r="B31" s="129">
         <v>6</v>
       </c>
-      <c r="C31" s="103" t="s">
+      <c r="C31" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="113" t="s">
+      <c r="D31" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="106" t="s">
+      <c r="E31" s="141" t="s">
         <v>13</v>
       </c>
       <c r="F31" s="41" t="s">
@@ -39913,17 +39943,17 @@
       </c>
     </row>
     <row r="32" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B32" s="116"/>
-      <c r="C32" s="104"/>
-      <c r="D32" s="114"/>
-      <c r="E32" s="107"/>
+      <c r="B32" s="130"/>
+      <c r="C32" s="137"/>
+      <c r="D32" s="140"/>
+      <c r="E32" s="142"/>
       <c r="F32" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B33" s="117"/>
-      <c r="C33" s="105"/>
+      <c r="B33" s="143"/>
+      <c r="C33" s="138"/>
       <c r="D33" s="39" t="s">
         <v>39</v>
       </c>
@@ -39967,10 +39997,10 @@
       </c>
     </row>
     <row r="36" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B36" s="126">
+      <c r="B36" s="113">
         <v>9</v>
       </c>
-      <c r="C36" s="123" t="s">
+      <c r="C36" s="110" t="s">
         <v>90</v>
       </c>
       <c r="D36" s="73" t="s">
@@ -39984,12 +40014,12 @@
       </c>
     </row>
     <row r="37" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B37" s="127"/>
-      <c r="C37" s="124"/>
-      <c r="D37" s="102" t="s">
+      <c r="B37" s="114"/>
+      <c r="C37" s="111"/>
+      <c r="D37" s="124" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="136" t="s">
+      <c r="E37" s="121" t="s">
         <v>96</v>
       </c>
       <c r="F37" s="55" t="s">
@@ -39997,37 +40027,37 @@
       </c>
     </row>
     <row r="38" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B38" s="127"/>
-      <c r="C38" s="124"/>
-      <c r="D38" s="139"/>
-      <c r="E38" s="137"/>
+      <c r="B38" s="114"/>
+      <c r="C38" s="111"/>
+      <c r="D38" s="125"/>
+      <c r="E38" s="122"/>
       <c r="F38" s="51" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B39" s="127"/>
-      <c r="C39" s="124"/>
-      <c r="D39" s="139"/>
-      <c r="E39" s="137"/>
+      <c r="B39" s="114"/>
+      <c r="C39" s="111"/>
+      <c r="D39" s="125"/>
+      <c r="E39" s="122"/>
       <c r="F39" s="51" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B40" s="127"/>
-      <c r="C40" s="124"/>
-      <c r="D40" s="139"/>
-      <c r="E40" s="138"/>
+      <c r="B40" s="114"/>
+      <c r="C40" s="111"/>
+      <c r="D40" s="125"/>
+      <c r="E40" s="123"/>
       <c r="F40" s="56" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B41" s="127"/>
-      <c r="C41" s="124"/>
-      <c r="D41" s="139"/>
-      <c r="E41" s="136" t="s">
+      <c r="B41" s="114"/>
+      <c r="C41" s="111"/>
+      <c r="D41" s="125"/>
+      <c r="E41" s="121" t="s">
         <v>98</v>
       </c>
       <c r="F41" s="57" t="s">
@@ -40035,54 +40065,54 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B42" s="127"/>
-      <c r="C42" s="124"/>
-      <c r="D42" s="139"/>
-      <c r="E42" s="137"/>
+      <c r="B42" s="114"/>
+      <c r="C42" s="111"/>
+      <c r="D42" s="125"/>
+      <c r="E42" s="122"/>
       <c r="F42" s="58" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B43" s="127"/>
-      <c r="C43" s="124"/>
-      <c r="D43" s="139"/>
-      <c r="E43" s="137"/>
+      <c r="B43" s="114"/>
+      <c r="C43" s="111"/>
+      <c r="D43" s="125"/>
+      <c r="E43" s="122"/>
       <c r="F43" s="58" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B44" s="127"/>
-      <c r="C44" s="124"/>
-      <c r="D44" s="139"/>
-      <c r="E44" s="137"/>
+      <c r="B44" s="114"/>
+      <c r="C44" s="111"/>
+      <c r="D44" s="125"/>
+      <c r="E44" s="122"/>
       <c r="F44" s="59" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B45" s="127"/>
-      <c r="C45" s="124"/>
-      <c r="D45" s="139"/>
-      <c r="E45" s="137"/>
+      <c r="B45" s="114"/>
+      <c r="C45" s="111"/>
+      <c r="D45" s="125"/>
+      <c r="E45" s="122"/>
       <c r="F45" s="59" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B46" s="127"/>
-      <c r="C46" s="124"/>
-      <c r="D46" s="140"/>
-      <c r="E46" s="138"/>
+      <c r="B46" s="114"/>
+      <c r="C46" s="111"/>
+      <c r="D46" s="126"/>
+      <c r="E46" s="123"/>
       <c r="F46" s="60" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="75">
-      <c r="B47" s="127"/>
-      <c r="C47" s="124"/>
-      <c r="D47" s="102" t="s">
+      <c r="B47" s="114"/>
+      <c r="C47" s="111"/>
+      <c r="D47" s="124" t="s">
         <v>97</v>
       </c>
       <c r="E47" s="10" t="s">
@@ -40093,10 +40123,10 @@
       </c>
     </row>
     <row r="48" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B48" s="127"/>
-      <c r="C48" s="124"/>
-      <c r="D48" s="139"/>
-      <c r="E48" s="141" t="s">
+      <c r="B48" s="114"/>
+      <c r="C48" s="111"/>
+      <c r="D48" s="125"/>
+      <c r="E48" s="127" t="s">
         <v>109</v>
       </c>
       <c r="F48" s="58" t="s">
@@ -40104,245 +40134,258 @@
       </c>
     </row>
     <row r="49" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B49" s="127"/>
-      <c r="C49" s="124"/>
-      <c r="D49" s="139"/>
-      <c r="E49" s="141"/>
+      <c r="B49" s="114"/>
+      <c r="C49" s="111"/>
+      <c r="D49" s="125"/>
+      <c r="E49" s="127"/>
       <c r="F49" s="59" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B50" s="127"/>
-      <c r="C50" s="124"/>
-      <c r="D50" s="139"/>
-      <c r="E50" s="141"/>
+      <c r="B50" s="114"/>
+      <c r="C50" s="111"/>
+      <c r="D50" s="125"/>
+      <c r="E50" s="127"/>
       <c r="F50" s="59" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B51" s="128"/>
-      <c r="C51" s="125"/>
-      <c r="D51" s="140"/>
-      <c r="E51" s="142"/>
+      <c r="B51" s="115"/>
+      <c r="C51" s="112"/>
+      <c r="D51" s="126"/>
+      <c r="E51" s="128"/>
       <c r="F51" s="60" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B52" s="135">
+    <row r="52" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B52" s="96"/>
+      <c r="C52" s="97"/>
+      <c r="D52" s="98" t="s">
+        <v>231</v>
+      </c>
+      <c r="E52" s="176" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="177"/>
+    </row>
+    <row r="53" spans="2:7" ht="42.75" customHeight="1">
+      <c r="B53" s="114">
         <v>10</v>
       </c>
-      <c r="C52" s="132" t="s">
+      <c r="C53" s="118" t="s">
         <v>117</v>
       </c>
-      <c r="D52" s="129" t="s">
+      <c r="D53" s="116" t="s">
         <v>126</v>
       </c>
-      <c r="E52" s="136" t="s">
+      <c r="E53" s="122" t="s">
         <v>118</v>
       </c>
-      <c r="F52" s="62" t="s">
+      <c r="F53" s="62" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B53" s="127"/>
-      <c r="C53" s="133"/>
-      <c r="D53" s="130"/>
-      <c r="E53" s="137"/>
-      <c r="F53" s="62" t="s">
+    <row r="54" spans="2:7" ht="42.75" customHeight="1">
+      <c r="B54" s="114"/>
+      <c r="C54" s="118"/>
+      <c r="D54" s="116"/>
+      <c r="E54" s="122"/>
+      <c r="F54" s="62" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B54" s="127"/>
-      <c r="C54" s="133"/>
-      <c r="D54" s="130"/>
-      <c r="E54" s="137"/>
-      <c r="F54" s="63" t="s">
+    <row r="55" spans="2:7" ht="42.75" customHeight="1">
+      <c r="B55" s="114"/>
+      <c r="C55" s="118"/>
+      <c r="D55" s="116"/>
+      <c r="E55" s="122"/>
+      <c r="F55" s="63" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B55" s="127"/>
-      <c r="C55" s="133"/>
-      <c r="D55" s="130"/>
-      <c r="E55" s="137"/>
-      <c r="F55" s="62" t="s">
+    <row r="56" spans="2:7" ht="42.75" customHeight="1">
+      <c r="B56" s="114"/>
+      <c r="C56" s="118"/>
+      <c r="D56" s="116"/>
+      <c r="E56" s="122"/>
+      <c r="F56" s="62" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B56" s="128"/>
-      <c r="C56" s="134"/>
-      <c r="D56" s="131"/>
-      <c r="E56" s="138"/>
-      <c r="F56" s="62" t="s">
+    <row r="57" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B57" s="115"/>
+      <c r="C57" s="119"/>
+      <c r="D57" s="117"/>
+      <c r="E57" s="123"/>
+      <c r="F57" s="62" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B57" s="33"/>
-      <c r="C57" s="123" t="s">
-        <v>211</v>
-      </c>
-      <c r="D57" s="72" t="s">
-        <v>212</v>
-      </c>
-      <c r="E57" s="36" t="s">
-        <v>215</v>
-      </c>
-      <c r="F57" s="37" t="s">
-        <v>214</v>
-      </c>
-      <c r="G57" s="110" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="58" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B58" s="33"/>
-      <c r="C58" s="170"/>
+      <c r="C58" s="110" t="s">
+        <v>206</v>
+      </c>
       <c r="D58" s="72" t="s">
+        <v>207</v>
+      </c>
+      <c r="E58" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="F58" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="G58" s="152" t="s">
         <v>213</v>
       </c>
-      <c r="E58" s="36" t="s">
-        <v>216</v>
-      </c>
-      <c r="F58" s="37" t="s">
-        <v>217</v>
-      </c>
-      <c r="G58" s="110"/>
     </row>
     <row r="59" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B59" s="166"/>
-      <c r="C59" s="167"/>
-      <c r="D59" s="168"/>
-      <c r="E59" s="169"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="93"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="131"/>
+      <c r="D59" s="72" t="s">
+        <v>208</v>
+      </c>
+      <c r="E59" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="F59" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="G59" s="152"/>
     </row>
     <row r="60" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B60" s="166"/>
-      <c r="C60" s="167"/>
-      <c r="D60" s="168"/>
-      <c r="E60" s="169"/>
+      <c r="B60" s="96"/>
+      <c r="C60" s="97"/>
+      <c r="D60" s="98" t="s">
+        <v>232</v>
+      </c>
+      <c r="E60" s="99"/>
       <c r="F60" s="14"/>
       <c r="G60" s="93"/>
     </row>
     <row r="61" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B61" s="166"/>
-      <c r="C61" s="167"/>
-      <c r="D61" s="168"/>
-      <c r="E61" s="169"/>
-      <c r="F61" s="14"/>
+      <c r="B61" s="96"/>
+      <c r="C61" s="97" t="s">
+        <v>235</v>
+      </c>
+      <c r="D61" s="178" t="s">
+        <v>233</v>
+      </c>
+      <c r="E61" s="99"/>
+      <c r="F61" s="14" t="s">
+        <v>234</v>
+      </c>
       <c r="G61" s="93"/>
     </row>
     <row r="62" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B62" s="166"/>
-      <c r="C62" s="167"/>
-      <c r="D62" s="168"/>
-      <c r="E62" s="169"/>
-      <c r="F62" s="14"/>
+      <c r="B62" s="96"/>
+      <c r="C62" s="97"/>
+      <c r="D62" s="133"/>
+      <c r="E62" s="99"/>
+      <c r="F62" s="14" t="s">
+        <v>236</v>
+      </c>
       <c r="G62" s="93"/>
     </row>
     <row r="63" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B63" s="166"/>
-      <c r="C63" s="167"/>
-      <c r="D63" s="168"/>
-      <c r="E63" s="169"/>
+      <c r="B63" s="96"/>
+      <c r="C63" s="97"/>
+      <c r="D63" s="176"/>
+      <c r="E63" s="99"/>
       <c r="F63" s="14"/>
       <c r="G63" s="93"/>
     </row>
-    <row r="64" spans="2:7" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B64" s="8"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="50"/>
+    <row r="64" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B64" s="96"/>
+      <c r="C64" s="97"/>
+      <c r="D64" s="176"/>
+      <c r="E64" s="99"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="93"/>
     </row>
-    <row r="65" spans="6:7" s="92" customFormat="1" ht="45.75" customHeight="1">
-      <c r="G65" s="110"/>
+    <row r="65" spans="2:7" ht="34.5" customHeight="1" thickBot="1">
+      <c r="B65" s="8"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="50"/>
     </row>
-    <row r="66" spans="6:7" s="92" customFormat="1" ht="45.75" customHeight="1">
-      <c r="G66" s="110"/>
+    <row r="66" spans="2:7" s="92" customFormat="1" ht="45.75" customHeight="1">
+      <c r="G66" s="152"/>
     </row>
-    <row r="67" spans="6:7" s="92" customFormat="1" ht="43.5" customHeight="1">
-      <c r="G67" s="93"/>
+    <row r="67" spans="2:7" s="92" customFormat="1" ht="45.75" customHeight="1">
+      <c r="G67" s="152"/>
     </row>
-    <row r="68" spans="6:7" s="92" customFormat="1" ht="43.5" customHeight="1">
+    <row r="68" spans="2:7" s="92" customFormat="1" ht="43.5" customHeight="1">
       <c r="G68" s="93"/>
     </row>
-    <row r="70" spans="6:7" s="92" customFormat="1" ht="43.5" customHeight="1">
-      <c r="G70" s="93"/>
+    <row r="69" spans="2:7" s="92" customFormat="1" ht="43.5" customHeight="1">
+      <c r="G69" s="93"/>
     </row>
-    <row r="71" spans="6:7" s="92" customFormat="1" ht="31.5" customHeight="1">
+    <row r="71" spans="2:7" s="92" customFormat="1" ht="43.5" customHeight="1">
       <c r="G71" s="93"/>
     </row>
-    <row r="72" spans="6:7" s="92" customFormat="1" ht="31.5" customHeight="1">
+    <row r="72" spans="2:7" s="92" customFormat="1" ht="31.5" customHeight="1">
       <c r="G72" s="93"/>
     </row>
-    <row r="73" spans="6:7" s="92" customFormat="1" ht="31.5" customHeight="1">
+    <row r="73" spans="2:7" s="92" customFormat="1" ht="31.5" customHeight="1">
       <c r="G73" s="93"/>
     </row>
-    <row r="74" spans="6:7" s="92" customFormat="1" ht="31.5" customHeight="1">
+    <row r="74" spans="2:7" s="92" customFormat="1" ht="31.5" customHeight="1">
       <c r="G74" s="93"/>
     </row>
-    <row r="75" spans="6:7" s="92" customFormat="1" ht="20.25">
+    <row r="75" spans="2:7" s="92" customFormat="1" ht="31.5" customHeight="1">
       <c r="G75" s="93"/>
     </row>
-    <row r="76" spans="6:7" ht="22.5">
-      <c r="F76" s="11"/>
+    <row r="76" spans="2:7" s="92" customFormat="1" ht="20.25">
+      <c r="G76" s="93"/>
     </row>
-    <row r="77" spans="6:7" ht="22.5">
-      <c r="F77" s="52"/>
+    <row r="77" spans="2:7" ht="22.5">
+      <c r="F77" s="11"/>
     </row>
-    <row r="78" spans="6:7" ht="22.5">
+    <row r="78" spans="2:7" ht="22.5">
       <c r="F78" s="52"/>
     </row>
-    <row r="79" spans="6:7" ht="22.5">
+    <row r="79" spans="2:7" ht="22.5">
       <c r="F79" s="52"/>
     </row>
-    <row r="80" spans="6:7" ht="22.5">
-      <c r="F80" s="53"/>
+    <row r="80" spans="2:7" ht="22.5">
+      <c r="F80" s="52"/>
     </row>
     <row r="81" spans="6:6" ht="22.5">
       <c r="F81" s="53"/>
     </row>
     <row r="82" spans="6:6" ht="22.5">
-      <c r="F82" s="54"/>
+      <c r="F82" s="53"/>
     </row>
-    <row r="86" spans="6:6" ht="22.5">
-      <c r="F86" s="52"/>
+    <row r="83" spans="6:6" ht="22.5">
+      <c r="F83" s="54"/>
     </row>
     <row r="87" spans="6:6" ht="22.5">
-      <c r="F87" s="53"/>
+      <c r="F87" s="52"/>
     </row>
     <row r="88" spans="6:6" ht="22.5">
       <c r="F88" s="53"/>
     </row>
     <row r="89" spans="6:6" ht="22.5">
-      <c r="F89" s="54"/>
+      <c r="F89" s="53"/>
+    </row>
+    <row r="90" spans="6:6" ht="22.5">
+      <c r="F90" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="C36:C51"/>
-    <mergeCell ref="B36:B51"/>
-    <mergeCell ref="D52:D56"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="E52:E56"/>
-    <mergeCell ref="E37:E40"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="D37:D46"/>
-    <mergeCell ref="D47:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="D7:D11"/>
+  <mergeCells count="40">
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="C12:C19"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D61:D62"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C31:C33"/>
     <mergeCell ref="D31:D32"/>
@@ -40359,13 +40402,22 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D12:D19"/>
     <mergeCell ref="E7:E11"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="C12:C19"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="C36:C51"/>
+    <mergeCell ref="B36:B51"/>
+    <mergeCell ref="D53:D57"/>
+    <mergeCell ref="C53:C57"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="E53:E57"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="D37:D46"/>
+    <mergeCell ref="D47:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="D7:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="28" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40380,7 +40432,7 @@
   <dimension ref="A2:M38"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D7" sqref="D7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -40395,12 +40447,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="30.75">
-      <c r="B2" s="151" t="s">
+      <c r="B2" s="153" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -40411,20 +40463,20 @@
       <c r="M2" s="4"/>
     </row>
     <row r="4" spans="2:13">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="143" t="s">
+      <c r="C4" s="154" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="145" t="s">
+      <c r="D4" s="156" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="146"/>
+      <c r="E4" s="157"/>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="144"/>
-      <c r="C5" s="144"/>
+      <c r="B5" s="155"/>
+      <c r="C5" s="155"/>
       <c r="D5" s="17" t="s">
         <v>54</v>
       </c>
@@ -40439,16 +40491,16 @@
       <c r="C6" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="147" t="s">
+      <c r="D6" s="160" t="s">
         <v>137</v>
       </c>
-      <c r="E6" s="148"/>
+      <c r="E6" s="161"/>
     </row>
     <row r="7" spans="2:13" ht="23.25" customHeight="1">
-      <c r="B7" s="152" t="s">
+      <c r="B7" s="162" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="155" t="s">
+      <c r="C7" s="165" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="16" t="s">
@@ -40458,12 +40510,12 @@
         <v>55</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="2:13">
-      <c r="B8" s="153"/>
-      <c r="C8" s="156"/>
+      <c r="B8" s="163"/>
+      <c r="C8" s="166"/>
       <c r="D8" s="16" t="s">
         <v>61</v>
       </c>
@@ -40472,8 +40524,8 @@
       </c>
     </row>
     <row r="9" spans="2:13">
-      <c r="B9" s="153"/>
-      <c r="C9" s="156"/>
+      <c r="B9" s="163"/>
+      <c r="C9" s="166"/>
       <c r="D9" s="16" t="s">
         <v>60</v>
       </c>
@@ -40482,50 +40534,50 @@
       </c>
     </row>
     <row r="10" spans="2:13">
-      <c r="B10" s="153"/>
-      <c r="C10" s="156"/>
+      <c r="B10" s="163"/>
+      <c r="C10" s="166"/>
       <c r="D10" s="16" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="2:13">
-      <c r="B11" s="153"/>
-      <c r="C11" s="156"/>
+      <c r="B11" s="163"/>
+      <c r="C11" s="166"/>
       <c r="D11" s="16" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:13">
-      <c r="B12" s="154"/>
-      <c r="C12" s="157"/>
+      <c r="B12" s="164"/>
+      <c r="C12" s="167"/>
       <c r="D12" s="16" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="15" spans="2:13">
-      <c r="B15" s="143" t="s">
+      <c r="B15" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="143" t="s">
+      <c r="C15" s="154" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="145" t="s">
+      <c r="D15" s="156" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="146"/>
+      <c r="E15" s="157"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
       <c r="D16" s="17" t="s">
         <v>54</v>
       </c>
@@ -40540,16 +40592,16 @@
       <c r="C17" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="147" t="s">
+      <c r="D17" s="160" t="s">
         <v>134</v>
       </c>
-      <c r="E17" s="148"/>
+      <c r="E17" s="161"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="149" t="s">
+      <c r="B18" s="158" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="150" t="s">
+      <c r="C18" s="159" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="16" t="s">
@@ -40560,8 +40612,8 @@
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="149"/>
-      <c r="C19" s="150"/>
+      <c r="B19" s="158"/>
+      <c r="C19" s="159"/>
       <c r="D19" s="16" t="s">
         <v>58</v>
       </c>
@@ -40570,8 +40622,8 @@
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="149"/>
-      <c r="C20" s="150"/>
+      <c r="B20" s="158"/>
+      <c r="C20" s="159"/>
       <c r="D20" s="16" t="s">
         <v>59</v>
       </c>
@@ -40580,30 +40632,30 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="149"/>
-      <c r="C21" s="150"/>
+      <c r="B21" s="158"/>
+      <c r="C21" s="159"/>
       <c r="D21" s="16" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="143" t="s">
+      <c r="B24" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="143" t="s">
+      <c r="C24" s="154" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="145" t="s">
+      <c r="D24" s="156" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="146"/>
+      <c r="E24" s="157"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="144"/>
-      <c r="C25" s="144"/>
+      <c r="B25" s="155"/>
+      <c r="C25" s="155"/>
       <c r="D25" s="17" t="s">
         <v>54</v>
       </c>
@@ -40618,16 +40670,16 @@
       <c r="C26" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="147" t="s">
+      <c r="D26" s="160" t="s">
         <v>140</v>
       </c>
-      <c r="E26" s="148"/>
+      <c r="E26" s="161"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="149" t="s">
+      <c r="B27" s="158" t="s">
         <v>138</v>
       </c>
-      <c r="C27" s="150" t="s">
+      <c r="C27" s="159" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="16" t="s">
@@ -40638,8 +40690,8 @@
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="149"/>
-      <c r="C28" s="150"/>
+      <c r="B28" s="158"/>
+      <c r="C28" s="159"/>
       <c r="D28" s="16" t="s">
         <v>64</v>
       </c>
@@ -40648,16 +40700,16 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="149"/>
-      <c r="C29" s="150"/>
+      <c r="B29" s="158"/>
+      <c r="C29" s="159"/>
       <c r="D29" s="16" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="149"/>
-      <c r="C30" s="150"/>
+      <c r="B30" s="158"/>
+      <c r="C30" s="159"/>
       <c r="D30" s="16" t="s">
         <v>65</v>
       </c>
@@ -40666,20 +40718,20 @@
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="143" t="s">
+      <c r="B32" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="143" t="s">
+      <c r="C32" s="154" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="145" t="s">
+      <c r="D32" s="156" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="146"/>
+      <c r="E32" s="157"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="144"/>
-      <c r="C33" s="144"/>
+      <c r="B33" s="155"/>
+      <c r="C33" s="155"/>
       <c r="D33" s="17" t="s">
         <v>54</v>
       </c>
@@ -40694,16 +40746,16 @@
       <c r="C34" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D34" s="147" t="s">
+      <c r="D34" s="160" t="s">
         <v>130</v>
       </c>
-      <c r="E34" s="148"/>
+      <c r="E34" s="161"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="149" t="s">
+      <c r="B35" s="158" t="s">
         <v>128</v>
       </c>
-      <c r="C35" s="150" t="s">
+      <c r="C35" s="159" t="s">
         <v>53</v>
       </c>
       <c r="D35" s="16" t="s">
@@ -40714,8 +40766,8 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="149"/>
-      <c r="C36" s="150"/>
+      <c r="B36" s="158"/>
+      <c r="C36" s="159"/>
       <c r="D36" s="16" t="s">
         <v>58</v>
       </c>
@@ -40724,18 +40776,18 @@
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="149"/>
-      <c r="C37" s="150"/>
+      <c r="B37" s="158"/>
+      <c r="C37" s="159"/>
       <c r="D37" s="16" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="149"/>
-      <c r="C38" s="150"/>
+      <c r="B38" s="158"/>
+      <c r="C38" s="159"/>
       <c r="D38" s="16" t="s">
         <v>131</v>
       </c>
@@ -40745,6 +40797,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -40758,18 +40822,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="C7:C12"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40785,7 +40837,7 @@
   <dimension ref="A4:E31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="A24:D24"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40798,21 +40850,21 @@
   <sheetData>
     <row r="4" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="143" t="s">
+      <c r="C4" s="154" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="145" t="s">
+      <c r="D4" s="156" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="146"/>
+      <c r="E4" s="157"/>
     </row>
     <row r="5" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="144"/>
-      <c r="C5" s="144"/>
+      <c r="B5" s="155"/>
+      <c r="C5" s="155"/>
       <c r="D5" s="17" t="s">
         <v>54</v>
       </c>
@@ -40822,10 +40874,10 @@
     </row>
     <row r="6" spans="1:5" s="5" customFormat="1" ht="23.25" customHeight="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="152" t="s">
+      <c r="B6" s="162" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="155" t="s">
+      <c r="C6" s="165" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="16" t="s">
@@ -40837,8 +40889,8 @@
     </row>
     <row r="7" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="153"/>
-      <c r="C7" s="156"/>
+      <c r="B7" s="163"/>
+      <c r="C7" s="166"/>
       <c r="D7" s="16" t="s">
         <v>61</v>
       </c>
@@ -40848,8 +40900,8 @@
     </row>
     <row r="8" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="153"/>
-      <c r="C8" s="156"/>
+      <c r="B8" s="163"/>
+      <c r="C8" s="166"/>
       <c r="D8" s="16" t="s">
         <v>60</v>
       </c>
@@ -40859,28 +40911,28 @@
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="153"/>
-      <c r="C9" s="156"/>
+      <c r="B9" s="163"/>
+      <c r="C9" s="166"/>
       <c r="D9" s="16" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="153"/>
-      <c r="C10" s="156"/>
+      <c r="B10" s="163"/>
+      <c r="C10" s="166"/>
       <c r="D10" s="16" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="154"/>
-      <c r="C11" s="157"/>
+      <c r="B11" s="164"/>
+      <c r="C11" s="167"/>
       <c r="D11" s="16" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E11" s="19"/>
     </row>
@@ -40970,20 +41022,20 @@
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" ht="23.25">
-      <c r="B25" s="143" t="s">
+      <c r="B25" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="143" t="s">
+      <c r="C25" s="154" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="145" t="s">
+      <c r="D25" s="156" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="146"/>
+      <c r="E25" s="157"/>
     </row>
     <row r="26" spans="1:5" ht="23.25">
-      <c r="B26" s="144"/>
-      <c r="C26" s="144"/>
+      <c r="B26" s="155"/>
+      <c r="C26" s="155"/>
       <c r="D26" s="17" t="s">
         <v>54</v>
       </c>
@@ -40998,16 +41050,16 @@
       <c r="C27" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="147" t="s">
+      <c r="D27" s="160" t="s">
         <v>134</v>
       </c>
-      <c r="E27" s="148"/>
+      <c r="E27" s="161"/>
     </row>
     <row r="28" spans="1:5" ht="23.25" customHeight="1">
-      <c r="B28" s="149" t="s">
+      <c r="B28" s="158" t="s">
         <v>132</v>
       </c>
-      <c r="C28" s="150" t="s">
+      <c r="C28" s="159" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="16" t="s">
@@ -41016,42 +41068,42 @@
       <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:5" ht="23.25">
-      <c r="B29" s="149"/>
-      <c r="C29" s="150"/>
+      <c r="B29" s="158"/>
+      <c r="C29" s="159"/>
       <c r="D29" s="16" t="s">
         <v>58</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:5" ht="23.25">
-      <c r="B30" s="149"/>
-      <c r="C30" s="150"/>
+      <c r="B30" s="158"/>
+      <c r="C30" s="159"/>
       <c r="D30" s="16" t="s">
         <v>59</v>
       </c>
       <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5" ht="23.25">
-      <c r="B31" s="149"/>
-      <c r="C31" s="150"/>
+      <c r="B31" s="158"/>
+      <c r="C31" s="159"/>
       <c r="D31" s="16" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E31" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B6:B11"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="C28:C31"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="B6:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -41066,8 +41118,8 @@
   </sheetPr>
   <dimension ref="A1:Z235"/>
   <sheetViews>
-    <sheetView topLeftCell="B60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB184" sqref="AB184"/>
+    <sheetView topLeftCell="B162" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -41088,46 +41140,46 @@
     </row>
     <row r="3" spans="1:26">
       <c r="S3" s="67"/>
-      <c r="T3" s="160" t="s">
+      <c r="T3" s="170" t="s">
         <v>81</v>
       </c>
-      <c r="U3" s="160"/>
-      <c r="V3" s="160"/>
-      <c r="W3" s="160"/>
-      <c r="X3" s="160"/>
-      <c r="Y3" s="160"/>
+      <c r="U3" s="170"/>
+      <c r="V3" s="170"/>
+      <c r="W3" s="170"/>
+      <c r="X3" s="170"/>
+      <c r="Y3" s="170"/>
       <c r="Z3" s="68"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="161">
+      <c r="A4" s="171">
         <v>1</v>
       </c>
       <c r="S4" s="67"/>
-      <c r="T4" s="160"/>
-      <c r="U4" s="160"/>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="160"/>
+      <c r="T4" s="170"/>
+      <c r="U4" s="170"/>
+      <c r="V4" s="170"/>
+      <c r="W4" s="170"/>
+      <c r="X4" s="170"/>
+      <c r="Y4" s="170"/>
       <c r="Z4" s="68"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="161"/>
+      <c r="A5" s="171"/>
       <c r="S5" s="67"/>
-      <c r="T5" s="158" t="s">
+      <c r="T5" s="168" t="s">
         <v>84</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="159" t="s">
+      <c r="U5" s="168"/>
+      <c r="V5" s="168"/>
+      <c r="W5" s="169" t="s">
         <v>83</v>
       </c>
-      <c r="X5" s="158"/>
-      <c r="Y5" s="158"/>
+      <c r="X5" s="168"/>
+      <c r="Y5" s="168"/>
       <c r="Z5" s="68"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="161"/>
+      <c r="A6" s="171"/>
       <c r="S6" s="67"/>
       <c r="V6" t="s">
         <v>80</v>
@@ -41136,7 +41188,7 @@
       <c r="Z6" s="68"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="161"/>
+      <c r="A7" s="171"/>
       <c r="S7" s="67"/>
       <c r="W7" s="15"/>
       <c r="Y7" t="s">
@@ -41145,13 +41197,13 @@
       <c r="Z7" s="68"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="161"/>
+      <c r="A8" s="171"/>
       <c r="S8" s="67"/>
       <c r="W8" s="15"/>
       <c r="Z8" s="68"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="161"/>
+      <c r="A9" s="171"/>
       <c r="S9" s="67"/>
       <c r="V9" t="s">
         <v>82</v>
@@ -41160,13 +41212,13 @@
       <c r="Z9" s="68"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="161"/>
+      <c r="A10" s="171"/>
       <c r="S10" s="67"/>
       <c r="W10" s="15"/>
       <c r="Z10" s="68"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="161"/>
+      <c r="A11" s="171"/>
       <c r="S11" s="67"/>
       <c r="W11" s="15"/>
       <c r="Z11" s="68"/>
@@ -41252,186 +41304,186 @@
       <c r="Z25" s="71"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="161">
+      <c r="A36" s="171">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="161"/>
+      <c r="A37" s="171"/>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="161"/>
+      <c r="A38" s="171"/>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="161"/>
+      <c r="A39" s="171"/>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="161"/>
+      <c r="A40" s="171"/>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="161"/>
+      <c r="A41" s="171"/>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="161"/>
+      <c r="A42" s="171"/>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="161"/>
+      <c r="A43" s="171"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="161">
+      <c r="A68" s="171">
         <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="161"/>
+      <c r="A69" s="171"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="161"/>
+      <c r="A70" s="171"/>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="161"/>
+      <c r="A71" s="171"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="161"/>
+      <c r="A72" s="171"/>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="161"/>
+      <c r="A73" s="171"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="161"/>
+      <c r="A74" s="171"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="161"/>
+      <c r="A75" s="171"/>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="161">
+      <c r="A100" s="171">
         <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="161"/>
+      <c r="A101" s="171"/>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="161"/>
+      <c r="A102" s="171"/>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="161"/>
+      <c r="A103" s="171"/>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="161"/>
+      <c r="A104" s="171"/>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="161"/>
+      <c r="A105" s="171"/>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="161"/>
+      <c r="A106" s="171"/>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="161"/>
+      <c r="A107" s="171"/>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="161">
+      <c r="A132" s="171">
         <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:1">
-      <c r="A133" s="161"/>
+      <c r="A133" s="171"/>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="161"/>
+      <c r="A134" s="171"/>
     </row>
     <row r="135" spans="1:1">
-      <c r="A135" s="161"/>
+      <c r="A135" s="171"/>
     </row>
     <row r="136" spans="1:1">
-      <c r="A136" s="161"/>
+      <c r="A136" s="171"/>
     </row>
     <row r="137" spans="1:1">
-      <c r="A137" s="161"/>
+      <c r="A137" s="171"/>
     </row>
     <row r="138" spans="1:1">
-      <c r="A138" s="161"/>
+      <c r="A138" s="171"/>
     </row>
     <row r="139" spans="1:1">
-      <c r="A139" s="161"/>
+      <c r="A139" s="171"/>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="161">
+      <c r="A164" s="171">
         <v>6</v>
       </c>
     </row>
     <row r="165" spans="1:1">
-      <c r="A165" s="161"/>
+      <c r="A165" s="171"/>
     </row>
     <row r="166" spans="1:1">
-      <c r="A166" s="161"/>
+      <c r="A166" s="171"/>
     </row>
     <row r="167" spans="1:1">
-      <c r="A167" s="161"/>
+      <c r="A167" s="171"/>
     </row>
     <row r="168" spans="1:1">
-      <c r="A168" s="161"/>
+      <c r="A168" s="171"/>
     </row>
     <row r="169" spans="1:1">
-      <c r="A169" s="161"/>
+      <c r="A169" s="171"/>
     </row>
     <row r="170" spans="1:1">
-      <c r="A170" s="161"/>
+      <c r="A170" s="171"/>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" s="161"/>
+      <c r="A171" s="171"/>
     </row>
     <row r="196" spans="1:1">
-      <c r="A196" s="161">
+      <c r="A196" s="171">
         <v>7</v>
       </c>
     </row>
     <row r="197" spans="1:1">
-      <c r="A197" s="161"/>
+      <c r="A197" s="171"/>
     </row>
     <row r="198" spans="1:1">
-      <c r="A198" s="161"/>
+      <c r="A198" s="171"/>
     </row>
     <row r="199" spans="1:1">
-      <c r="A199" s="161"/>
+      <c r="A199" s="171"/>
     </row>
     <row r="200" spans="1:1">
-      <c r="A200" s="161"/>
+      <c r="A200" s="171"/>
     </row>
     <row r="201" spans="1:1">
-      <c r="A201" s="161"/>
+      <c r="A201" s="171"/>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" s="161"/>
+      <c r="A202" s="171"/>
     </row>
     <row r="203" spans="1:1">
-      <c r="A203" s="161"/>
+      <c r="A203" s="171"/>
     </row>
     <row r="228" spans="1:1">
-      <c r="A228" s="161">
+      <c r="A228" s="171">
         <v>8</v>
       </c>
     </row>
     <row r="229" spans="1:1">
-      <c r="A229" s="161"/>
+      <c r="A229" s="171"/>
     </row>
     <row r="230" spans="1:1">
-      <c r="A230" s="161"/>
+      <c r="A230" s="171"/>
     </row>
     <row r="231" spans="1:1">
-      <c r="A231" s="161"/>
+      <c r="A231" s="171"/>
     </row>
     <row r="232" spans="1:1">
-      <c r="A232" s="161"/>
+      <c r="A232" s="171"/>
     </row>
     <row r="233" spans="1:1">
-      <c r="A233" s="161"/>
+      <c r="A233" s="171"/>
     </row>
     <row r="234" spans="1:1">
-      <c r="A234" s="161"/>
+      <c r="A234" s="171"/>
     </row>
     <row r="235" spans="1:1">
-      <c r="A235" s="161"/>
+      <c r="A235" s="171"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -41478,62 +41530,62 @@
   </cols>
   <sheetData>
     <row r="70" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="C70" s="162" t="s">
-        <v>189</v>
+      <c r="C70" s="172" t="s">
+        <v>184</v>
       </c>
-      <c r="D70" s="162" t="s">
+      <c r="D70" s="172" t="s">
+        <v>169</v>
+      </c>
+      <c r="E70" s="172" t="s">
+        <v>168</v>
+      </c>
+      <c r="F70" s="175" t="s">
         <v>174</v>
       </c>
-      <c r="E70" s="162" t="s">
+      <c r="G70" s="172" t="s">
+        <v>167</v>
+      </c>
+      <c r="H70" s="172" t="s">
         <v>173</v>
       </c>
-      <c r="F70" s="165" t="s">
-        <v>179</v>
+      <c r="I70" s="172"/>
+      <c r="J70" s="172" t="s">
+        <v>3</v>
       </c>
-      <c r="G70" s="162" t="s">
+      <c r="K70" s="172"/>
+      <c r="L70" s="172"/>
+      <c r="M70" s="172"/>
+    </row>
+    <row r="71" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
+      <c r="C71" s="172"/>
+      <c r="D71" s="172"/>
+      <c r="E71" s="172"/>
+      <c r="F71" s="172"/>
+      <c r="G71" s="172"/>
+      <c r="H71" s="75" t="s">
         <v>172</v>
       </c>
-      <c r="H70" s="162" t="s">
-        <v>178</v>
-      </c>
-      <c r="I70" s="162"/>
-      <c r="J70" s="162" t="s">
-        <v>3</v>
-      </c>
-      <c r="K70" s="162"/>
-      <c r="L70" s="162"/>
-      <c r="M70" s="162"/>
-    </row>
-    <row r="71" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="C71" s="162"/>
-      <c r="D71" s="162"/>
-      <c r="E71" s="162"/>
-      <c r="F71" s="162"/>
-      <c r="G71" s="162"/>
-      <c r="H71" s="75" t="s">
-        <v>177</v>
-      </c>
       <c r="I71" s="76" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="J71" s="75" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="K71" s="75" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="L71" s="75" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="M71" s="84" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="3:13" s="2" customFormat="1" ht="151.5" customHeight="1">
-      <c r="C72" s="163" t="s">
-        <v>205</v>
+      <c r="C72" s="173" t="s">
+        <v>200</v>
       </c>
-      <c r="D72" s="164"/>
+      <c r="D72" s="174"/>
       <c r="E72" s="77"/>
       <c r="F72" s="78"/>
       <c r="G72" s="78"/>
@@ -41544,113 +41596,113 @@
     </row>
     <row r="73" spans="3:13" s="2" customFormat="1" ht="139.5">
       <c r="C73" s="89" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E73" s="77" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F73" s="78" t="s">
+        <v>176</v>
+      </c>
+      <c r="G73" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="H73" s="79" t="s">
+        <v>178</v>
+      </c>
+      <c r="I73" s="80" t="s">
+        <v>179</v>
+      </c>
+      <c r="J73" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="G73" s="78" t="s">
+      <c r="K73" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="H73" s="79" t="s">
-        <v>183</v>
-      </c>
-      <c r="I73" s="80" t="s">
-        <v>184</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="L73" s="81" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="M73" s="85" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="D74" s="82" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G74" s="78" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="L74" s="81" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="M74" s="85" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="75" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C75" s="88" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="M75" s="86"/>
     </row>
     <row r="76" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="D76" s="82" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="M76" s="86"/>
     </row>
     <row r="77" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="D77" s="82" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="M77" s="86"/>
     </row>
     <row r="78" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C78" s="83" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="M78" s="86"/>
     </row>
     <row r="79" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C79" s="83" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="M79" s="86"/>
     </row>
     <row r="80" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C80" s="83" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="M80" s="86"/>
     </row>
     <row r="81" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C81" s="83" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="M81" s="86"/>
     </row>
     <row r="82" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C82" s="83" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="M82" s="86"/>
     </row>
     <row r="83" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C83" s="83" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="M83" s="86"/>
     </row>

</xml_diff>

<commit_message>
I've authenticated the app with Firebase authentication and implemented both a login page and a signup page
</commit_message>
<xml_diff>
--- a/Final-React-Project-Design.xlsx
+++ b/Final-React-Project-Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basheer\Desktop\בשיר\Full Stack Work\Full Stack Cors - YanivArad\Projects\React-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC355FA-0CE9-4C86-916B-67194A13CA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEC5E39-A5E3-4FC7-A302-2B95C36CF47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="240">
   <si>
     <t>Num</t>
   </si>
@@ -6647,6 +6647,15 @@
     <xf numFmtId="0" fontId="59" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -6659,14 +6668,95 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6695,19 +6785,7 @@
     <xf numFmtId="0" fontId="47" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6722,80 +6800,11 @@
     <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6809,16 +6818,19 @@
     <xf numFmtId="0" fontId="25" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6862,18 +6874,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -39179,7 +39179,7 @@
   <dimension ref="B3:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15"/>
@@ -39197,44 +39197,44 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="109" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="107" t="s">
+      <c r="B6" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="107" t="s">
+      <c r="C6" s="110" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="107" t="s">
+      <c r="D6" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="107" t="s">
+      <c r="E6" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="107" t="s">
+      <c r="F6" s="110" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="107"/>
-      <c r="C7" s="107"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
+      <c r="B7" s="110"/>
+      <c r="C7" s="110"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="46">
@@ -39272,7 +39272,7 @@
       <c r="B10" s="46">
         <v>2</v>
       </c>
-      <c r="C10" s="104" t="s">
+      <c r="C10" s="107" t="s">
         <v>68</v>
       </c>
       <c r="D10" s="47" t="s">
@@ -39289,7 +39289,7 @@
       <c r="B11" s="46">
         <v>3</v>
       </c>
-      <c r="C11" s="105"/>
+      <c r="C11" s="108"/>
       <c r="D11" s="46" t="s">
         <v>70</v>
       </c>
@@ -39449,7 +39449,9 @@
       <c r="E20" s="46" t="s">
         <v>223</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="21" spans="2:6" ht="30">
       <c r="B21" s="46">
@@ -39464,7 +39466,9 @@
       <c r="E21" s="46" t="s">
         <v>238</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" s="46">
@@ -39479,7 +39483,9 @@
       <c r="E22" s="46" t="s">
         <v>239</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" s="46">
@@ -39491,7 +39497,7 @@
       <c r="D23" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="E23" s="179">
+      <c r="E23" s="106">
         <v>44938</v>
       </c>
       <c r="F23" s="1"/>
@@ -39506,7 +39512,7 @@
       <c r="D24" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="E24" s="179">
+      <c r="E24" s="106">
         <v>44938</v>
       </c>
       <c r="F24" s="1"/>
@@ -39615,36 +39621,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="51.75" customHeight="1">
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="139" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" thickBot="1">
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B4" s="134" t="s">
+      <c r="B4" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="147" t="s">
+      <c r="C4" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="147" t="s">
+      <c r="D4" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="147" t="s">
+      <c r="E4" s="119" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="148"/>
+      <c r="F4" s="134"/>
     </row>
     <row r="5" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B5" s="135"/>
-      <c r="C5" s="150"/>
-      <c r="D5" s="150"/>
+      <c r="B5" s="127"/>
+      <c r="C5" s="120"/>
+      <c r="D5" s="120"/>
       <c r="E5" s="31" t="s">
         <v>9</v>
       </c>
@@ -39653,10 +39659,10 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B6" s="113">
+      <c r="B6" s="143">
         <v>1</v>
       </c>
-      <c r="C6" s="110" t="s">
+      <c r="C6" s="122" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="73" t="s">
@@ -39670,12 +39676,12 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B7" s="114"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="124" t="s">
+      <c r="B7" s="144"/>
+      <c r="C7" s="141"/>
+      <c r="D7" s="113" t="s">
         <v>225</v>
       </c>
-      <c r="E7" s="121" t="s">
+      <c r="E7" s="136" t="s">
         <v>230</v>
       </c>
       <c r="F7" s="101" t="s">
@@ -39683,50 +39689,50 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B8" s="114"/>
-      <c r="C8" s="111"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="122"/>
+      <c r="B8" s="144"/>
+      <c r="C8" s="141"/>
+      <c r="D8" s="151"/>
+      <c r="E8" s="137"/>
       <c r="F8" s="101" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B9" s="114"/>
-      <c r="C9" s="111"/>
-      <c r="D9" s="125"/>
-      <c r="E9" s="122"/>
+      <c r="B9" s="144"/>
+      <c r="C9" s="141"/>
+      <c r="D9" s="151"/>
+      <c r="E9" s="137"/>
       <c r="F9" s="101" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B10" s="114"/>
-      <c r="C10" s="111"/>
-      <c r="D10" s="125"/>
-      <c r="E10" s="122"/>
+      <c r="B10" s="144"/>
+      <c r="C10" s="141"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="137"/>
       <c r="F10" s="102"/>
     </row>
     <row r="11" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B11" s="132"/>
-      <c r="C11" s="131"/>
-      <c r="D11" s="133"/>
-      <c r="E11" s="151"/>
+      <c r="B11" s="156"/>
+      <c r="C11" s="123"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="138"/>
       <c r="F11" s="103" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="22.5">
-      <c r="B12" s="129">
+      <c r="B12" s="130">
         <v>2</v>
       </c>
-      <c r="C12" s="136" t="s">
+      <c r="C12" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="144" t="s">
+      <c r="D12" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="141" t="s">
+      <c r="E12" s="117" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="38" t="s">
@@ -39734,63 +39740,63 @@
       </c>
     </row>
     <row r="13" spans="2:6" ht="22.5">
-      <c r="B13" s="130"/>
-      <c r="C13" s="137"/>
-      <c r="D13" s="145"/>
-      <c r="E13" s="142"/>
+      <c r="B13" s="131"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="118"/>
       <c r="F13" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="22.5">
-      <c r="B14" s="130"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="145"/>
-      <c r="E14" s="142"/>
+      <c r="B14" s="131"/>
+      <c r="C14" s="115"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="118"/>
       <c r="F14" s="21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="22.5">
-      <c r="B15" s="130"/>
-      <c r="C15" s="137"/>
-      <c r="D15" s="145"/>
-      <c r="E15" s="142"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="118"/>
       <c r="F15" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="22.5">
-      <c r="B16" s="130"/>
-      <c r="C16" s="137"/>
-      <c r="D16" s="145"/>
-      <c r="E16" s="142"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="115"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="118"/>
       <c r="F16" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="22.5">
-      <c r="B17" s="130"/>
-      <c r="C17" s="137"/>
-      <c r="D17" s="145"/>
-      <c r="E17" s="142"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="115"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="118"/>
       <c r="F17" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="22.5">
-      <c r="B18" s="130"/>
-      <c r="C18" s="137"/>
-      <c r="D18" s="145"/>
-      <c r="E18" s="142"/>
+      <c r="B18" s="131"/>
+      <c r="C18" s="115"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="118"/>
       <c r="F18" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B19" s="143"/>
-      <c r="C19" s="138"/>
-      <c r="D19" s="146"/>
+      <c r="B19" s="132"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="133"/>
       <c r="E19" s="40" t="s">
         <v>13</v>
       </c>
@@ -39799,16 +39805,16 @@
       </c>
     </row>
     <row r="20" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B20" s="129">
+      <c r="B20" s="130">
         <v>3</v>
       </c>
-      <c r="C20" s="136" t="s">
+      <c r="C20" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="144" t="s">
+      <c r="D20" s="111" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="141" t="s">
+      <c r="E20" s="117" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="41" t="s">
@@ -39816,45 +39822,45 @@
       </c>
     </row>
     <row r="21" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B21" s="130"/>
-      <c r="C21" s="137"/>
-      <c r="D21" s="145"/>
-      <c r="E21" s="142"/>
+      <c r="B21" s="131"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="118"/>
       <c r="F21" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B22" s="130"/>
-      <c r="C22" s="137"/>
-      <c r="D22" s="145"/>
-      <c r="E22" s="142"/>
+      <c r="B22" s="131"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="118"/>
       <c r="F22" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B23" s="130"/>
-      <c r="C23" s="137"/>
-      <c r="D23" s="145"/>
-      <c r="E23" s="142"/>
+      <c r="B23" s="131"/>
+      <c r="C23" s="115"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="118"/>
       <c r="F23" s="26" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B24" s="130"/>
-      <c r="C24" s="137"/>
-      <c r="D24" s="145"/>
-      <c r="E24" s="142"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="115"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="27" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B25" s="143"/>
-      <c r="C25" s="138"/>
-      <c r="D25" s="146"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="116"/>
+      <c r="D25" s="133"/>
       <c r="E25" s="40" t="s">
         <v>13</v>
       </c>
@@ -39863,16 +39869,16 @@
       </c>
     </row>
     <row r="26" spans="2:6" ht="22.5">
-      <c r="B26" s="129">
+      <c r="B26" s="130">
         <v>4</v>
       </c>
-      <c r="C26" s="136" t="s">
+      <c r="C26" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="144" t="s">
+      <c r="D26" s="111" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="141" t="s">
+      <c r="E26" s="117" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="41" t="s">
@@ -39880,27 +39886,27 @@
       </c>
     </row>
     <row r="27" spans="2:6" ht="22.5">
-      <c r="B27" s="130"/>
-      <c r="C27" s="137"/>
-      <c r="D27" s="145"/>
-      <c r="E27" s="142"/>
+      <c r="B27" s="131"/>
+      <c r="C27" s="115"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="118"/>
       <c r="F27" s="28" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="22.5">
-      <c r="B28" s="130"/>
-      <c r="C28" s="137"/>
-      <c r="D28" s="145"/>
-      <c r="E28" s="142"/>
+      <c r="B28" s="131"/>
+      <c r="C28" s="115"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="118"/>
       <c r="F28" s="29" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="42" customHeight="1" thickBot="1">
-      <c r="B29" s="120"/>
-      <c r="C29" s="149"/>
-      <c r="D29" s="124"/>
+      <c r="B29" s="155"/>
+      <c r="C29" s="135"/>
+      <c r="D29" s="113"/>
       <c r="E29" s="12" t="s">
         <v>13</v>
       </c>
@@ -39926,16 +39932,16 @@
       </c>
     </row>
     <row r="31" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B31" s="129">
+      <c r="B31" s="130">
         <v>6</v>
       </c>
-      <c r="C31" s="136" t="s">
+      <c r="C31" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="139" t="s">
+      <c r="D31" s="128" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="141" t="s">
+      <c r="E31" s="117" t="s">
         <v>13</v>
       </c>
       <c r="F31" s="41" t="s">
@@ -39943,17 +39949,17 @@
       </c>
     </row>
     <row r="32" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B32" s="130"/>
-      <c r="C32" s="137"/>
-      <c r="D32" s="140"/>
-      <c r="E32" s="142"/>
+      <c r="B32" s="131"/>
+      <c r="C32" s="115"/>
+      <c r="D32" s="129"/>
+      <c r="E32" s="118"/>
       <c r="F32" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B33" s="143"/>
-      <c r="C33" s="138"/>
+      <c r="B33" s="132"/>
+      <c r="C33" s="116"/>
       <c r="D33" s="39" t="s">
         <v>39</v>
       </c>
@@ -39997,10 +40003,10 @@
       </c>
     </row>
     <row r="36" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B36" s="113">
+      <c r="B36" s="143">
         <v>9</v>
       </c>
-      <c r="C36" s="110" t="s">
+      <c r="C36" s="122" t="s">
         <v>90</v>
       </c>
       <c r="D36" s="73" t="s">
@@ -40014,12 +40020,12 @@
       </c>
     </row>
     <row r="37" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B37" s="114"/>
-      <c r="C37" s="111"/>
-      <c r="D37" s="124" t="s">
+      <c r="B37" s="144"/>
+      <c r="C37" s="141"/>
+      <c r="D37" s="113" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="121" t="s">
+      <c r="E37" s="136" t="s">
         <v>96</v>
       </c>
       <c r="F37" s="55" t="s">
@@ -40027,37 +40033,37 @@
       </c>
     </row>
     <row r="38" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B38" s="114"/>
-      <c r="C38" s="111"/>
-      <c r="D38" s="125"/>
-      <c r="E38" s="122"/>
+      <c r="B38" s="144"/>
+      <c r="C38" s="141"/>
+      <c r="D38" s="151"/>
+      <c r="E38" s="137"/>
       <c r="F38" s="51" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B39" s="114"/>
-      <c r="C39" s="111"/>
-      <c r="D39" s="125"/>
-      <c r="E39" s="122"/>
+      <c r="B39" s="144"/>
+      <c r="C39" s="141"/>
+      <c r="D39" s="151"/>
+      <c r="E39" s="137"/>
       <c r="F39" s="51" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B40" s="114"/>
-      <c r="C40" s="111"/>
-      <c r="D40" s="125"/>
-      <c r="E40" s="123"/>
+      <c r="B40" s="144"/>
+      <c r="C40" s="141"/>
+      <c r="D40" s="151"/>
+      <c r="E40" s="150"/>
       <c r="F40" s="56" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B41" s="114"/>
-      <c r="C41" s="111"/>
-      <c r="D41" s="125"/>
-      <c r="E41" s="121" t="s">
+      <c r="B41" s="144"/>
+      <c r="C41" s="141"/>
+      <c r="D41" s="151"/>
+      <c r="E41" s="136" t="s">
         <v>98</v>
       </c>
       <c r="F41" s="57" t="s">
@@ -40065,54 +40071,54 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B42" s="114"/>
-      <c r="C42" s="111"/>
-      <c r="D42" s="125"/>
-      <c r="E42" s="122"/>
+      <c r="B42" s="144"/>
+      <c r="C42" s="141"/>
+      <c r="D42" s="151"/>
+      <c r="E42" s="137"/>
       <c r="F42" s="58" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B43" s="114"/>
-      <c r="C43" s="111"/>
-      <c r="D43" s="125"/>
-      <c r="E43" s="122"/>
+      <c r="B43" s="144"/>
+      <c r="C43" s="141"/>
+      <c r="D43" s="151"/>
+      <c r="E43" s="137"/>
       <c r="F43" s="58" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B44" s="114"/>
-      <c r="C44" s="111"/>
-      <c r="D44" s="125"/>
-      <c r="E44" s="122"/>
+      <c r="B44" s="144"/>
+      <c r="C44" s="141"/>
+      <c r="D44" s="151"/>
+      <c r="E44" s="137"/>
       <c r="F44" s="59" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B45" s="114"/>
-      <c r="C45" s="111"/>
-      <c r="D45" s="125"/>
-      <c r="E45" s="122"/>
+      <c r="B45" s="144"/>
+      <c r="C45" s="141"/>
+      <c r="D45" s="151"/>
+      <c r="E45" s="137"/>
       <c r="F45" s="59" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B46" s="114"/>
-      <c r="C46" s="111"/>
-      <c r="D46" s="126"/>
-      <c r="E46" s="123"/>
+      <c r="B46" s="144"/>
+      <c r="C46" s="141"/>
+      <c r="D46" s="152"/>
+      <c r="E46" s="150"/>
       <c r="F46" s="60" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="75">
-      <c r="B47" s="114"/>
-      <c r="C47" s="111"/>
-      <c r="D47" s="124" t="s">
+      <c r="B47" s="144"/>
+      <c r="C47" s="141"/>
+      <c r="D47" s="113" t="s">
         <v>97</v>
       </c>
       <c r="E47" s="10" t="s">
@@ -40123,10 +40129,10 @@
       </c>
     </row>
     <row r="48" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B48" s="114"/>
-      <c r="C48" s="111"/>
-      <c r="D48" s="125"/>
-      <c r="E48" s="127" t="s">
+      <c r="B48" s="144"/>
+      <c r="C48" s="141"/>
+      <c r="D48" s="151"/>
+      <c r="E48" s="153" t="s">
         <v>109</v>
       </c>
       <c r="F48" s="58" t="s">
@@ -40134,28 +40140,28 @@
       </c>
     </row>
     <row r="49" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B49" s="114"/>
-      <c r="C49" s="111"/>
-      <c r="D49" s="125"/>
-      <c r="E49" s="127"/>
+      <c r="B49" s="144"/>
+      <c r="C49" s="141"/>
+      <c r="D49" s="151"/>
+      <c r="E49" s="153"/>
       <c r="F49" s="59" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B50" s="114"/>
-      <c r="C50" s="111"/>
-      <c r="D50" s="125"/>
-      <c r="E50" s="127"/>
+      <c r="B50" s="144"/>
+      <c r="C50" s="141"/>
+      <c r="D50" s="151"/>
+      <c r="E50" s="153"/>
       <c r="F50" s="59" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B51" s="115"/>
-      <c r="C51" s="112"/>
-      <c r="D51" s="126"/>
-      <c r="E51" s="128"/>
+      <c r="B51" s="145"/>
+      <c r="C51" s="142"/>
+      <c r="D51" s="152"/>
+      <c r="E51" s="154"/>
       <c r="F51" s="60" t="s">
         <v>99</v>
       </c>
@@ -40166,22 +40172,22 @@
       <c r="D52" s="98" t="s">
         <v>231</v>
       </c>
-      <c r="E52" s="176" t="s">
+      <c r="E52" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="177"/>
+      <c r="F52" s="105"/>
     </row>
     <row r="53" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B53" s="114">
+      <c r="B53" s="144">
         <v>10</v>
       </c>
-      <c r="C53" s="118" t="s">
+      <c r="C53" s="148" t="s">
         <v>117</v>
       </c>
-      <c r="D53" s="116" t="s">
+      <c r="D53" s="146" t="s">
         <v>126</v>
       </c>
-      <c r="E53" s="122" t="s">
+      <c r="E53" s="137" t="s">
         <v>118</v>
       </c>
       <c r="F53" s="62" t="s">
@@ -40189,44 +40195,44 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B54" s="114"/>
-      <c r="C54" s="118"/>
-      <c r="D54" s="116"/>
-      <c r="E54" s="122"/>
+      <c r="B54" s="144"/>
+      <c r="C54" s="148"/>
+      <c r="D54" s="146"/>
+      <c r="E54" s="137"/>
       <c r="F54" s="62" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B55" s="114"/>
-      <c r="C55" s="118"/>
-      <c r="D55" s="116"/>
-      <c r="E55" s="122"/>
+      <c r="B55" s="144"/>
+      <c r="C55" s="148"/>
+      <c r="D55" s="146"/>
+      <c r="E55" s="137"/>
       <c r="F55" s="63" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B56" s="114"/>
-      <c r="C56" s="118"/>
-      <c r="D56" s="116"/>
-      <c r="E56" s="122"/>
+      <c r="B56" s="144"/>
+      <c r="C56" s="148"/>
+      <c r="D56" s="146"/>
+      <c r="E56" s="137"/>
       <c r="F56" s="62" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="57" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B57" s="115"/>
-      <c r="C57" s="119"/>
-      <c r="D57" s="117"/>
-      <c r="E57" s="123"/>
+      <c r="B57" s="145"/>
+      <c r="C57" s="149"/>
+      <c r="D57" s="147"/>
+      <c r="E57" s="150"/>
       <c r="F57" s="62" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="58" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B58" s="33"/>
-      <c r="C58" s="110" t="s">
+      <c r="C58" s="122" t="s">
         <v>206</v>
       </c>
       <c r="D58" s="72" t="s">
@@ -40238,13 +40244,13 @@
       <c r="F58" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="G58" s="152" t="s">
+      <c r="G58" s="121" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="59" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B59" s="33"/>
-      <c r="C59" s="131"/>
+      <c r="C59" s="123"/>
       <c r="D59" s="72" t="s">
         <v>208</v>
       </c>
@@ -40254,7 +40260,7 @@
       <c r="F59" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="G59" s="152"/>
+      <c r="G59" s="121"/>
     </row>
     <row r="60" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B60" s="96"/>
@@ -40271,7 +40277,7 @@
       <c r="C61" s="97" t="s">
         <v>235</v>
       </c>
-      <c r="D61" s="178" t="s">
+      <c r="D61" s="124" t="s">
         <v>233</v>
       </c>
       <c r="E61" s="99"/>
@@ -40283,7 +40289,7 @@
     <row r="62" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B62" s="96"/>
       <c r="C62" s="97"/>
-      <c r="D62" s="133"/>
+      <c r="D62" s="125"/>
       <c r="E62" s="99"/>
       <c r="F62" s="14" t="s">
         <v>236</v>
@@ -40293,7 +40299,7 @@
     <row r="63" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B63" s="96"/>
       <c r="C63" s="97"/>
-      <c r="D63" s="176"/>
+      <c r="D63" s="104"/>
       <c r="E63" s="99"/>
       <c r="F63" s="14"/>
       <c r="G63" s="93"/>
@@ -40301,7 +40307,7 @@
     <row r="64" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B64" s="96"/>
       <c r="C64" s="97"/>
-      <c r="D64" s="176"/>
+      <c r="D64" s="104"/>
       <c r="E64" s="99"/>
       <c r="F64" s="14"/>
       <c r="G64" s="93"/>
@@ -40314,10 +40320,10 @@
       <c r="F65" s="50"/>
     </row>
     <row r="66" spans="2:7" s="92" customFormat="1" ht="45.75" customHeight="1">
-      <c r="G66" s="152"/>
+      <c r="G66" s="121"/>
     </row>
     <row r="67" spans="2:7" s="92" customFormat="1" ht="45.75" customHeight="1">
-      <c r="G67" s="152"/>
+      <c r="G67" s="121"/>
     </row>
     <row r="68" spans="2:7" s="92" customFormat="1" ht="43.5" customHeight="1">
       <c r="G68" s="93"/>
@@ -40378,14 +40384,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="C12:C19"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="C36:C51"/>
+    <mergeCell ref="B36:B51"/>
+    <mergeCell ref="D53:D57"/>
+    <mergeCell ref="C53:C57"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="E53:E57"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="D37:D46"/>
+    <mergeCell ref="D47:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="D7:D11"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C31:C33"/>
     <mergeCell ref="D31:D32"/>
@@ -40402,22 +40416,14 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D12:D19"/>
     <mergeCell ref="E7:E11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="C36:C51"/>
-    <mergeCell ref="B36:B51"/>
-    <mergeCell ref="D53:D57"/>
-    <mergeCell ref="C53:C57"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="E53:E57"/>
-    <mergeCell ref="E37:E40"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="D37:D46"/>
-    <mergeCell ref="D47:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="C12:C19"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D61:D62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="28" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40431,8 +40437,8 @@
   </sheetPr>
   <dimension ref="A2:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -40447,12 +40453,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="30.75">
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="165" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -40463,20 +40469,20 @@
       <c r="M2" s="4"/>
     </row>
     <row r="4" spans="2:13">
-      <c r="B4" s="154" t="s">
+      <c r="B4" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="154" t="s">
+      <c r="C4" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="156" t="s">
+      <c r="D4" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="157"/>
+      <c r="E4" s="160"/>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="155"/>
-      <c r="C5" s="155"/>
+      <c r="B5" s="158"/>
+      <c r="C5" s="158"/>
       <c r="D5" s="17" t="s">
         <v>54</v>
       </c>
@@ -40491,16 +40497,16 @@
       <c r="C6" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="160" t="s">
+      <c r="D6" s="161" t="s">
         <v>137</v>
       </c>
-      <c r="E6" s="161"/>
+      <c r="E6" s="162"/>
     </row>
     <row r="7" spans="2:13" ht="23.25" customHeight="1">
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="166" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="165" t="s">
+      <c r="C7" s="169" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="16" t="s">
@@ -40514,8 +40520,8 @@
       </c>
     </row>
     <row r="8" spans="2:13">
-      <c r="B8" s="163"/>
-      <c r="C8" s="166"/>
+      <c r="B8" s="167"/>
+      <c r="C8" s="170"/>
       <c r="D8" s="16" t="s">
         <v>61</v>
       </c>
@@ -40524,8 +40530,8 @@
       </c>
     </row>
     <row r="9" spans="2:13">
-      <c r="B9" s="163"/>
-      <c r="C9" s="166"/>
+      <c r="B9" s="167"/>
+      <c r="C9" s="170"/>
       <c r="D9" s="16" t="s">
         <v>60</v>
       </c>
@@ -40534,8 +40540,8 @@
       </c>
     </row>
     <row r="10" spans="2:13">
-      <c r="B10" s="163"/>
-      <c r="C10" s="166"/>
+      <c r="B10" s="167"/>
+      <c r="C10" s="170"/>
       <c r="D10" s="16" t="s">
         <v>214</v>
       </c>
@@ -40544,8 +40550,8 @@
       </c>
     </row>
     <row r="11" spans="2:13">
-      <c r="B11" s="163"/>
-      <c r="C11" s="166"/>
+      <c r="B11" s="167"/>
+      <c r="C11" s="170"/>
       <c r="D11" s="16" t="s">
         <v>215</v>
       </c>
@@ -40554,8 +40560,8 @@
       </c>
     </row>
     <row r="12" spans="2:13">
-      <c r="B12" s="164"/>
-      <c r="C12" s="167"/>
+      <c r="B12" s="168"/>
+      <c r="C12" s="171"/>
       <c r="D12" s="16" t="s">
         <v>217</v>
       </c>
@@ -40564,20 +40570,20 @@
       </c>
     </row>
     <row r="15" spans="2:13">
-      <c r="B15" s="154" t="s">
+      <c r="B15" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="154" t="s">
+      <c r="C15" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="156" t="s">
+      <c r="D15" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="157"/>
+      <c r="E15" s="160"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="B16" s="155"/>
-      <c r="C16" s="155"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
       <c r="D16" s="17" t="s">
         <v>54</v>
       </c>
@@ -40592,16 +40598,16 @@
       <c r="C17" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="160" t="s">
+      <c r="D17" s="161" t="s">
         <v>134</v>
       </c>
-      <c r="E17" s="161"/>
+      <c r="E17" s="162"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="163" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="159" t="s">
+      <c r="C18" s="164" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="16" t="s">
@@ -40612,8 +40618,8 @@
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="158"/>
-      <c r="C19" s="159"/>
+      <c r="B19" s="163"/>
+      <c r="C19" s="164"/>
       <c r="D19" s="16" t="s">
         <v>58</v>
       </c>
@@ -40622,8 +40628,8 @@
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="158"/>
-      <c r="C20" s="159"/>
+      <c r="B20" s="163"/>
+      <c r="C20" s="164"/>
       <c r="D20" s="16" t="s">
         <v>59</v>
       </c>
@@ -40632,8 +40638,8 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="158"/>
-      <c r="C21" s="159"/>
+      <c r="B21" s="163"/>
+      <c r="C21" s="164"/>
       <c r="D21" s="16" t="s">
         <v>215</v>
       </c>
@@ -40642,20 +40648,20 @@
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="154" t="s">
+      <c r="B24" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="154" t="s">
+      <c r="C24" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="156" t="s">
+      <c r="D24" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="157"/>
+      <c r="E24" s="160"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="155"/>
-      <c r="C25" s="155"/>
+      <c r="B25" s="158"/>
+      <c r="C25" s="158"/>
       <c r="D25" s="17" t="s">
         <v>54</v>
       </c>
@@ -40670,16 +40676,16 @@
       <c r="C26" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="160" t="s">
+      <c r="D26" s="161" t="s">
         <v>140</v>
       </c>
-      <c r="E26" s="161"/>
+      <c r="E26" s="162"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="158" t="s">
+      <c r="B27" s="163" t="s">
         <v>138</v>
       </c>
-      <c r="C27" s="159" t="s">
+      <c r="C27" s="164" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="16" t="s">
@@ -40690,8 +40696,8 @@
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="158"/>
-      <c r="C28" s="159"/>
+      <c r="B28" s="163"/>
+      <c r="C28" s="164"/>
       <c r="D28" s="16" t="s">
         <v>64</v>
       </c>
@@ -40700,16 +40706,16 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="158"/>
-      <c r="C29" s="159"/>
+      <c r="B29" s="163"/>
+      <c r="C29" s="164"/>
       <c r="D29" s="16" t="s">
         <v>218</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="158"/>
-      <c r="C30" s="159"/>
+      <c r="B30" s="163"/>
+      <c r="C30" s="164"/>
       <c r="D30" s="16" t="s">
         <v>65</v>
       </c>
@@ -40718,20 +40724,20 @@
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="154" t="s">
+      <c r="B32" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="154" t="s">
+      <c r="C32" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="156" t="s">
+      <c r="D32" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="157"/>
+      <c r="E32" s="160"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="155"/>
-      <c r="C33" s="155"/>
+      <c r="B33" s="158"/>
+      <c r="C33" s="158"/>
       <c r="D33" s="17" t="s">
         <v>54</v>
       </c>
@@ -40746,16 +40752,16 @@
       <c r="C34" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D34" s="160" t="s">
+      <c r="D34" s="161" t="s">
         <v>130</v>
       </c>
-      <c r="E34" s="161"/>
+      <c r="E34" s="162"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="158" t="s">
+      <c r="B35" s="163" t="s">
         <v>128</v>
       </c>
-      <c r="C35" s="159" t="s">
+      <c r="C35" s="164" t="s">
         <v>53</v>
       </c>
       <c r="D35" s="16" t="s">
@@ -40766,8 +40772,8 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="158"/>
-      <c r="C36" s="159"/>
+      <c r="B36" s="163"/>
+      <c r="C36" s="164"/>
       <c r="D36" s="16" t="s">
         <v>58</v>
       </c>
@@ -40776,8 +40782,8 @@
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="158"/>
-      <c r="C37" s="159"/>
+      <c r="B37" s="163"/>
+      <c r="C37" s="164"/>
       <c r="D37" s="16" t="s">
         <v>175</v>
       </c>
@@ -40786,8 +40792,8 @@
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="158"/>
-      <c r="C38" s="159"/>
+      <c r="B38" s="163"/>
+      <c r="C38" s="164"/>
       <c r="D38" s="16" t="s">
         <v>131</v>
       </c>
@@ -40797,18 +40803,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D26:E26"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -40822,6 +40816,18 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="C7:C12"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40850,21 +40856,21 @@
   <sheetData>
     <row r="4" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="154" t="s">
+      <c r="B4" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="154" t="s">
+      <c r="C4" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="156" t="s">
+      <c r="D4" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="157"/>
+      <c r="E4" s="160"/>
     </row>
     <row r="5" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="155"/>
-      <c r="C5" s="155"/>
+      <c r="B5" s="158"/>
+      <c r="C5" s="158"/>
       <c r="D5" s="17" t="s">
         <v>54</v>
       </c>
@@ -40874,10 +40880,10 @@
     </row>
     <row r="6" spans="1:5" s="5" customFormat="1" ht="23.25" customHeight="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="162" t="s">
+      <c r="B6" s="166" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="165" t="s">
+      <c r="C6" s="169" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="16" t="s">
@@ -40889,8 +40895,8 @@
     </row>
     <row r="7" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="163"/>
-      <c r="C7" s="166"/>
+      <c r="B7" s="167"/>
+      <c r="C7" s="170"/>
       <c r="D7" s="16" t="s">
         <v>61</v>
       </c>
@@ -40900,8 +40906,8 @@
     </row>
     <row r="8" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="163"/>
-      <c r="C8" s="166"/>
+      <c r="B8" s="167"/>
+      <c r="C8" s="170"/>
       <c r="D8" s="16" t="s">
         <v>60</v>
       </c>
@@ -40911,8 +40917,8 @@
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="163"/>
-      <c r="C9" s="166"/>
+      <c r="B9" s="167"/>
+      <c r="C9" s="170"/>
       <c r="D9" s="16" t="s">
         <v>214</v>
       </c>
@@ -40920,8 +40926,8 @@
     </row>
     <row r="10" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="163"/>
-      <c r="C10" s="166"/>
+      <c r="B10" s="167"/>
+      <c r="C10" s="170"/>
       <c r="D10" s="16" t="s">
         <v>215</v>
       </c>
@@ -40929,8 +40935,8 @@
     </row>
     <row r="11" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="164"/>
-      <c r="C11" s="167"/>
+      <c r="B11" s="168"/>
+      <c r="C11" s="171"/>
       <c r="D11" s="16" t="s">
         <v>217</v>
       </c>
@@ -41022,20 +41028,20 @@
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" ht="23.25">
-      <c r="B25" s="154" t="s">
+      <c r="B25" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="154" t="s">
+      <c r="C25" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="156" t="s">
+      <c r="D25" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="157"/>
+      <c r="E25" s="160"/>
     </row>
     <row r="26" spans="1:5" ht="23.25">
-      <c r="B26" s="155"/>
-      <c r="C26" s="155"/>
+      <c r="B26" s="158"/>
+      <c r="C26" s="158"/>
       <c r="D26" s="17" t="s">
         <v>54</v>
       </c>
@@ -41050,16 +41056,16 @@
       <c r="C27" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="160" t="s">
+      <c r="D27" s="161" t="s">
         <v>134</v>
       </c>
-      <c r="E27" s="161"/>
+      <c r="E27" s="162"/>
     </row>
     <row r="28" spans="1:5" ht="23.25" customHeight="1">
-      <c r="B28" s="158" t="s">
+      <c r="B28" s="163" t="s">
         <v>132</v>
       </c>
-      <c r="C28" s="159" t="s">
+      <c r="C28" s="164" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="16" t="s">
@@ -41068,24 +41074,24 @@
       <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:5" ht="23.25">
-      <c r="B29" s="158"/>
-      <c r="C29" s="159"/>
+      <c r="B29" s="163"/>
+      <c r="C29" s="164"/>
       <c r="D29" s="16" t="s">
         <v>58</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:5" ht="23.25">
-      <c r="B30" s="158"/>
-      <c r="C30" s="159"/>
+      <c r="B30" s="163"/>
+      <c r="C30" s="164"/>
       <c r="D30" s="16" t="s">
         <v>59</v>
       </c>
       <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5" ht="23.25">
-      <c r="B31" s="158"/>
-      <c r="C31" s="159"/>
+      <c r="B31" s="163"/>
+      <c r="C31" s="164"/>
       <c r="D31" s="16" t="s">
         <v>215</v>
       </c>
@@ -41093,17 +41099,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="B6:B11"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="C28:C31"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B6:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -41118,8 +41124,8 @@
   </sheetPr>
   <dimension ref="A1:Z235"/>
   <sheetViews>
-    <sheetView topLeftCell="B162" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y7" sqref="Y7"/>
+    <sheetView topLeftCell="B144" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R233" sqref="R233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -41140,46 +41146,46 @@
     </row>
     <row r="3" spans="1:26">
       <c r="S3" s="67"/>
-      <c r="T3" s="170" t="s">
+      <c r="T3" s="174" t="s">
         <v>81</v>
       </c>
-      <c r="U3" s="170"/>
-      <c r="V3" s="170"/>
-      <c r="W3" s="170"/>
-      <c r="X3" s="170"/>
-      <c r="Y3" s="170"/>
+      <c r="U3" s="174"/>
+      <c r="V3" s="174"/>
+      <c r="W3" s="174"/>
+      <c r="X3" s="174"/>
+      <c r="Y3" s="174"/>
       <c r="Z3" s="68"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="171">
+      <c r="A4" s="175">
         <v>1</v>
       </c>
       <c r="S4" s="67"/>
-      <c r="T4" s="170"/>
-      <c r="U4" s="170"/>
-      <c r="V4" s="170"/>
-      <c r="W4" s="170"/>
-      <c r="X4" s="170"/>
-      <c r="Y4" s="170"/>
+      <c r="T4" s="174"/>
+      <c r="U4" s="174"/>
+      <c r="V4" s="174"/>
+      <c r="W4" s="174"/>
+      <c r="X4" s="174"/>
+      <c r="Y4" s="174"/>
       <c r="Z4" s="68"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="171"/>
+      <c r="A5" s="175"/>
       <c r="S5" s="67"/>
-      <c r="T5" s="168" t="s">
+      <c r="T5" s="172" t="s">
         <v>84</v>
       </c>
-      <c r="U5" s="168"/>
-      <c r="V5" s="168"/>
-      <c r="W5" s="169" t="s">
+      <c r="U5" s="172"/>
+      <c r="V5" s="172"/>
+      <c r="W5" s="173" t="s">
         <v>83</v>
       </c>
-      <c r="X5" s="168"/>
-      <c r="Y5" s="168"/>
+      <c r="X5" s="172"/>
+      <c r="Y5" s="172"/>
       <c r="Z5" s="68"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="171"/>
+      <c r="A6" s="175"/>
       <c r="S6" s="67"/>
       <c r="V6" t="s">
         <v>80</v>
@@ -41188,7 +41194,7 @@
       <c r="Z6" s="68"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="171"/>
+      <c r="A7" s="175"/>
       <c r="S7" s="67"/>
       <c r="W7" s="15"/>
       <c r="Y7" t="s">
@@ -41197,13 +41203,13 @@
       <c r="Z7" s="68"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="171"/>
+      <c r="A8" s="175"/>
       <c r="S8" s="67"/>
       <c r="W8" s="15"/>
       <c r="Z8" s="68"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="171"/>
+      <c r="A9" s="175"/>
       <c r="S9" s="67"/>
       <c r="V9" t="s">
         <v>82</v>
@@ -41212,13 +41218,13 @@
       <c r="Z9" s="68"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="171"/>
+      <c r="A10" s="175"/>
       <c r="S10" s="67"/>
       <c r="W10" s="15"/>
       <c r="Z10" s="68"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="171"/>
+      <c r="A11" s="175"/>
       <c r="S11" s="67"/>
       <c r="W11" s="15"/>
       <c r="Z11" s="68"/>
@@ -41304,186 +41310,186 @@
       <c r="Z25" s="71"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="171">
+      <c r="A36" s="175">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="171"/>
+      <c r="A37" s="175"/>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="171"/>
+      <c r="A38" s="175"/>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="171"/>
+      <c r="A39" s="175"/>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="171"/>
+      <c r="A40" s="175"/>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="171"/>
+      <c r="A41" s="175"/>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="171"/>
+      <c r="A42" s="175"/>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="171"/>
+      <c r="A43" s="175"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="171">
+      <c r="A68" s="175">
         <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="171"/>
+      <c r="A69" s="175"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="171"/>
+      <c r="A70" s="175"/>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="171"/>
+      <c r="A71" s="175"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="171"/>
+      <c r="A72" s="175"/>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="171"/>
+      <c r="A73" s="175"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="171"/>
+      <c r="A74" s="175"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="171"/>
+      <c r="A75" s="175"/>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="171">
+      <c r="A100" s="175">
         <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="171"/>
+      <c r="A101" s="175"/>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="171"/>
+      <c r="A102" s="175"/>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="171"/>
+      <c r="A103" s="175"/>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="171"/>
+      <c r="A104" s="175"/>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="171"/>
+      <c r="A105" s="175"/>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="171"/>
+      <c r="A106" s="175"/>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="171"/>
+      <c r="A107" s="175"/>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="171">
+      <c r="A132" s="175">
         <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:1">
-      <c r="A133" s="171"/>
+      <c r="A133" s="175"/>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="171"/>
+      <c r="A134" s="175"/>
     </row>
     <row r="135" spans="1:1">
-      <c r="A135" s="171"/>
+      <c r="A135" s="175"/>
     </row>
     <row r="136" spans="1:1">
-      <c r="A136" s="171"/>
+      <c r="A136" s="175"/>
     </row>
     <row r="137" spans="1:1">
-      <c r="A137" s="171"/>
+      <c r="A137" s="175"/>
     </row>
     <row r="138" spans="1:1">
-      <c r="A138" s="171"/>
+      <c r="A138" s="175"/>
     </row>
     <row r="139" spans="1:1">
-      <c r="A139" s="171"/>
+      <c r="A139" s="175"/>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="171">
+      <c r="A164" s="175">
         <v>6</v>
       </c>
     </row>
     <row r="165" spans="1:1">
-      <c r="A165" s="171"/>
+      <c r="A165" s="175"/>
     </row>
     <row r="166" spans="1:1">
-      <c r="A166" s="171"/>
+      <c r="A166" s="175"/>
     </row>
     <row r="167" spans="1:1">
-      <c r="A167" s="171"/>
+      <c r="A167" s="175"/>
     </row>
     <row r="168" spans="1:1">
-      <c r="A168" s="171"/>
+      <c r="A168" s="175"/>
     </row>
     <row r="169" spans="1:1">
-      <c r="A169" s="171"/>
+      <c r="A169" s="175"/>
     </row>
     <row r="170" spans="1:1">
-      <c r="A170" s="171"/>
+      <c r="A170" s="175"/>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" s="171"/>
+      <c r="A171" s="175"/>
     </row>
     <row r="196" spans="1:1">
-      <c r="A196" s="171">
+      <c r="A196" s="175">
         <v>7</v>
       </c>
     </row>
     <row r="197" spans="1:1">
-      <c r="A197" s="171"/>
+      <c r="A197" s="175"/>
     </row>
     <row r="198" spans="1:1">
-      <c r="A198" s="171"/>
+      <c r="A198" s="175"/>
     </row>
     <row r="199" spans="1:1">
-      <c r="A199" s="171"/>
+      <c r="A199" s="175"/>
     </row>
     <row r="200" spans="1:1">
-      <c r="A200" s="171"/>
+      <c r="A200" s="175"/>
     </row>
     <row r="201" spans="1:1">
-      <c r="A201" s="171"/>
+      <c r="A201" s="175"/>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" s="171"/>
+      <c r="A202" s="175"/>
     </row>
     <row r="203" spans="1:1">
-      <c r="A203" s="171"/>
+      <c r="A203" s="175"/>
     </row>
     <row r="228" spans="1:1">
-      <c r="A228" s="171">
+      <c r="A228" s="175">
         <v>8</v>
       </c>
     </row>
     <row r="229" spans="1:1">
-      <c r="A229" s="171"/>
+      <c r="A229" s="175"/>
     </row>
     <row r="230" spans="1:1">
-      <c r="A230" s="171"/>
+      <c r="A230" s="175"/>
     </row>
     <row r="231" spans="1:1">
-      <c r="A231" s="171"/>
+      <c r="A231" s="175"/>
     </row>
     <row r="232" spans="1:1">
-      <c r="A232" s="171"/>
+      <c r="A232" s="175"/>
     </row>
     <row r="233" spans="1:1">
-      <c r="A233" s="171"/>
+      <c r="A233" s="175"/>
     </row>
     <row r="234" spans="1:1">
-      <c r="A234" s="171"/>
+      <c r="A234" s="175"/>
     </row>
     <row r="235" spans="1:1">
-      <c r="A235" s="171"/>
+      <c r="A235" s="175"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -41530,38 +41536,38 @@
   </cols>
   <sheetData>
     <row r="70" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="C70" s="172" t="s">
+      <c r="C70" s="176" t="s">
         <v>184</v>
       </c>
-      <c r="D70" s="172" t="s">
+      <c r="D70" s="176" t="s">
         <v>169</v>
       </c>
-      <c r="E70" s="172" t="s">
+      <c r="E70" s="176" t="s">
         <v>168</v>
       </c>
-      <c r="F70" s="175" t="s">
+      <c r="F70" s="179" t="s">
         <v>174</v>
       </c>
-      <c r="G70" s="172" t="s">
+      <c r="G70" s="176" t="s">
         <v>167</v>
       </c>
-      <c r="H70" s="172" t="s">
+      <c r="H70" s="176" t="s">
         <v>173</v>
       </c>
-      <c r="I70" s="172"/>
-      <c r="J70" s="172" t="s">
+      <c r="I70" s="176"/>
+      <c r="J70" s="176" t="s">
         <v>3</v>
       </c>
-      <c r="K70" s="172"/>
-      <c r="L70" s="172"/>
-      <c r="M70" s="172"/>
+      <c r="K70" s="176"/>
+      <c r="L70" s="176"/>
+      <c r="M70" s="176"/>
     </row>
     <row r="71" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="C71" s="172"/>
-      <c r="D71" s="172"/>
-      <c r="E71" s="172"/>
-      <c r="F71" s="172"/>
-      <c r="G71" s="172"/>
+      <c r="C71" s="176"/>
+      <c r="D71" s="176"/>
+      <c r="E71" s="176"/>
+      <c r="F71" s="176"/>
+      <c r="G71" s="176"/>
       <c r="H71" s="75" t="s">
         <v>172</v>
       </c>
@@ -41582,10 +41588,10 @@
       </c>
     </row>
     <row r="72" spans="3:13" s="2" customFormat="1" ht="151.5" customHeight="1">
-      <c r="C72" s="173" t="s">
+      <c r="C72" s="177" t="s">
         <v>200</v>
       </c>
-      <c r="D72" s="174"/>
+      <c r="D72" s="178"/>
       <c r="E72" s="77"/>
       <c r="F72" s="78"/>
       <c r="G72" s="78"/>

</xml_diff>

<commit_message>
I improved and synchronized between the external DB <Firebase> and the app store <Redux>, I checked all cases of adding, updating and deleting data, including unusual cases
</commit_message>
<xml_diff>
--- a/Final-React-Project-Design.xlsx
+++ b/Final-React-Project-Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basheer\Desktop\בשיר\Full Stack Work\Full Stack Cors - YanivArad\Projects\React-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEC5E39-A5E3-4FC7-A302-2B95C36CF47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88373DD-A9E9-4689-A63A-1C157CB89B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="970" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan Work" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Actions" sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Plan Work'!$A$7:$F$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Plan Work'!$A$5:$F$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="247">
   <si>
     <t>Num</t>
   </si>
@@ -4021,29 +4021,6 @@
     <t>authenticate the app with firebase authetication</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Step 10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Users collection</t>
-    </r>
-  </si>
-  <si>
     <t>Perform tests for the application</t>
   </si>
   <si>
@@ -5004,52 +4981,6 @@
     <t>18/11/23</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Step 11</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Tests</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Step 10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - optimization</t>
-    </r>
-  </si>
-  <si>
     <t>Improving the efficiency of the application</t>
   </si>
   <si>
@@ -5304,14 +5235,154 @@
     <t>28-29/11/23</t>
   </si>
   <si>
-    <t>30/11/23</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - improve and sync store data</t>
+    </r>
+  </si>
+  <si>
+    <t>Improve and Sync between the external DB [Firebase] and the internal DB [redux]</t>
+  </si>
+  <si>
+    <t>29/11/23-5/12/23</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Users collection</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - optimization</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Tests</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Build dashboard page - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Optionally</t>
+    </r>
+  </si>
+  <si>
+    <t>I will add a dashboard page that gives the possibility to manage the necessary data</t>
+  </si>
+  <si>
+    <t>5-7/12/2023</t>
+  </si>
+  <si>
+    <t>8-9/12/2023</t>
+  </si>
+  <si>
+    <t>10-11/12/2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="64">
+  <fonts count="65">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5733,6 +5804,13 @@
       <color rgb="FF6F42C1"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -6358,7 +6436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -6559,9 +6637,6 @@
     <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6607,9 +6682,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6668,95 +6740,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6785,7 +6776,16 @@
     <xf numFmtId="0" fontId="47" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6800,11 +6800,86 @@
     <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6818,19 +6893,16 @@
     <xf numFmtId="0" fontId="25" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6873,6 +6945,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -39176,19 +39251,19 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="B3:F33"/>
+  <dimension ref="B1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="45" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="45" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" style="45" customWidth="1"/>
+    <col min="3" max="3" width="69.85546875" style="45" customWidth="1"/>
     <col min="4" max="4" width="61.85546875" style="45" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="45" customWidth="1"/>
+    <col min="5" max="5" width="21" style="45" customWidth="1"/>
     <col min="6" max="6" width="19.140625" style="45" customWidth="1"/>
     <col min="7" max="7" width="36.140625" style="45" customWidth="1"/>
     <col min="8" max="8" width="15" style="45"/>
@@ -39196,56 +39271,90 @@
     <col min="10" max="16384" width="15" style="45"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6">
-      <c r="B3" s="109" t="s">
+    <row r="1" spans="2:6">
+      <c r="B1" s="107" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="109"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="109"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="110" t="s">
+      <c r="B4" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="110" t="s">
+      <c r="C4" s="108" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="110" t="s">
+      <c r="D4" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="110" t="s">
+      <c r="E4" s="108" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="110" t="s">
+      <c r="F4" s="108" t="s">
         <v>123</v>
       </c>
     </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="46">
+        <v>1</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="110"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
+      <c r="B7" s="46">
+        <v>1</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
-      <c r="C8" s="46" t="s">
-        <v>74</v>
+      <c r="C8" s="105" t="s">
+        <v>68</v>
       </c>
-      <c r="D8" s="46"/>
+      <c r="D8" s="47" t="s">
+        <v>71</v>
+      </c>
       <c r="E8" s="46" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>124</v>
@@ -39253,33 +39362,31 @@
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="46">
-        <v>1</v>
+        <v>3</v>
       </c>
-      <c r="C9" s="46" t="s">
-        <v>72</v>
-      </c>
+      <c r="C9" s="106"/>
       <c r="D9" s="46" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="48" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="46">
-        <v>2</v>
+        <v>4</v>
       </c>
-      <c r="C10" s="107" t="s">
-        <v>68</v>
+      <c r="C10" s="46" t="s">
+        <v>76</v>
       </c>
-      <c r="D10" s="47" t="s">
-        <v>71</v>
+      <c r="D10" s="46" t="s">
+        <v>146</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>127</v>
+        <v>218</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>124</v>
@@ -39287,31 +39394,33 @@
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="46">
-        <v>3</v>
+        <v>5</v>
       </c>
-      <c r="C11" s="108"/>
+      <c r="C11" s="46" t="s">
+        <v>147</v>
+      </c>
       <c r="D11" s="46" t="s">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>127</v>
+        <v>221</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="F11" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="46">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>76</v>
+        <v>148</v>
       </c>
       <c r="D12" s="46" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>124</v>
@@ -39319,16 +39428,16 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="46">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D13" s="46" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>124</v>
@@ -39336,16 +39445,16 @@
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="46">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D14" s="46" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>124</v>
@@ -39353,16 +39462,16 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="46">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="D15" s="46" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>124</v>
@@ -39370,16 +39479,16 @@
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="46">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D16" s="46" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>124</v>
@@ -39387,16 +39496,16 @@
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="46">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D17" s="46" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>124</v>
@@ -39404,194 +39513,154 @@
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="46">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D18" s="46" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" ht="30">
       <c r="B19" s="46">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" ht="30">
       <c r="B20" s="46">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>157</v>
+        <v>236</v>
       </c>
       <c r="D20" s="46" t="s">
-        <v>154</v>
+        <v>237</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="30">
+    <row r="21" spans="2:6">
       <c r="B21" s="46">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>156</v>
+        <v>239</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
-      <c r="E21" s="46" t="s">
-        <v>238</v>
+      <c r="E21" s="104" t="s">
+        <v>244</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>124</v>
-      </c>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" s="46">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>162</v>
+        <v>240</v>
       </c>
-      <c r="D22" s="74" t="s">
-        <v>161</v>
+      <c r="D22" s="46" t="s">
+        <v>219</v>
       </c>
-      <c r="E22" s="46" t="s">
-        <v>239</v>
+      <c r="E22" s="104" t="s">
+        <v>245</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>124</v>
-      </c>
+      <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" ht="30">
       <c r="B23" s="46">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C23" s="46" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>222</v>
+        <v>243</v>
       </c>
-      <c r="E23" s="106">
-        <v>44938</v>
+      <c r="E23" s="104" t="s">
+        <v>246</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" s="46">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C24" s="46" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
       <c r="D24" s="46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
-      <c r="E24" s="106">
-        <v>44938</v>
+      <c r="E24" s="104">
+        <v>45272</v>
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="46">
-        <v>17</v>
+    <row r="25" spans="2:6" ht="37.5">
+      <c r="C25" s="89" t="s">
+        <v>200</v>
       </c>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="1"/>
+      <c r="D25" s="178" t="s">
+        <v>201</v>
+      </c>
     </row>
-    <row r="26" spans="2:6">
-      <c r="B26" s="46">
-        <v>18</v>
+    <row r="27" spans="2:6" ht="37.5">
+      <c r="C27" s="89" t="s">
+        <v>202</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="46">
-        <v>19</v>
+      <c r="D27" s="178" t="s">
+        <v>203</v>
       </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="B28" s="46">
-        <v>20</v>
-      </c>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="2:6" ht="37.5">
-      <c r="C29" s="90" t="s">
-        <v>201</v>
-      </c>
-      <c r="D29" s="91" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="37.5">
-      <c r="C31" s="90" t="s">
-        <v>203</v>
-      </c>
-      <c r="D31" s="91" t="s">
+      <c r="D29" s="178" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" ht="37.5">
-      <c r="D33" s="91" t="s">
-        <v>205</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B3:F4"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
-  <conditionalFormatting sqref="F8:F28">
+  <conditionalFormatting sqref="F6:F24">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="V">
-      <formula>NOT(ISERROR(SEARCH("V",F8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("V",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C29" r:id="rId1" xr:uid="{B5AF2755-436A-4008-9BA4-CBBB84CC1736}"/>
-    <hyperlink ref="C31" r:id="rId2" xr:uid="{3D76CBC8-DA15-470A-8E1E-DBBC4061AE14}"/>
+    <hyperlink ref="C25" r:id="rId1" xr:uid="{B5AF2755-436A-4008-9BA4-CBBB84CC1736}"/>
+    <hyperlink ref="C27" r:id="rId2" xr:uid="{3D76CBC8-DA15-470A-8E1E-DBBC4061AE14}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
@@ -39617,40 +39686,40 @@
     <col min="3" max="3" width="25.85546875" style="6" customWidth="1"/>
     <col min="4" max="5" width="46.28515625" style="6" customWidth="1"/>
     <col min="6" max="6" width="178.140625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="67.85546875" style="94" customWidth="1"/>
+    <col min="7" max="7" width="67.85546875" style="92" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="51.75" customHeight="1">
-      <c r="B2" s="139" t="s">
+      <c r="B2" s="109" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" thickBot="1">
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="119" t="s">
+      <c r="C4" s="148" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="148" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="119" t="s">
+      <c r="E4" s="148" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="134"/>
+      <c r="F4" s="149"/>
     </row>
     <row r="5" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B5" s="127"/>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="151"/>
+      <c r="D5" s="151"/>
       <c r="E5" s="31" t="s">
         <v>9</v>
       </c>
@@ -39659,10 +39728,10 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B6" s="143">
+      <c r="B6" s="114">
         <v>1</v>
       </c>
-      <c r="C6" s="122" t="s">
+      <c r="C6" s="111" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="73" t="s">
@@ -39671,68 +39740,68 @@
       <c r="E6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="100" t="s">
+      <c r="F6" s="98" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B7" s="144"/>
-      <c r="C7" s="141"/>
-      <c r="D7" s="113" t="s">
+      <c r="B7" s="115"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="124" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" s="123" t="s">
+        <v>227</v>
+      </c>
+      <c r="F7" s="99" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B8" s="115"/>
+      <c r="C8" s="112"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="99" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B9" s="115"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="99" t="s">
         <v>225</v>
       </c>
-      <c r="E7" s="136" t="s">
-        <v>230</v>
-      </c>
-      <c r="F7" s="101" t="s">
+    </row>
+    <row r="10" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B10" s="115"/>
+      <c r="C10" s="112"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="100"/>
+    </row>
+    <row r="11" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
+      <c r="B11" s="133"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="134"/>
+      <c r="E11" s="152"/>
+      <c r="F11" s="101" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B8" s="144"/>
-      <c r="C8" s="141"/>
-      <c r="D8" s="151"/>
-      <c r="E8" s="137"/>
-      <c r="F8" s="101" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B9" s="144"/>
-      <c r="C9" s="141"/>
-      <c r="D9" s="151"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="101" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B10" s="144"/>
-      <c r="C10" s="141"/>
-      <c r="D10" s="151"/>
-      <c r="E10" s="137"/>
-      <c r="F10" s="102"/>
-    </row>
-    <row r="11" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B11" s="156"/>
-      <c r="C11" s="123"/>
-      <c r="D11" s="125"/>
-      <c r="E11" s="138"/>
-      <c r="F11" s="103" t="s">
-        <v>229</v>
-      </c>
-    </row>
     <row r="12" spans="2:6" ht="22.5">
-      <c r="B12" s="130">
+      <c r="B12" s="129">
         <v>2</v>
       </c>
-      <c r="C12" s="114" t="s">
+      <c r="C12" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="111" t="s">
+      <c r="D12" s="145" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="117" t="s">
+      <c r="E12" s="142" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="38" t="s">
@@ -39740,63 +39809,63 @@
       </c>
     </row>
     <row r="13" spans="2:6" ht="22.5">
-      <c r="B13" s="131"/>
-      <c r="C13" s="115"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="118"/>
+      <c r="B13" s="130"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="146"/>
+      <c r="E13" s="143"/>
       <c r="F13" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="22.5">
-      <c r="B14" s="131"/>
-      <c r="C14" s="115"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="118"/>
+      <c r="B14" s="130"/>
+      <c r="C14" s="138"/>
+      <c r="D14" s="146"/>
+      <c r="E14" s="143"/>
       <c r="F14" s="21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="22.5">
-      <c r="B15" s="131"/>
-      <c r="C15" s="115"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="118"/>
+      <c r="B15" s="130"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="146"/>
+      <c r="E15" s="143"/>
       <c r="F15" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="22.5">
-      <c r="B16" s="131"/>
-      <c r="C16" s="115"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="118"/>
+      <c r="B16" s="130"/>
+      <c r="C16" s="138"/>
+      <c r="D16" s="146"/>
+      <c r="E16" s="143"/>
       <c r="F16" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="22.5">
-      <c r="B17" s="131"/>
-      <c r="C17" s="115"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="118"/>
+      <c r="B17" s="130"/>
+      <c r="C17" s="138"/>
+      <c r="D17" s="146"/>
+      <c r="E17" s="143"/>
       <c r="F17" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="22.5">
-      <c r="B18" s="131"/>
-      <c r="C18" s="115"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="118"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="146"/>
+      <c r="E18" s="143"/>
       <c r="F18" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B19" s="132"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="133"/>
+      <c r="B19" s="144"/>
+      <c r="C19" s="139"/>
+      <c r="D19" s="147"/>
       <c r="E19" s="40" t="s">
         <v>13</v>
       </c>
@@ -39805,16 +39874,16 @@
       </c>
     </row>
     <row r="20" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B20" s="130">
+      <c r="B20" s="129">
         <v>3</v>
       </c>
-      <c r="C20" s="114" t="s">
+      <c r="C20" s="137" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="111" t="s">
+      <c r="D20" s="145" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="117" t="s">
+      <c r="E20" s="142" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="41" t="s">
@@ -39822,45 +39891,45 @@
       </c>
     </row>
     <row r="21" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B21" s="131"/>
-      <c r="C21" s="115"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="118"/>
+      <c r="B21" s="130"/>
+      <c r="C21" s="138"/>
+      <c r="D21" s="146"/>
+      <c r="E21" s="143"/>
       <c r="F21" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B22" s="131"/>
-      <c r="C22" s="115"/>
-      <c r="D22" s="112"/>
-      <c r="E22" s="118"/>
+      <c r="B22" s="130"/>
+      <c r="C22" s="138"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="143"/>
       <c r="F22" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B23" s="131"/>
-      <c r="C23" s="115"/>
-      <c r="D23" s="112"/>
-      <c r="E23" s="118"/>
+      <c r="B23" s="130"/>
+      <c r="C23" s="138"/>
+      <c r="D23" s="146"/>
+      <c r="E23" s="143"/>
       <c r="F23" s="26" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B24" s="131"/>
-      <c r="C24" s="115"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="118"/>
+      <c r="B24" s="130"/>
+      <c r="C24" s="138"/>
+      <c r="D24" s="146"/>
+      <c r="E24" s="143"/>
       <c r="F24" s="27" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B25" s="132"/>
-      <c r="C25" s="116"/>
-      <c r="D25" s="133"/>
+      <c r="B25" s="144"/>
+      <c r="C25" s="139"/>
+      <c r="D25" s="147"/>
       <c r="E25" s="40" t="s">
         <v>13</v>
       </c>
@@ -39869,16 +39938,16 @@
       </c>
     </row>
     <row r="26" spans="2:6" ht="22.5">
-      <c r="B26" s="130">
+      <c r="B26" s="129">
         <v>4</v>
       </c>
-      <c r="C26" s="114" t="s">
+      <c r="C26" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="111" t="s">
+      <c r="D26" s="145" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="117" t="s">
+      <c r="E26" s="142" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="41" t="s">
@@ -39886,27 +39955,27 @@
       </c>
     </row>
     <row r="27" spans="2:6" ht="22.5">
-      <c r="B27" s="131"/>
-      <c r="C27" s="115"/>
-      <c r="D27" s="112"/>
-      <c r="E27" s="118"/>
+      <c r="B27" s="130"/>
+      <c r="C27" s="138"/>
+      <c r="D27" s="146"/>
+      <c r="E27" s="143"/>
       <c r="F27" s="28" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="22.5">
-      <c r="B28" s="131"/>
-      <c r="C28" s="115"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="118"/>
+      <c r="B28" s="130"/>
+      <c r="C28" s="138"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="143"/>
       <c r="F28" s="29" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="42" customHeight="1" thickBot="1">
-      <c r="B29" s="155"/>
-      <c r="C29" s="135"/>
-      <c r="D29" s="113"/>
+      <c r="B29" s="131"/>
+      <c r="C29" s="150"/>
+      <c r="D29" s="124"/>
       <c r="E29" s="12" t="s">
         <v>13</v>
       </c>
@@ -39932,16 +40001,16 @@
       </c>
     </row>
     <row r="31" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B31" s="130">
+      <c r="B31" s="129">
         <v>6</v>
       </c>
-      <c r="C31" s="114" t="s">
+      <c r="C31" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="128" t="s">
+      <c r="D31" s="140" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="117" t="s">
+      <c r="E31" s="142" t="s">
         <v>13</v>
       </c>
       <c r="F31" s="41" t="s">
@@ -39949,17 +40018,17 @@
       </c>
     </row>
     <row r="32" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B32" s="131"/>
-      <c r="C32" s="115"/>
-      <c r="D32" s="129"/>
-      <c r="E32" s="118"/>
+      <c r="B32" s="130"/>
+      <c r="C32" s="138"/>
+      <c r="D32" s="141"/>
+      <c r="E32" s="143"/>
       <c r="F32" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B33" s="132"/>
-      <c r="C33" s="116"/>
+      <c r="B33" s="144"/>
+      <c r="C33" s="139"/>
       <c r="D33" s="39" t="s">
         <v>39</v>
       </c>
@@ -40003,10 +40072,10 @@
       </c>
     </row>
     <row r="36" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B36" s="143">
+      <c r="B36" s="114">
         <v>9</v>
       </c>
-      <c r="C36" s="122" t="s">
+      <c r="C36" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D36" s="73" t="s">
@@ -40020,12 +40089,12 @@
       </c>
     </row>
     <row r="37" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B37" s="144"/>
-      <c r="C37" s="141"/>
-      <c r="D37" s="113" t="s">
+      <c r="B37" s="115"/>
+      <c r="C37" s="112"/>
+      <c r="D37" s="124" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="136" t="s">
+      <c r="E37" s="123" t="s">
         <v>96</v>
       </c>
       <c r="F37" s="55" t="s">
@@ -40033,37 +40102,37 @@
       </c>
     </row>
     <row r="38" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B38" s="144"/>
-      <c r="C38" s="141"/>
-      <c r="D38" s="151"/>
-      <c r="E38" s="137"/>
+      <c r="B38" s="115"/>
+      <c r="C38" s="112"/>
+      <c r="D38" s="125"/>
+      <c r="E38" s="121"/>
       <c r="F38" s="51" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B39" s="144"/>
-      <c r="C39" s="141"/>
-      <c r="D39" s="151"/>
-      <c r="E39" s="137"/>
+      <c r="B39" s="115"/>
+      <c r="C39" s="112"/>
+      <c r="D39" s="125"/>
+      <c r="E39" s="121"/>
       <c r="F39" s="51" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B40" s="144"/>
-      <c r="C40" s="141"/>
-      <c r="D40" s="151"/>
-      <c r="E40" s="150"/>
+      <c r="B40" s="115"/>
+      <c r="C40" s="112"/>
+      <c r="D40" s="125"/>
+      <c r="E40" s="122"/>
       <c r="F40" s="56" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B41" s="144"/>
-      <c r="C41" s="141"/>
-      <c r="D41" s="151"/>
-      <c r="E41" s="136" t="s">
+      <c r="B41" s="115"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="125"/>
+      <c r="E41" s="123" t="s">
         <v>98</v>
       </c>
       <c r="F41" s="57" t="s">
@@ -40071,54 +40140,54 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B42" s="144"/>
-      <c r="C42" s="141"/>
-      <c r="D42" s="151"/>
-      <c r="E42" s="137"/>
+      <c r="B42" s="115"/>
+      <c r="C42" s="112"/>
+      <c r="D42" s="125"/>
+      <c r="E42" s="121"/>
       <c r="F42" s="58" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B43" s="144"/>
-      <c r="C43" s="141"/>
-      <c r="D43" s="151"/>
-      <c r="E43" s="137"/>
+      <c r="B43" s="115"/>
+      <c r="C43" s="112"/>
+      <c r="D43" s="125"/>
+      <c r="E43" s="121"/>
       <c r="F43" s="58" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B44" s="144"/>
-      <c r="C44" s="141"/>
-      <c r="D44" s="151"/>
-      <c r="E44" s="137"/>
+      <c r="B44" s="115"/>
+      <c r="C44" s="112"/>
+      <c r="D44" s="125"/>
+      <c r="E44" s="121"/>
       <c r="F44" s="59" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B45" s="144"/>
-      <c r="C45" s="141"/>
-      <c r="D45" s="151"/>
-      <c r="E45" s="137"/>
+      <c r="B45" s="115"/>
+      <c r="C45" s="112"/>
+      <c r="D45" s="125"/>
+      <c r="E45" s="121"/>
       <c r="F45" s="59" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B46" s="144"/>
-      <c r="C46" s="141"/>
-      <c r="D46" s="152"/>
-      <c r="E46" s="150"/>
+      <c r="B46" s="115"/>
+      <c r="C46" s="112"/>
+      <c r="D46" s="126"/>
+      <c r="E46" s="122"/>
       <c r="F46" s="60" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="75">
-      <c r="B47" s="144"/>
-      <c r="C47" s="141"/>
-      <c r="D47" s="113" t="s">
+      <c r="B47" s="115"/>
+      <c r="C47" s="112"/>
+      <c r="D47" s="124" t="s">
         <v>97</v>
       </c>
       <c r="E47" s="10" t="s">
@@ -40129,10 +40198,10 @@
       </c>
     </row>
     <row r="48" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B48" s="144"/>
-      <c r="C48" s="141"/>
-      <c r="D48" s="151"/>
-      <c r="E48" s="153" t="s">
+      <c r="B48" s="115"/>
+      <c r="C48" s="112"/>
+      <c r="D48" s="125"/>
+      <c r="E48" s="127" t="s">
         <v>109</v>
       </c>
       <c r="F48" s="58" t="s">
@@ -40140,54 +40209,54 @@
       </c>
     </row>
     <row r="49" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B49" s="144"/>
-      <c r="C49" s="141"/>
-      <c r="D49" s="151"/>
-      <c r="E49" s="153"/>
+      <c r="B49" s="115"/>
+      <c r="C49" s="112"/>
+      <c r="D49" s="125"/>
+      <c r="E49" s="127"/>
       <c r="F49" s="59" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B50" s="144"/>
-      <c r="C50" s="141"/>
-      <c r="D50" s="151"/>
-      <c r="E50" s="153"/>
+      <c r="B50" s="115"/>
+      <c r="C50" s="112"/>
+      <c r="D50" s="125"/>
+      <c r="E50" s="127"/>
       <c r="F50" s="59" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B51" s="145"/>
-      <c r="C51" s="142"/>
-      <c r="D51" s="152"/>
-      <c r="E51" s="154"/>
+      <c r="B51" s="116"/>
+      <c r="C51" s="113"/>
+      <c r="D51" s="126"/>
+      <c r="E51" s="128"/>
       <c r="F51" s="60" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="52" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B52" s="96"/>
-      <c r="C52" s="97"/>
-      <c r="D52" s="98" t="s">
-        <v>231</v>
+      <c r="B52" s="94"/>
+      <c r="C52" s="95"/>
+      <c r="D52" s="96" t="s">
+        <v>228</v>
       </c>
-      <c r="E52" s="104" t="s">
+      <c r="E52" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="105"/>
+      <c r="F52" s="103"/>
     </row>
     <row r="53" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B53" s="144">
+      <c r="B53" s="115">
         <v>10</v>
       </c>
-      <c r="C53" s="148" t="s">
+      <c r="C53" s="119" t="s">
         <v>117</v>
       </c>
-      <c r="D53" s="146" t="s">
+      <c r="D53" s="117" t="s">
         <v>126</v>
       </c>
-      <c r="E53" s="137" t="s">
+      <c r="E53" s="121" t="s">
         <v>118</v>
       </c>
       <c r="F53" s="62" t="s">
@@ -40195,122 +40264,122 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B54" s="144"/>
-      <c r="C54" s="148"/>
-      <c r="D54" s="146"/>
-      <c r="E54" s="137"/>
+      <c r="B54" s="115"/>
+      <c r="C54" s="119"/>
+      <c r="D54" s="117"/>
+      <c r="E54" s="121"/>
       <c r="F54" s="62" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B55" s="144"/>
-      <c r="C55" s="148"/>
-      <c r="D55" s="146"/>
-      <c r="E55" s="137"/>
+      <c r="B55" s="115"/>
+      <c r="C55" s="119"/>
+      <c r="D55" s="117"/>
+      <c r="E55" s="121"/>
       <c r="F55" s="63" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B56" s="144"/>
-      <c r="C56" s="148"/>
-      <c r="D56" s="146"/>
-      <c r="E56" s="137"/>
+      <c r="B56" s="115"/>
+      <c r="C56" s="119"/>
+      <c r="D56" s="117"/>
+      <c r="E56" s="121"/>
       <c r="F56" s="62" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="57" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B57" s="145"/>
-      <c r="C57" s="149"/>
-      <c r="D57" s="147"/>
-      <c r="E57" s="150"/>
+      <c r="B57" s="116"/>
+      <c r="C57" s="120"/>
+      <c r="D57" s="118"/>
+      <c r="E57" s="122"/>
       <c r="F57" s="62" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="58" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B58" s="33"/>
-      <c r="C58" s="122" t="s">
+      <c r="C58" s="111" t="s">
+        <v>205</v>
+      </c>
+      <c r="D58" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="D58" s="72" t="s">
-        <v>207</v>
-      </c>
       <c r="E58" s="36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F58" s="37" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
-      <c r="G58" s="121" t="s">
-        <v>213</v>
+      <c r="G58" s="153" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="59" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B59" s="33"/>
-      <c r="C59" s="123"/>
+      <c r="C59" s="132"/>
       <c r="D59" s="72" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E59" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="F59" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="F59" s="37" t="s">
-        <v>212</v>
-      </c>
-      <c r="G59" s="121"/>
+      <c r="G59" s="153"/>
     </row>
     <row r="60" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B60" s="96"/>
-      <c r="C60" s="97"/>
-      <c r="D60" s="98" t="s">
+      <c r="B60" s="94"/>
+      <c r="C60" s="95"/>
+      <c r="D60" s="96" t="s">
+        <v>229</v>
+      </c>
+      <c r="E60" s="97"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="91"/>
+    </row>
+    <row r="61" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B61" s="94"/>
+      <c r="C61" s="95" t="s">
         <v>232</v>
       </c>
-      <c r="E60" s="99"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="93"/>
+      <c r="D61" s="154" t="s">
+        <v>230</v>
+      </c>
+      <c r="E61" s="97"/>
+      <c r="F61" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="G61" s="91"/>
     </row>
-    <row r="61" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B61" s="96"/>
-      <c r="C61" s="97" t="s">
-        <v>235</v>
-      </c>
-      <c r="D61" s="124" t="s">
+    <row r="62" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B62" s="94"/>
+      <c r="C62" s="95"/>
+      <c r="D62" s="134"/>
+      <c r="E62" s="97"/>
+      <c r="F62" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="E61" s="99"/>
-      <c r="F61" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="G61" s="93"/>
-    </row>
-    <row r="62" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B62" s="96"/>
-      <c r="C62" s="97"/>
-      <c r="D62" s="125"/>
-      <c r="E62" s="99"/>
-      <c r="F62" s="14" t="s">
-        <v>236</v>
-      </c>
-      <c r="G62" s="93"/>
+      <c r="G62" s="91"/>
     </row>
     <row r="63" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B63" s="96"/>
-      <c r="C63" s="97"/>
-      <c r="D63" s="104"/>
-      <c r="E63" s="99"/>
+      <c r="B63" s="94"/>
+      <c r="C63" s="95"/>
+      <c r="D63" s="102"/>
+      <c r="E63" s="97"/>
       <c r="F63" s="14"/>
-      <c r="G63" s="93"/>
+      <c r="G63" s="91"/>
     </row>
     <row r="64" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B64" s="96"/>
-      <c r="C64" s="97"/>
-      <c r="D64" s="104"/>
-      <c r="E64" s="99"/>
+      <c r="B64" s="94"/>
+      <c r="C64" s="95"/>
+      <c r="D64" s="102"/>
+      <c r="E64" s="97"/>
       <c r="F64" s="14"/>
-      <c r="G64" s="93"/>
+      <c r="G64" s="91"/>
     </row>
     <row r="65" spans="2:7" ht="34.5" customHeight="1" thickBot="1">
       <c r="B65" s="8"/>
@@ -40319,35 +40388,35 @@
       <c r="E65" s="9"/>
       <c r="F65" s="50"/>
     </row>
-    <row r="66" spans="2:7" s="92" customFormat="1" ht="45.75" customHeight="1">
-      <c r="G66" s="121"/>
+    <row r="66" spans="2:7" s="90" customFormat="1" ht="45.75" customHeight="1">
+      <c r="G66" s="153"/>
     </row>
-    <row r="67" spans="2:7" s="92" customFormat="1" ht="45.75" customHeight="1">
-      <c r="G67" s="121"/>
+    <row r="67" spans="2:7" s="90" customFormat="1" ht="45.75" customHeight="1">
+      <c r="G67" s="153"/>
     </row>
-    <row r="68" spans="2:7" s="92" customFormat="1" ht="43.5" customHeight="1">
-      <c r="G68" s="93"/>
+    <row r="68" spans="2:7" s="90" customFormat="1" ht="43.5" customHeight="1">
+      <c r="G68" s="91"/>
     </row>
-    <row r="69" spans="2:7" s="92" customFormat="1" ht="43.5" customHeight="1">
-      <c r="G69" s="93"/>
+    <row r="69" spans="2:7" s="90" customFormat="1" ht="43.5" customHeight="1">
+      <c r="G69" s="91"/>
     </row>
-    <row r="71" spans="2:7" s="92" customFormat="1" ht="43.5" customHeight="1">
-      <c r="G71" s="93"/>
+    <row r="71" spans="2:7" s="90" customFormat="1" ht="43.5" customHeight="1">
+      <c r="G71" s="91"/>
     </row>
-    <row r="72" spans="2:7" s="92" customFormat="1" ht="31.5" customHeight="1">
-      <c r="G72" s="93"/>
+    <row r="72" spans="2:7" s="90" customFormat="1" ht="31.5" customHeight="1">
+      <c r="G72" s="91"/>
     </row>
-    <row r="73" spans="2:7" s="92" customFormat="1" ht="31.5" customHeight="1">
-      <c r="G73" s="93"/>
+    <row r="73" spans="2:7" s="90" customFormat="1" ht="31.5" customHeight="1">
+      <c r="G73" s="91"/>
     </row>
-    <row r="74" spans="2:7" s="92" customFormat="1" ht="31.5" customHeight="1">
-      <c r="G74" s="93"/>
+    <row r="74" spans="2:7" s="90" customFormat="1" ht="31.5" customHeight="1">
+      <c r="G74" s="91"/>
     </row>
-    <row r="75" spans="2:7" s="92" customFormat="1" ht="31.5" customHeight="1">
-      <c r="G75" s="93"/>
+    <row r="75" spans="2:7" s="90" customFormat="1" ht="31.5" customHeight="1">
+      <c r="G75" s="91"/>
     </row>
-    <row r="76" spans="2:7" s="92" customFormat="1" ht="20.25">
-      <c r="G76" s="93"/>
+    <row r="76" spans="2:7" s="90" customFormat="1" ht="20.25">
+      <c r="G76" s="91"/>
     </row>
     <row r="77" spans="2:7" ht="22.5">
       <c r="F77" s="11"/>
@@ -40384,6 +40453,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="C12:C19"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="E12:E18"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D12:D19"/>
+    <mergeCell ref="E7:E11"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="C36:C51"/>
     <mergeCell ref="B36:B51"/>
@@ -40400,30 +40493,6 @@
     <mergeCell ref="C6:C11"/>
     <mergeCell ref="B6:B11"/>
     <mergeCell ref="D7:D11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="E20:E24"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="D20:D25"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="E12:E18"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D12:D19"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="C12:C19"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D61:D62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="28" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40453,12 +40522,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="30.75">
-      <c r="B2" s="165" t="s">
+      <c r="B2" s="155" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -40469,20 +40538,20 @@
       <c r="M2" s="4"/>
     </row>
     <row r="4" spans="2:13">
-      <c r="B4" s="157" t="s">
+      <c r="B4" s="156" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="157" t="s">
+      <c r="C4" s="156" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="159" t="s">
+      <c r="D4" s="158" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="160"/>
+      <c r="E4" s="159"/>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="158"/>
-      <c r="C5" s="158"/>
+      <c r="B5" s="157"/>
+      <c r="C5" s="157"/>
       <c r="D5" s="17" t="s">
         <v>54</v>
       </c>
@@ -40497,16 +40566,16 @@
       <c r="C6" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="161" t="s">
+      <c r="D6" s="162" t="s">
         <v>137</v>
       </c>
-      <c r="E6" s="162"/>
+      <c r="E6" s="163"/>
     </row>
     <row r="7" spans="2:13" ht="23.25" customHeight="1">
-      <c r="B7" s="166" t="s">
+      <c r="B7" s="164" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="169" t="s">
+      <c r="C7" s="167" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="16" t="s">
@@ -40516,12 +40585,12 @@
         <v>55</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="2:13">
-      <c r="B8" s="167"/>
-      <c r="C8" s="170"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="168"/>
       <c r="D8" s="16" t="s">
         <v>61</v>
       </c>
@@ -40530,8 +40599,8 @@
       </c>
     </row>
     <row r="9" spans="2:13">
-      <c r="B9" s="167"/>
-      <c r="C9" s="170"/>
+      <c r="B9" s="165"/>
+      <c r="C9" s="168"/>
       <c r="D9" s="16" t="s">
         <v>60</v>
       </c>
@@ -40540,50 +40609,50 @@
       </c>
     </row>
     <row r="10" spans="2:13">
-      <c r="B10" s="167"/>
-      <c r="C10" s="170"/>
+      <c r="B10" s="165"/>
+      <c r="C10" s="168"/>
       <c r="D10" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="2:13">
-      <c r="B11" s="167"/>
-      <c r="C11" s="170"/>
+      <c r="B11" s="165"/>
+      <c r="C11" s="168"/>
       <c r="D11" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:13">
-      <c r="B12" s="168"/>
-      <c r="C12" s="171"/>
+      <c r="B12" s="166"/>
+      <c r="C12" s="169"/>
       <c r="D12" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="15" spans="2:13">
-      <c r="B15" s="157" t="s">
+      <c r="B15" s="156" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="157" t="s">
+      <c r="C15" s="156" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="159" t="s">
+      <c r="D15" s="158" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="160"/>
+      <c r="E15" s="159"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
+      <c r="B16" s="157"/>
+      <c r="C16" s="157"/>
       <c r="D16" s="17" t="s">
         <v>54</v>
       </c>
@@ -40598,16 +40667,16 @@
       <c r="C17" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="161" t="s">
+      <c r="D17" s="162" t="s">
         <v>134</v>
       </c>
-      <c r="E17" s="162"/>
+      <c r="E17" s="163"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="163" t="s">
+      <c r="B18" s="160" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="164" t="s">
+      <c r="C18" s="161" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="16" t="s">
@@ -40618,8 +40687,8 @@
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="163"/>
-      <c r="C19" s="164"/>
+      <c r="B19" s="160"/>
+      <c r="C19" s="161"/>
       <c r="D19" s="16" t="s">
         <v>58</v>
       </c>
@@ -40628,8 +40697,8 @@
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="163"/>
-      <c r="C20" s="164"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="161"/>
       <c r="D20" s="16" t="s">
         <v>59</v>
       </c>
@@ -40638,30 +40707,30 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="163"/>
-      <c r="C21" s="164"/>
+      <c r="B21" s="160"/>
+      <c r="C21" s="161"/>
       <c r="D21" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="157" t="s">
+      <c r="B24" s="156" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="157" t="s">
+      <c r="C24" s="156" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="159" t="s">
+      <c r="D24" s="158" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="160"/>
+      <c r="E24" s="159"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="158"/>
-      <c r="C25" s="158"/>
+      <c r="B25" s="157"/>
+      <c r="C25" s="157"/>
       <c r="D25" s="17" t="s">
         <v>54</v>
       </c>
@@ -40676,16 +40745,16 @@
       <c r="C26" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="161" t="s">
+      <c r="D26" s="162" t="s">
         <v>140</v>
       </c>
-      <c r="E26" s="162"/>
+      <c r="E26" s="163"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="163" t="s">
+      <c r="B27" s="160" t="s">
         <v>138</v>
       </c>
-      <c r="C27" s="164" t="s">
+      <c r="C27" s="161" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="16" t="s">
@@ -40696,8 +40765,8 @@
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="163"/>
-      <c r="C28" s="164"/>
+      <c r="B28" s="160"/>
+      <c r="C28" s="161"/>
       <c r="D28" s="16" t="s">
         <v>64</v>
       </c>
@@ -40706,16 +40775,16 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="163"/>
-      <c r="C29" s="164"/>
+      <c r="B29" s="160"/>
+      <c r="C29" s="161"/>
       <c r="D29" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="163"/>
-      <c r="C30" s="164"/>
+      <c r="B30" s="160"/>
+      <c r="C30" s="161"/>
       <c r="D30" s="16" t="s">
         <v>65</v>
       </c>
@@ -40724,20 +40793,20 @@
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="157" t="s">
+      <c r="B32" s="156" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="157" t="s">
+      <c r="C32" s="156" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="159" t="s">
+      <c r="D32" s="158" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="160"/>
+      <c r="E32" s="159"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="158"/>
-      <c r="C33" s="158"/>
+      <c r="B33" s="157"/>
+      <c r="C33" s="157"/>
       <c r="D33" s="17" t="s">
         <v>54</v>
       </c>
@@ -40752,16 +40821,16 @@
       <c r="C34" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D34" s="161" t="s">
+      <c r="D34" s="162" t="s">
         <v>130</v>
       </c>
-      <c r="E34" s="162"/>
+      <c r="E34" s="163"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="163" t="s">
+      <c r="B35" s="160" t="s">
         <v>128</v>
       </c>
-      <c r="C35" s="164" t="s">
+      <c r="C35" s="161" t="s">
         <v>53</v>
       </c>
       <c r="D35" s="16" t="s">
@@ -40772,8 +40841,8 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="163"/>
-      <c r="C36" s="164"/>
+      <c r="B36" s="160"/>
+      <c r="C36" s="161"/>
       <c r="D36" s="16" t="s">
         <v>58</v>
       </c>
@@ -40782,18 +40851,18 @@
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="163"/>
-      <c r="C37" s="164"/>
+      <c r="B37" s="160"/>
+      <c r="C37" s="161"/>
       <c r="D37" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="163"/>
-      <c r="C38" s="164"/>
+      <c r="B38" s="160"/>
+      <c r="C38" s="161"/>
       <c r="D38" s="16" t="s">
         <v>131</v>
       </c>
@@ -40803,6 +40872,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -40816,18 +40897,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="C7:C12"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40856,21 +40925,21 @@
   <sheetData>
     <row r="4" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="157" t="s">
+      <c r="B4" s="156" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="157" t="s">
+      <c r="C4" s="156" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="159" t="s">
+      <c r="D4" s="158" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="160"/>
+      <c r="E4" s="159"/>
     </row>
     <row r="5" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="158"/>
-      <c r="C5" s="158"/>
+      <c r="B5" s="157"/>
+      <c r="C5" s="157"/>
       <c r="D5" s="17" t="s">
         <v>54</v>
       </c>
@@ -40880,10 +40949,10 @@
     </row>
     <row r="6" spans="1:5" s="5" customFormat="1" ht="23.25" customHeight="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="166" t="s">
+      <c r="B6" s="164" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="169" t="s">
+      <c r="C6" s="167" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="16" t="s">
@@ -40895,8 +40964,8 @@
     </row>
     <row r="7" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="167"/>
-      <c r="C7" s="170"/>
+      <c r="B7" s="165"/>
+      <c r="C7" s="168"/>
       <c r="D7" s="16" t="s">
         <v>61</v>
       </c>
@@ -40906,8 +40975,8 @@
     </row>
     <row r="8" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="167"/>
-      <c r="C8" s="170"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="168"/>
       <c r="D8" s="16" t="s">
         <v>60</v>
       </c>
@@ -40917,28 +40986,28 @@
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="167"/>
-      <c r="C9" s="170"/>
+      <c r="B9" s="165"/>
+      <c r="C9" s="168"/>
       <c r="D9" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="167"/>
-      <c r="C10" s="170"/>
+      <c r="B10" s="165"/>
+      <c r="C10" s="168"/>
       <c r="D10" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="168"/>
-      <c r="C11" s="171"/>
+      <c r="B11" s="166"/>
+      <c r="C11" s="169"/>
       <c r="D11" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E11" s="19"/>
     </row>
@@ -40982,7 +41051,7 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="95"/>
+      <c r="E17" s="93"/>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A18" s="2"/>
@@ -41028,20 +41097,20 @@
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" ht="23.25">
-      <c r="B25" s="157" t="s">
+      <c r="B25" s="156" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="157" t="s">
+      <c r="C25" s="156" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="159" t="s">
+      <c r="D25" s="158" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="160"/>
+      <c r="E25" s="159"/>
     </row>
     <row r="26" spans="1:5" ht="23.25">
-      <c r="B26" s="158"/>
-      <c r="C26" s="158"/>
+      <c r="B26" s="157"/>
+      <c r="C26" s="157"/>
       <c r="D26" s="17" t="s">
         <v>54</v>
       </c>
@@ -41056,16 +41125,16 @@
       <c r="C27" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="161" t="s">
+      <c r="D27" s="162" t="s">
         <v>134</v>
       </c>
-      <c r="E27" s="162"/>
+      <c r="E27" s="163"/>
     </row>
     <row r="28" spans="1:5" ht="23.25" customHeight="1">
-      <c r="B28" s="163" t="s">
+      <c r="B28" s="160" t="s">
         <v>132</v>
       </c>
-      <c r="C28" s="164" t="s">
+      <c r="C28" s="161" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="16" t="s">
@@ -41074,42 +41143,42 @@
       <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:5" ht="23.25">
-      <c r="B29" s="163"/>
-      <c r="C29" s="164"/>
+      <c r="B29" s="160"/>
+      <c r="C29" s="161"/>
       <c r="D29" s="16" t="s">
         <v>58</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:5" ht="23.25">
-      <c r="B30" s="163"/>
-      <c r="C30" s="164"/>
+      <c r="B30" s="160"/>
+      <c r="C30" s="161"/>
       <c r="D30" s="16" t="s">
         <v>59</v>
       </c>
       <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5" ht="23.25">
-      <c r="B31" s="163"/>
-      <c r="C31" s="164"/>
+      <c r="B31" s="160"/>
+      <c r="C31" s="161"/>
       <c r="D31" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E31" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B6:B11"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="C28:C31"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="B6:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -41146,46 +41215,46 @@
     </row>
     <row r="3" spans="1:26">
       <c r="S3" s="67"/>
-      <c r="T3" s="174" t="s">
+      <c r="T3" s="172" t="s">
         <v>81</v>
       </c>
-      <c r="U3" s="174"/>
-      <c r="V3" s="174"/>
-      <c r="W3" s="174"/>
-      <c r="X3" s="174"/>
-      <c r="Y3" s="174"/>
+      <c r="U3" s="172"/>
+      <c r="V3" s="172"/>
+      <c r="W3" s="172"/>
+      <c r="X3" s="172"/>
+      <c r="Y3" s="172"/>
       <c r="Z3" s="68"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="175">
+      <c r="A4" s="173">
         <v>1</v>
       </c>
       <c r="S4" s="67"/>
-      <c r="T4" s="174"/>
-      <c r="U4" s="174"/>
-      <c r="V4" s="174"/>
-      <c r="W4" s="174"/>
-      <c r="X4" s="174"/>
-      <c r="Y4" s="174"/>
+      <c r="T4" s="172"/>
+      <c r="U4" s="172"/>
+      <c r="V4" s="172"/>
+      <c r="W4" s="172"/>
+      <c r="X4" s="172"/>
+      <c r="Y4" s="172"/>
       <c r="Z4" s="68"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="175"/>
+      <c r="A5" s="173"/>
       <c r="S5" s="67"/>
-      <c r="T5" s="172" t="s">
+      <c r="T5" s="170" t="s">
         <v>84</v>
       </c>
-      <c r="U5" s="172"/>
-      <c r="V5" s="172"/>
-      <c r="W5" s="173" t="s">
+      <c r="U5" s="170"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="171" t="s">
         <v>83</v>
       </c>
-      <c r="X5" s="172"/>
-      <c r="Y5" s="172"/>
+      <c r="X5" s="170"/>
+      <c r="Y5" s="170"/>
       <c r="Z5" s="68"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="175"/>
+      <c r="A6" s="173"/>
       <c r="S6" s="67"/>
       <c r="V6" t="s">
         <v>80</v>
@@ -41194,7 +41263,7 @@
       <c r="Z6" s="68"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="175"/>
+      <c r="A7" s="173"/>
       <c r="S7" s="67"/>
       <c r="W7" s="15"/>
       <c r="Y7" t="s">
@@ -41203,13 +41272,13 @@
       <c r="Z7" s="68"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="175"/>
+      <c r="A8" s="173"/>
       <c r="S8" s="67"/>
       <c r="W8" s="15"/>
       <c r="Z8" s="68"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="175"/>
+      <c r="A9" s="173"/>
       <c r="S9" s="67"/>
       <c r="V9" t="s">
         <v>82</v>
@@ -41218,13 +41287,13 @@
       <c r="Z9" s="68"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="175"/>
+      <c r="A10" s="173"/>
       <c r="S10" s="67"/>
       <c r="W10" s="15"/>
       <c r="Z10" s="68"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="175"/>
+      <c r="A11" s="173"/>
       <c r="S11" s="67"/>
       <c r="W11" s="15"/>
       <c r="Z11" s="68"/>
@@ -41310,186 +41379,186 @@
       <c r="Z25" s="71"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="175">
+      <c r="A36" s="173">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="175"/>
+      <c r="A37" s="173"/>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="175"/>
+      <c r="A38" s="173"/>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="175"/>
+      <c r="A39" s="173"/>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="175"/>
+      <c r="A40" s="173"/>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="175"/>
+      <c r="A41" s="173"/>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="175"/>
+      <c r="A42" s="173"/>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="175"/>
+      <c r="A43" s="173"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="175">
+      <c r="A68" s="173">
         <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="175"/>
+      <c r="A69" s="173"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="175"/>
+      <c r="A70" s="173"/>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="175"/>
+      <c r="A71" s="173"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="175"/>
+      <c r="A72" s="173"/>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="175"/>
+      <c r="A73" s="173"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="175"/>
+      <c r="A74" s="173"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="175"/>
+      <c r="A75" s="173"/>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="175">
+      <c r="A100" s="173">
         <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="175"/>
+      <c r="A101" s="173"/>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="175"/>
+      <c r="A102" s="173"/>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="175"/>
+      <c r="A103" s="173"/>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="175"/>
+      <c r="A104" s="173"/>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="175"/>
+      <c r="A105" s="173"/>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="175"/>
+      <c r="A106" s="173"/>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="175"/>
+      <c r="A107" s="173"/>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="175">
+      <c r="A132" s="173">
         <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:1">
-      <c r="A133" s="175"/>
+      <c r="A133" s="173"/>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="175"/>
+      <c r="A134" s="173"/>
     </row>
     <row r="135" spans="1:1">
-      <c r="A135" s="175"/>
+      <c r="A135" s="173"/>
     </row>
     <row r="136" spans="1:1">
-      <c r="A136" s="175"/>
+      <c r="A136" s="173"/>
     </row>
     <row r="137" spans="1:1">
-      <c r="A137" s="175"/>
+      <c r="A137" s="173"/>
     </row>
     <row r="138" spans="1:1">
-      <c r="A138" s="175"/>
+      <c r="A138" s="173"/>
     </row>
     <row r="139" spans="1:1">
-      <c r="A139" s="175"/>
+      <c r="A139" s="173"/>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="175">
+      <c r="A164" s="173">
         <v>6</v>
       </c>
     </row>
     <row r="165" spans="1:1">
-      <c r="A165" s="175"/>
+      <c r="A165" s="173"/>
     </row>
     <row r="166" spans="1:1">
-      <c r="A166" s="175"/>
+      <c r="A166" s="173"/>
     </row>
     <row r="167" spans="1:1">
-      <c r="A167" s="175"/>
+      <c r="A167" s="173"/>
     </row>
     <row r="168" spans="1:1">
-      <c r="A168" s="175"/>
+      <c r="A168" s="173"/>
     </row>
     <row r="169" spans="1:1">
-      <c r="A169" s="175"/>
+      <c r="A169" s="173"/>
     </row>
     <row r="170" spans="1:1">
-      <c r="A170" s="175"/>
+      <c r="A170" s="173"/>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" s="175"/>
+      <c r="A171" s="173"/>
     </row>
     <row r="196" spans="1:1">
-      <c r="A196" s="175">
+      <c r="A196" s="173">
         <v>7</v>
       </c>
     </row>
     <row r="197" spans="1:1">
-      <c r="A197" s="175"/>
+      <c r="A197" s="173"/>
     </row>
     <row r="198" spans="1:1">
-      <c r="A198" s="175"/>
+      <c r="A198" s="173"/>
     </row>
     <row r="199" spans="1:1">
-      <c r="A199" s="175"/>
+      <c r="A199" s="173"/>
     </row>
     <row r="200" spans="1:1">
-      <c r="A200" s="175"/>
+      <c r="A200" s="173"/>
     </row>
     <row r="201" spans="1:1">
-      <c r="A201" s="175"/>
+      <c r="A201" s="173"/>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" s="175"/>
+      <c r="A202" s="173"/>
     </row>
     <row r="203" spans="1:1">
-      <c r="A203" s="175"/>
+      <c r="A203" s="173"/>
     </row>
     <row r="228" spans="1:1">
-      <c r="A228" s="175">
+      <c r="A228" s="173">
         <v>8</v>
       </c>
     </row>
     <row r="229" spans="1:1">
-      <c r="A229" s="175"/>
+      <c r="A229" s="173"/>
     </row>
     <row r="230" spans="1:1">
-      <c r="A230" s="175"/>
+      <c r="A230" s="173"/>
     </row>
     <row r="231" spans="1:1">
-      <c r="A231" s="175"/>
+      <c r="A231" s="173"/>
     </row>
     <row r="232" spans="1:1">
-      <c r="A232" s="175"/>
+      <c r="A232" s="173"/>
     </row>
     <row r="233" spans="1:1">
-      <c r="A233" s="175"/>
+      <c r="A233" s="173"/>
     </row>
     <row r="234" spans="1:1">
-      <c r="A234" s="175"/>
+      <c r="A234" s="173"/>
     </row>
     <row r="235" spans="1:1">
-      <c r="A235" s="175"/>
+      <c r="A235" s="173"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -41531,243 +41600,243 @@
     <col min="10" max="10" width="44.42578125" customWidth="1"/>
     <col min="11" max="11" width="65" customWidth="1"/>
     <col min="12" max="12" width="116.7109375" customWidth="1"/>
-    <col min="13" max="13" width="44.42578125" style="87" customWidth="1"/>
+    <col min="13" max="13" width="44.42578125" style="86" customWidth="1"/>
     <col min="14" max="21" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="70" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="C70" s="176" t="s">
-        <v>184</v>
+      <c r="C70" s="174" t="s">
+        <v>183</v>
       </c>
-      <c r="D70" s="176" t="s">
+      <c r="D70" s="174" t="s">
+        <v>168</v>
+      </c>
+      <c r="E70" s="174" t="s">
+        <v>167</v>
+      </c>
+      <c r="F70" s="177" t="s">
+        <v>173</v>
+      </c>
+      <c r="G70" s="174" t="s">
+        <v>166</v>
+      </c>
+      <c r="H70" s="174" t="s">
+        <v>172</v>
+      </c>
+      <c r="I70" s="174"/>
+      <c r="J70" s="174" t="s">
+        <v>3</v>
+      </c>
+      <c r="K70" s="174"/>
+      <c r="L70" s="174"/>
+      <c r="M70" s="174"/>
+    </row>
+    <row r="71" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
+      <c r="C71" s="174"/>
+      <c r="D71" s="174"/>
+      <c r="E71" s="174"/>
+      <c r="F71" s="174"/>
+      <c r="G71" s="174"/>
+      <c r="H71" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="I71" s="75" t="s">
+        <v>163</v>
+      </c>
+      <c r="J71" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="K71" s="74" t="s">
+        <v>164</v>
+      </c>
+      <c r="L71" s="74" t="s">
+        <v>165</v>
+      </c>
+      <c r="M71" s="83" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="72" spans="3:13" s="2" customFormat="1" ht="151.5" customHeight="1">
+      <c r="C72" s="175" t="s">
+        <v>199</v>
+      </c>
+      <c r="D72" s="176"/>
+      <c r="E72" s="76"/>
+      <c r="F72" s="77"/>
+      <c r="G72" s="77"/>
+      <c r="H72" s="78"/>
+      <c r="I72" s="79"/>
+      <c r="L72" s="80"/>
+      <c r="M72" s="84"/>
+    </row>
+    <row r="73" spans="3:13" s="2" customFormat="1" ht="139.5">
+      <c r="C73" s="88" t="s">
         <v>169</v>
       </c>
-      <c r="E70" s="176" t="s">
-        <v>168</v>
+      <c r="D73" s="2" t="s">
+        <v>169</v>
       </c>
-      <c r="F70" s="179" t="s">
-        <v>174</v>
+      <c r="E73" s="76" t="s">
+        <v>197</v>
       </c>
-      <c r="G70" s="176" t="s">
-        <v>167</v>
+      <c r="F73" s="77" t="s">
+        <v>175</v>
       </c>
-      <c r="H70" s="176" t="s">
-        <v>173</v>
+      <c r="G73" s="77" t="s">
+        <v>176</v>
       </c>
-      <c r="I70" s="176"/>
-      <c r="J70" s="176" t="s">
-        <v>3</v>
+      <c r="H73" s="78" t="s">
+        <v>177</v>
       </c>
-      <c r="K70" s="176"/>
-      <c r="L70" s="176"/>
-      <c r="M70" s="176"/>
-    </row>
-    <row r="71" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="C71" s="176"/>
-      <c r="D71" s="176"/>
-      <c r="E71" s="176"/>
-      <c r="F71" s="176"/>
-      <c r="G71" s="176"/>
-      <c r="H71" s="75" t="s">
-        <v>172</v>
+      <c r="I73" s="79" t="s">
+        <v>178</v>
       </c>
-      <c r="I71" s="76" t="s">
-        <v>164</v>
+      <c r="J73" s="2" t="s">
+        <v>180</v>
       </c>
-      <c r="J71" s="75" t="s">
-        <v>171</v>
+      <c r="K73" s="2" t="s">
+        <v>181</v>
       </c>
-      <c r="K71" s="75" t="s">
-        <v>165</v>
+      <c r="L73" s="80" t="s">
+        <v>179</v>
       </c>
-      <c r="L71" s="75" t="s">
-        <v>166</v>
-      </c>
-      <c r="M71" s="84" t="s">
+      <c r="M73" s="84" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="72" spans="3:13" s="2" customFormat="1" ht="151.5" customHeight="1">
-      <c r="C72" s="177" t="s">
-        <v>200</v>
+    <row r="74" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
+      <c r="D74" s="81" t="s">
+        <v>182</v>
       </c>
-      <c r="D72" s="178"/>
-      <c r="E72" s="77"/>
-      <c r="F72" s="78"/>
-      <c r="G72" s="78"/>
-      <c r="H72" s="79"/>
-      <c r="I72" s="80"/>
-      <c r="L72" s="81"/>
-      <c r="M72" s="85"/>
-    </row>
-    <row r="73" spans="3:13" s="2" customFormat="1" ht="139.5">
-      <c r="C73" s="89" t="s">
-        <v>170</v>
+      <c r="E74" s="2" t="s">
+        <v>196</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>170</v>
+      <c r="G74" s="77" t="s">
+        <v>194</v>
       </c>
-      <c r="E73" s="77" t="s">
-        <v>198</v>
+      <c r="J74" s="2" t="s">
+        <v>180</v>
       </c>
-      <c r="F73" s="78" t="s">
-        <v>176</v>
-      </c>
-      <c r="G73" s="78" t="s">
-        <v>177</v>
-      </c>
-      <c r="H73" s="79" t="s">
-        <v>178</v>
-      </c>
-      <c r="I73" s="80" t="s">
-        <v>179</v>
-      </c>
-      <c r="J73" s="2" t="s">
+      <c r="K74" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="K73" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="L73" s="81" t="s">
-        <v>180</v>
-      </c>
-      <c r="M73" s="85" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="74" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
-      <c r="D74" s="82" t="s">
-        <v>183</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G74" s="78" t="s">
+      <c r="L74" s="80" t="s">
         <v>195</v>
       </c>
-      <c r="J74" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="L74" s="81" t="s">
-        <v>196</v>
-      </c>
-      <c r="M74" s="85" t="s">
-        <v>194</v>
+      <c r="M74" s="84" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="75" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
-      <c r="C75" s="88" t="s">
-        <v>199</v>
+      <c r="C75" s="87" t="s">
+        <v>198</v>
       </c>
-      <c r="M75" s="86"/>
+      <c r="M75" s="85"/>
     </row>
     <row r="76" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
-      <c r="D76" s="82" t="s">
+      <c r="D76" s="81" t="s">
+        <v>189</v>
+      </c>
+      <c r="M76" s="85"/>
+    </row>
+    <row r="77" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
+      <c r="D77" s="81" t="s">
         <v>190</v>
       </c>
-      <c r="M76" s="86"/>
+      <c r="M77" s="85"/>
     </row>
-    <row r="77" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
-      <c r="D77" s="82" t="s">
+    <row r="78" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
+      <c r="C78" s="82" t="s">
+        <v>184</v>
+      </c>
+      <c r="M78" s="85"/>
+    </row>
+    <row r="79" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
+      <c r="C79" s="82" t="s">
+        <v>185</v>
+      </c>
+      <c r="M79" s="85"/>
+    </row>
+    <row r="80" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
+      <c r="C80" s="82" t="s">
+        <v>186</v>
+      </c>
+      <c r="M80" s="85"/>
+    </row>
+    <row r="81" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
+      <c r="C81" s="82" t="s">
+        <v>187</v>
+      </c>
+      <c r="M81" s="85"/>
+    </row>
+    <row r="82" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
+      <c r="C82" s="82" t="s">
+        <v>188</v>
+      </c>
+      <c r="M82" s="85"/>
+    </row>
+    <row r="83" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
+      <c r="C83" s="82" t="s">
         <v>191</v>
       </c>
-      <c r="M77" s="86"/>
-    </row>
-    <row r="78" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
-      <c r="C78" s="83" t="s">
-        <v>185</v>
-      </c>
-      <c r="M78" s="86"/>
-    </row>
-    <row r="79" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
-      <c r="C79" s="83" t="s">
-        <v>186</v>
-      </c>
-      <c r="M79" s="86"/>
-    </row>
-    <row r="80" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
-      <c r="C80" s="83" t="s">
-        <v>187</v>
-      </c>
-      <c r="M80" s="86"/>
-    </row>
-    <row r="81" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
-      <c r="C81" s="83" t="s">
-        <v>188</v>
-      </c>
-      <c r="M81" s="86"/>
-    </row>
-    <row r="82" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
-      <c r="C82" s="83" t="s">
-        <v>189</v>
-      </c>
-      <c r="M82" s="86"/>
-    </row>
-    <row r="83" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
-      <c r="C83" s="83" t="s">
-        <v>192</v>
-      </c>
-      <c r="M83" s="86"/>
+      <c r="M83" s="85"/>
     </row>
     <row r="84" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M84" s="86"/>
+      <c r="M84" s="85"/>
     </row>
     <row r="85" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M85" s="86"/>
+      <c r="M85" s="85"/>
     </row>
     <row r="86" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M86" s="86"/>
+      <c r="M86" s="85"/>
     </row>
     <row r="87" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M87" s="86"/>
+      <c r="M87" s="85"/>
     </row>
     <row r="88" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M88" s="86"/>
+      <c r="M88" s="85"/>
     </row>
     <row r="89" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M89" s="86"/>
+      <c r="M89" s="85"/>
     </row>
     <row r="90" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M90" s="86"/>
+      <c r="M90" s="85"/>
     </row>
     <row r="91" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M91" s="86"/>
+      <c r="M91" s="85"/>
     </row>
     <row r="92" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M92" s="86"/>
+      <c r="M92" s="85"/>
     </row>
     <row r="93" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M93" s="86"/>
+      <c r="M93" s="85"/>
     </row>
     <row r="94" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M94" s="86"/>
+      <c r="M94" s="85"/>
     </row>
     <row r="95" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M95" s="86"/>
+      <c r="M95" s="85"/>
     </row>
     <row r="96" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M96" s="86"/>
+      <c r="M96" s="85"/>
     </row>
     <row r="97" spans="13:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M97" s="86"/>
+      <c r="M97" s="85"/>
     </row>
     <row r="98" spans="13:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M98" s="86"/>
+      <c r="M98" s="85"/>
     </row>
     <row r="99" spans="13:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M99" s="86"/>
+      <c r="M99" s="85"/>
     </row>
     <row r="100" spans="13:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M100" s="86"/>
+      <c r="M100" s="85"/>
     </row>
     <row r="101" spans="13:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M101" s="86"/>
+      <c r="M101" s="85"/>
     </row>
     <row r="102" spans="13:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="M102" s="86"/>
+      <c r="M102" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
I implemented a user management page to manage the definition of users' role
</commit_message>
<xml_diff>
--- a/Final-React-Project-Design.xlsx
+++ b/Final-React-Project-Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basheer\Desktop\בשיר\Full Stack Work\Full Stack Cors - YanivArad\Projects\React-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88373DD-A9E9-4689-A63A-1C157CB89B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B93EC7-E3B2-47A9-9A9A-B4EB8CD326BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="970" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <sheet name="Actions" sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Plan Work'!$A$5:$F$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Plan Work'!$A$5:$F$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="253">
   <si>
     <t>Num</t>
   </si>
@@ -3897,58 +3897,6 @@
     <t>Build the purchases model</t>
   </si>
   <si>
-    <t>Build the Home Page</t>
-  </si>
-  <si>
-    <t>Build the calculation in the app like amount of purchases products, new products, top selling adv</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Step 9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Statistical calculations</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Step 8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Home Page</t>
-    </r>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -5232,138 +5180,7 @@
     <t>20-27/11/23</t>
   </si>
   <si>
-    <t>28-29/11/23</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Step 10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - improve and sync store data</t>
-    </r>
-  </si>
-  <si>
     <t>Improve and Sync between the external DB [Firebase] and the internal DB [redux]</t>
-  </si>
-  <si>
-    <t>29/11/23-5/12/23</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Step 11</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Users collection</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Step 12</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - optimization</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Step 14</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Tests</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Step 13</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Build dashboard page - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Optionally</t>
-    </r>
   </si>
   <si>
     <t>I will add a dashboard page that gives the possibility to manage the necessary data</t>
@@ -5376,6 +5193,247 @@
   </si>
   <si>
     <t>10-11/12/2023</t>
+  </si>
+  <si>
+    <t>Authentication to Firebase with email and password</t>
+  </si>
+  <si>
+    <t>29/11/23</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Authentication App</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Assign roles</t>
+    </r>
+  </si>
+  <si>
+    <t>Assign admin and regular roles, use service cloud.firestore</t>
+  </si>
+  <si>
+    <t>30/11/23</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Share components</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Home Page and Statistical calculations</t>
+    </r>
+  </si>
+  <si>
+    <t>Build the Home Page, and the calculation in the app like amount of purchases products, new products, top selling adv</t>
+  </si>
+  <si>
+    <t>1-2/12/23</t>
+  </si>
+  <si>
+    <t>3-5/12/23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improved the display of the parent components, and building sharing between components </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - improve and sync store data</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Users collection</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - optimization</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Build dashboard page - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Optionally</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Tests</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -6728,6 +6786,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -6740,14 +6801,95 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6776,16 +6918,7 @@
     <xf numFmtId="0" fontId="47" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6800,86 +6933,11 @@
     <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6893,16 +6951,19 @@
     <xf numFmtId="0" fontId="25" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6945,9 +7006,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -39251,10 +39309,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="B1:F29"/>
+  <dimension ref="B1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15"/>
@@ -39272,44 +39330,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6">
-      <c r="B1" s="107" t="s">
+      <c r="B1" s="108" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
     </row>
     <row r="2" spans="2:6">
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="108" t="s">
+      <c r="B4" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="C4" s="109" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="108" t="s">
+      <c r="D4" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="108" t="s">
+      <c r="E4" s="109" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="108" t="s">
+      <c r="F4" s="109" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="46">
@@ -39328,7 +39386,7 @@
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="46" t="s">
         <v>72</v>
@@ -39345,9 +39403,9 @@
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="46">
-        <v>2</v>
+        <v>3</v>
       </c>
-      <c r="C8" s="105" t="s">
+      <c r="C8" s="106" t="s">
         <v>68</v>
       </c>
       <c r="D8" s="47" t="s">
@@ -39362,9 +39420,9 @@
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="46">
-        <v>3</v>
+        <v>4</v>
       </c>
-      <c r="C9" s="106"/>
+      <c r="C9" s="107"/>
       <c r="D9" s="46" t="s">
         <v>70</v>
       </c>
@@ -39377,7 +39435,7 @@
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="46" t="s">
         <v>76</v>
@@ -39386,7 +39444,7 @@
         <v>146</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>124</v>
@@ -39394,7 +39452,7 @@
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" s="46" t="s">
         <v>147</v>
@@ -39403,7 +39461,7 @@
         <v>143</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>124</v>
@@ -39411,7 +39469,7 @@
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="46">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="46" t="s">
         <v>148</v>
@@ -39420,7 +39478,7 @@
         <v>144</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>124</v>
@@ -39428,7 +39486,7 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="46">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="46" t="s">
         <v>149</v>
@@ -39437,7 +39495,7 @@
         <v>145</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>124</v>
@@ -39445,7 +39503,7 @@
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="46">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="46" t="s">
         <v>150</v>
@@ -39454,7 +39512,7 @@
         <v>142</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>124</v>
@@ -39462,16 +39520,16 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="46">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D15" s="46" t="s">
         <v>151</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>124</v>
@@ -39479,16 +39537,16 @@
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="46">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D16" s="46" t="s">
         <v>152</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>124</v>
@@ -39496,151 +39554,185 @@
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="46">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D17" s="46" t="s">
         <v>153</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" ht="30">
       <c r="B18" s="46">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>157</v>
+        <v>243</v>
       </c>
       <c r="D18" s="46" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="30">
+    <row r="19" spans="2:6">
       <c r="B19" s="46">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>156</v>
+        <v>238</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>155</v>
+        <v>236</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="30">
+    <row r="20" spans="2:6">
       <c r="B20" s="46">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D20" s="46" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" ht="30">
       <c r="B21" s="46">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>161</v>
+        <v>247</v>
       </c>
-      <c r="E21" s="104" t="s">
-        <v>244</v>
+      <c r="E21" s="46" t="s">
+        <v>245</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" ht="30">
       <c r="B22" s="46">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="D22" s="46" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
-      <c r="E22" s="104" t="s">
-        <v>245</v>
+      <c r="E22" s="46" t="s">
+        <v>246</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="23" spans="2:6" ht="30">
+    <row r="23" spans="2:6">
       <c r="B23" s="46">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C23" s="46" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>243</v>
+        <v>157</v>
       </c>
       <c r="E23" s="104" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" s="46">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C24" s="46" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="D24" s="46" t="s">
-        <v>162</v>
+        <v>215</v>
       </c>
-      <c r="E24" s="104">
-        <v>45272</v>
+      <c r="E24" s="104" t="s">
+        <v>234</v>
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="2:6" ht="37.5">
-      <c r="C25" s="89" t="s">
-        <v>200</v>
+    <row r="25" spans="2:6" ht="30">
+      <c r="B25" s="46">
+        <v>20</v>
       </c>
-      <c r="D25" s="178" t="s">
-        <v>201</v>
+      <c r="C25" s="46" t="s">
+        <v>251</v>
       </c>
+      <c r="D25" s="46" t="s">
+        <v>232</v>
+      </c>
+      <c r="E25" s="104" t="s">
+        <v>235</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="46">
+        <v>21</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>252</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>158</v>
+      </c>
+      <c r="E26" s="104">
+        <v>45272</v>
+      </c>
+      <c r="F26" s="1"/>
     </row>
     <row r="27" spans="2:6" ht="37.5">
       <c r="C27" s="89" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
-      <c r="D27" s="178" t="s">
-        <v>203</v>
+      <c r="D27" s="105" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="37.5">
-      <c r="D29" s="178" t="s">
-        <v>204</v>
+      <c r="C29" s="89" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="105" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="37.5">
+      <c r="D31" s="105" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -39653,14 +39745,14 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="E4:E5"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F24">
+  <conditionalFormatting sqref="F6:F26">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="V">
       <formula>NOT(ISERROR(SEARCH("V",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C25" r:id="rId1" xr:uid="{B5AF2755-436A-4008-9BA4-CBBB84CC1736}"/>
-    <hyperlink ref="C27" r:id="rId2" xr:uid="{3D76CBC8-DA15-470A-8E1E-DBBC4061AE14}"/>
+    <hyperlink ref="C27" r:id="rId1" xr:uid="{B5AF2755-436A-4008-9BA4-CBBB84CC1736}"/>
+    <hyperlink ref="C29" r:id="rId2" xr:uid="{3D76CBC8-DA15-470A-8E1E-DBBC4061AE14}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
@@ -39690,36 +39782,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="51.75" customHeight="1">
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="138" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="F2" s="139"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" thickBot="1">
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="148" t="s">
+      <c r="C4" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="148" t="s">
+      <c r="D4" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="148" t="s">
+      <c r="E4" s="118" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="149"/>
+      <c r="F4" s="133"/>
     </row>
     <row r="5" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B5" s="136"/>
-      <c r="C5" s="151"/>
-      <c r="D5" s="151"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
       <c r="E5" s="31" t="s">
         <v>9</v>
       </c>
@@ -39728,10 +39820,10 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B6" s="114">
+      <c r="B6" s="142">
         <v>1</v>
       </c>
-      <c r="C6" s="111" t="s">
+      <c r="C6" s="121" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="73" t="s">
@@ -39745,63 +39837,63 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B7" s="115"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="124" t="s">
-        <v>222</v>
+      <c r="B7" s="143"/>
+      <c r="C7" s="140"/>
+      <c r="D7" s="112" t="s">
+        <v>218</v>
       </c>
-      <c r="E7" s="123" t="s">
-        <v>227</v>
+      <c r="E7" s="135" t="s">
+        <v>223</v>
       </c>
       <c r="F7" s="99" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B8" s="115"/>
-      <c r="C8" s="112"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="121"/>
+      <c r="B8" s="143"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="150"/>
+      <c r="E8" s="136"/>
       <c r="F8" s="99" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B9" s="115"/>
-      <c r="C9" s="112"/>
-      <c r="D9" s="125"/>
-      <c r="E9" s="121"/>
+      <c r="B9" s="143"/>
+      <c r="C9" s="140"/>
+      <c r="D9" s="150"/>
+      <c r="E9" s="136"/>
       <c r="F9" s="99" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B10" s="115"/>
-      <c r="C10" s="112"/>
-      <c r="D10" s="125"/>
-      <c r="E10" s="121"/>
+      <c r="B10" s="143"/>
+      <c r="C10" s="140"/>
+      <c r="D10" s="150"/>
+      <c r="E10" s="136"/>
       <c r="F10" s="100"/>
     </row>
     <row r="11" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B11" s="133"/>
-      <c r="C11" s="132"/>
-      <c r="D11" s="134"/>
-      <c r="E11" s="152"/>
+      <c r="B11" s="155"/>
+      <c r="C11" s="122"/>
+      <c r="D11" s="124"/>
+      <c r="E11" s="137"/>
       <c r="F11" s="101" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="22.5">
       <c r="B12" s="129">
         <v>2</v>
       </c>
-      <c r="C12" s="137" t="s">
+      <c r="C12" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="145" t="s">
+      <c r="D12" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="142" t="s">
+      <c r="E12" s="116" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="38" t="s">
@@ -39810,62 +39902,62 @@
     </row>
     <row r="13" spans="2:6" ht="22.5">
       <c r="B13" s="130"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="146"/>
-      <c r="E13" s="143"/>
+      <c r="C13" s="114"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="117"/>
       <c r="F13" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="22.5">
       <c r="B14" s="130"/>
-      <c r="C14" s="138"/>
-      <c r="D14" s="146"/>
-      <c r="E14" s="143"/>
+      <c r="C14" s="114"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="117"/>
       <c r="F14" s="21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="22.5">
       <c r="B15" s="130"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="146"/>
-      <c r="E15" s="143"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="111"/>
+      <c r="E15" s="117"/>
       <c r="F15" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="22.5">
       <c r="B16" s="130"/>
-      <c r="C16" s="138"/>
-      <c r="D16" s="146"/>
-      <c r="E16" s="143"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="111"/>
+      <c r="E16" s="117"/>
       <c r="F16" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="22.5">
       <c r="B17" s="130"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="143"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="111"/>
+      <c r="E17" s="117"/>
       <c r="F17" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="22.5">
       <c r="B18" s="130"/>
-      <c r="C18" s="138"/>
-      <c r="D18" s="146"/>
-      <c r="E18" s="143"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="117"/>
       <c r="F18" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B19" s="144"/>
-      <c r="C19" s="139"/>
-      <c r="D19" s="147"/>
+      <c r="B19" s="131"/>
+      <c r="C19" s="115"/>
+      <c r="D19" s="132"/>
       <c r="E19" s="40" t="s">
         <v>13</v>
       </c>
@@ -39877,13 +39969,13 @@
       <c r="B20" s="129">
         <v>3</v>
       </c>
-      <c r="C20" s="137" t="s">
+      <c r="C20" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="145" t="s">
+      <c r="D20" s="110" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="142" t="s">
+      <c r="E20" s="116" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="41" t="s">
@@ -39892,44 +39984,44 @@
     </row>
     <row r="21" spans="2:6" ht="34.5" customHeight="1">
       <c r="B21" s="130"/>
-      <c r="C21" s="138"/>
-      <c r="D21" s="146"/>
-      <c r="E21" s="143"/>
+      <c r="C21" s="114"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="117"/>
       <c r="F21" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="34.5" customHeight="1">
       <c r="B22" s="130"/>
-      <c r="C22" s="138"/>
-      <c r="D22" s="146"/>
-      <c r="E22" s="143"/>
+      <c r="C22" s="114"/>
+      <c r="D22" s="111"/>
+      <c r="E22" s="117"/>
       <c r="F22" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="34.5" customHeight="1">
       <c r="B23" s="130"/>
-      <c r="C23" s="138"/>
-      <c r="D23" s="146"/>
-      <c r="E23" s="143"/>
+      <c r="C23" s="114"/>
+      <c r="D23" s="111"/>
+      <c r="E23" s="117"/>
       <c r="F23" s="26" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="34.5" customHeight="1">
       <c r="B24" s="130"/>
-      <c r="C24" s="138"/>
-      <c r="D24" s="146"/>
-      <c r="E24" s="143"/>
+      <c r="C24" s="114"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="117"/>
       <c r="F24" s="27" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B25" s="144"/>
-      <c r="C25" s="139"/>
-      <c r="D25" s="147"/>
+      <c r="B25" s="131"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="132"/>
       <c r="E25" s="40" t="s">
         <v>13</v>
       </c>
@@ -39941,13 +40033,13 @@
       <c r="B26" s="129">
         <v>4</v>
       </c>
-      <c r="C26" s="137" t="s">
+      <c r="C26" s="113" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="145" t="s">
+      <c r="D26" s="110" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="142" t="s">
+      <c r="E26" s="116" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="41" t="s">
@@ -39956,26 +40048,26 @@
     </row>
     <row r="27" spans="2:6" ht="22.5">
       <c r="B27" s="130"/>
-      <c r="C27" s="138"/>
-      <c r="D27" s="146"/>
-      <c r="E27" s="143"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="111"/>
+      <c r="E27" s="117"/>
       <c r="F27" s="28" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="22.5">
       <c r="B28" s="130"/>
-      <c r="C28" s="138"/>
-      <c r="D28" s="146"/>
-      <c r="E28" s="143"/>
+      <c r="C28" s="114"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="117"/>
       <c r="F28" s="29" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="42" customHeight="1" thickBot="1">
-      <c r="B29" s="131"/>
-      <c r="C29" s="150"/>
-      <c r="D29" s="124"/>
+      <c r="B29" s="154"/>
+      <c r="C29" s="134"/>
+      <c r="D29" s="112"/>
       <c r="E29" s="12" t="s">
         <v>13</v>
       </c>
@@ -40004,13 +40096,13 @@
       <c r="B31" s="129">
         <v>6</v>
       </c>
-      <c r="C31" s="137" t="s">
+      <c r="C31" s="113" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="140" t="s">
+      <c r="D31" s="127" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="142" t="s">
+      <c r="E31" s="116" t="s">
         <v>13</v>
       </c>
       <c r="F31" s="41" t="s">
@@ -40019,16 +40111,16 @@
     </row>
     <row r="32" spans="2:6" ht="34.5" customHeight="1">
       <c r="B32" s="130"/>
-      <c r="C32" s="138"/>
-      <c r="D32" s="141"/>
-      <c r="E32" s="143"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="128"/>
+      <c r="E32" s="117"/>
       <c r="F32" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B33" s="144"/>
-      <c r="C33" s="139"/>
+      <c r="B33" s="131"/>
+      <c r="C33" s="115"/>
       <c r="D33" s="39" t="s">
         <v>39</v>
       </c>
@@ -40072,10 +40164,10 @@
       </c>
     </row>
     <row r="36" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B36" s="114">
+      <c r="B36" s="142">
         <v>9</v>
       </c>
-      <c r="C36" s="111" t="s">
+      <c r="C36" s="121" t="s">
         <v>90</v>
       </c>
       <c r="D36" s="73" t="s">
@@ -40089,12 +40181,12 @@
       </c>
     </row>
     <row r="37" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B37" s="115"/>
-      <c r="C37" s="112"/>
-      <c r="D37" s="124" t="s">
+      <c r="B37" s="143"/>
+      <c r="C37" s="140"/>
+      <c r="D37" s="112" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="123" t="s">
+      <c r="E37" s="135" t="s">
         <v>96</v>
       </c>
       <c r="F37" s="55" t="s">
@@ -40102,37 +40194,37 @@
       </c>
     </row>
     <row r="38" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B38" s="115"/>
-      <c r="C38" s="112"/>
-      <c r="D38" s="125"/>
-      <c r="E38" s="121"/>
+      <c r="B38" s="143"/>
+      <c r="C38" s="140"/>
+      <c r="D38" s="150"/>
+      <c r="E38" s="136"/>
       <c r="F38" s="51" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B39" s="115"/>
-      <c r="C39" s="112"/>
-      <c r="D39" s="125"/>
-      <c r="E39" s="121"/>
+      <c r="B39" s="143"/>
+      <c r="C39" s="140"/>
+      <c r="D39" s="150"/>
+      <c r="E39" s="136"/>
       <c r="F39" s="51" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B40" s="115"/>
-      <c r="C40" s="112"/>
-      <c r="D40" s="125"/>
-      <c r="E40" s="122"/>
+      <c r="B40" s="143"/>
+      <c r="C40" s="140"/>
+      <c r="D40" s="150"/>
+      <c r="E40" s="149"/>
       <c r="F40" s="56" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B41" s="115"/>
-      <c r="C41" s="112"/>
-      <c r="D41" s="125"/>
-      <c r="E41" s="123" t="s">
+      <c r="B41" s="143"/>
+      <c r="C41" s="140"/>
+      <c r="D41" s="150"/>
+      <c r="E41" s="135" t="s">
         <v>98</v>
       </c>
       <c r="F41" s="57" t="s">
@@ -40140,54 +40232,54 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B42" s="115"/>
-      <c r="C42" s="112"/>
-      <c r="D42" s="125"/>
-      <c r="E42" s="121"/>
+      <c r="B42" s="143"/>
+      <c r="C42" s="140"/>
+      <c r="D42" s="150"/>
+      <c r="E42" s="136"/>
       <c r="F42" s="58" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B43" s="115"/>
-      <c r="C43" s="112"/>
-      <c r="D43" s="125"/>
-      <c r="E43" s="121"/>
+      <c r="B43" s="143"/>
+      <c r="C43" s="140"/>
+      <c r="D43" s="150"/>
+      <c r="E43" s="136"/>
       <c r="F43" s="58" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B44" s="115"/>
-      <c r="C44" s="112"/>
-      <c r="D44" s="125"/>
-      <c r="E44" s="121"/>
+      <c r="B44" s="143"/>
+      <c r="C44" s="140"/>
+      <c r="D44" s="150"/>
+      <c r="E44" s="136"/>
       <c r="F44" s="59" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B45" s="115"/>
-      <c r="C45" s="112"/>
-      <c r="D45" s="125"/>
-      <c r="E45" s="121"/>
+      <c r="B45" s="143"/>
+      <c r="C45" s="140"/>
+      <c r="D45" s="150"/>
+      <c r="E45" s="136"/>
       <c r="F45" s="59" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B46" s="115"/>
-      <c r="C46" s="112"/>
-      <c r="D46" s="126"/>
-      <c r="E46" s="122"/>
+      <c r="B46" s="143"/>
+      <c r="C46" s="140"/>
+      <c r="D46" s="151"/>
+      <c r="E46" s="149"/>
       <c r="F46" s="60" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="75">
-      <c r="B47" s="115"/>
-      <c r="C47" s="112"/>
-      <c r="D47" s="124" t="s">
+      <c r="B47" s="143"/>
+      <c r="C47" s="140"/>
+      <c r="D47" s="112" t="s">
         <v>97</v>
       </c>
       <c r="E47" s="10" t="s">
@@ -40198,10 +40290,10 @@
       </c>
     </row>
     <row r="48" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B48" s="115"/>
-      <c r="C48" s="112"/>
-      <c r="D48" s="125"/>
-      <c r="E48" s="127" t="s">
+      <c r="B48" s="143"/>
+      <c r="C48" s="140"/>
+      <c r="D48" s="150"/>
+      <c r="E48" s="152" t="s">
         <v>109</v>
       </c>
       <c r="F48" s="58" t="s">
@@ -40209,28 +40301,28 @@
       </c>
     </row>
     <row r="49" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B49" s="115"/>
-      <c r="C49" s="112"/>
-      <c r="D49" s="125"/>
-      <c r="E49" s="127"/>
+      <c r="B49" s="143"/>
+      <c r="C49" s="140"/>
+      <c r="D49" s="150"/>
+      <c r="E49" s="152"/>
       <c r="F49" s="59" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B50" s="115"/>
-      <c r="C50" s="112"/>
-      <c r="D50" s="125"/>
-      <c r="E50" s="127"/>
+      <c r="B50" s="143"/>
+      <c r="C50" s="140"/>
+      <c r="D50" s="150"/>
+      <c r="E50" s="152"/>
       <c r="F50" s="59" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B51" s="116"/>
-      <c r="C51" s="113"/>
-      <c r="D51" s="126"/>
-      <c r="E51" s="128"/>
+      <c r="B51" s="144"/>
+      <c r="C51" s="141"/>
+      <c r="D51" s="151"/>
+      <c r="E51" s="153"/>
       <c r="F51" s="60" t="s">
         <v>99</v>
       </c>
@@ -40239,7 +40331,7 @@
       <c r="B52" s="94"/>
       <c r="C52" s="95"/>
       <c r="D52" s="96" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E52" s="102" t="s">
         <v>13</v>
@@ -40247,16 +40339,16 @@
       <c r="F52" s="103"/>
     </row>
     <row r="53" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B53" s="115">
+      <c r="B53" s="143">
         <v>10</v>
       </c>
-      <c r="C53" s="119" t="s">
+      <c r="C53" s="147" t="s">
         <v>117</v>
       </c>
-      <c r="D53" s="117" t="s">
+      <c r="D53" s="145" t="s">
         <v>126</v>
       </c>
-      <c r="E53" s="121" t="s">
+      <c r="E53" s="136" t="s">
         <v>118</v>
       </c>
       <c r="F53" s="62" t="s">
@@ -40264,78 +40356,78 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B54" s="115"/>
-      <c r="C54" s="119"/>
-      <c r="D54" s="117"/>
-      <c r="E54" s="121"/>
+      <c r="B54" s="143"/>
+      <c r="C54" s="147"/>
+      <c r="D54" s="145"/>
+      <c r="E54" s="136"/>
       <c r="F54" s="62" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B55" s="115"/>
-      <c r="C55" s="119"/>
-      <c r="D55" s="117"/>
-      <c r="E55" s="121"/>
+      <c r="B55" s="143"/>
+      <c r="C55" s="147"/>
+      <c r="D55" s="145"/>
+      <c r="E55" s="136"/>
       <c r="F55" s="63" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B56" s="115"/>
-      <c r="C56" s="119"/>
-      <c r="D56" s="117"/>
-      <c r="E56" s="121"/>
+      <c r="B56" s="143"/>
+      <c r="C56" s="147"/>
+      <c r="D56" s="145"/>
+      <c r="E56" s="136"/>
       <c r="F56" s="62" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="57" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B57" s="116"/>
-      <c r="C57" s="120"/>
-      <c r="D57" s="118"/>
-      <c r="E57" s="122"/>
+      <c r="B57" s="144"/>
+      <c r="C57" s="148"/>
+      <c r="D57" s="146"/>
+      <c r="E57" s="149"/>
       <c r="F57" s="62" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="58" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B58" s="33"/>
-      <c r="C58" s="111" t="s">
+      <c r="C58" s="121" t="s">
+        <v>201</v>
+      </c>
+      <c r="D58" s="72" t="s">
+        <v>202</v>
+      </c>
+      <c r="E58" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="D58" s="72" t="s">
-        <v>206</v>
+      <c r="F58" s="37" t="s">
+        <v>204</v>
       </c>
-      <c r="E58" s="36" t="s">
-        <v>209</v>
-      </c>
-      <c r="F58" s="37" t="s">
+      <c r="G58" s="120" t="s">
         <v>208</v>
-      </c>
-      <c r="G58" s="153" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="59" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B59" s="33"/>
-      <c r="C59" s="132"/>
+      <c r="C59" s="122"/>
       <c r="D59" s="72" t="s">
+        <v>203</v>
+      </c>
+      <c r="E59" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="F59" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="E59" s="36" t="s">
-        <v>210</v>
-      </c>
-      <c r="F59" s="37" t="s">
-        <v>211</v>
-      </c>
-      <c r="G59" s="153"/>
+      <c r="G59" s="120"/>
     </row>
     <row r="60" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B60" s="94"/>
       <c r="C60" s="95"/>
       <c r="D60" s="96" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E60" s="97"/>
       <c r="F60" s="14"/>
@@ -40344,24 +40436,24 @@
     <row r="61" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B61" s="94"/>
       <c r="C61" s="95" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
-      <c r="D61" s="154" t="s">
-        <v>230</v>
+      <c r="D61" s="123" t="s">
+        <v>226</v>
       </c>
       <c r="E61" s="97"/>
       <c r="F61" s="14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G61" s="91"/>
     </row>
     <row r="62" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B62" s="94"/>
       <c r="C62" s="95"/>
-      <c r="D62" s="134"/>
+      <c r="D62" s="124"/>
       <c r="E62" s="97"/>
       <c r="F62" s="14" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G62" s="91"/>
     </row>
@@ -40389,10 +40481,10 @@
       <c r="F65" s="50"/>
     </row>
     <row r="66" spans="2:7" s="90" customFormat="1" ht="45.75" customHeight="1">
-      <c r="G66" s="153"/>
+      <c r="G66" s="120"/>
     </row>
     <row r="67" spans="2:7" s="90" customFormat="1" ht="45.75" customHeight="1">
-      <c r="G67" s="153"/>
+      <c r="G67" s="120"/>
     </row>
     <row r="68" spans="2:7" s="90" customFormat="1" ht="43.5" customHeight="1">
       <c r="G68" s="91"/>
@@ -40453,14 +40545,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="C12:C19"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="C36:C51"/>
+    <mergeCell ref="B36:B51"/>
+    <mergeCell ref="D53:D57"/>
+    <mergeCell ref="C53:C57"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="E53:E57"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="D37:D46"/>
+    <mergeCell ref="D47:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="D7:D11"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C31:C33"/>
     <mergeCell ref="D31:D32"/>
@@ -40477,22 +40577,14 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D12:D19"/>
     <mergeCell ref="E7:E11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="C36:C51"/>
-    <mergeCell ref="B36:B51"/>
-    <mergeCell ref="D53:D57"/>
-    <mergeCell ref="C53:C57"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="E53:E57"/>
-    <mergeCell ref="E37:E40"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="D37:D46"/>
-    <mergeCell ref="D47:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="C12:C19"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D61:D62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="28" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40522,12 +40614,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="30.75">
-      <c r="B2" s="155" t="s">
+      <c r="B2" s="164" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -40566,16 +40658,16 @@
       <c r="C6" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="162" t="s">
+      <c r="D6" s="160" t="s">
         <v>137</v>
       </c>
-      <c r="E6" s="163"/>
+      <c r="E6" s="161"/>
     </row>
     <row r="7" spans="2:13" ht="23.25" customHeight="1">
-      <c r="B7" s="164" t="s">
+      <c r="B7" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="167" t="s">
+      <c r="C7" s="168" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="16" t="s">
@@ -40585,12 +40677,12 @@
         <v>55</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="2:13">
-      <c r="B8" s="165"/>
-      <c r="C8" s="168"/>
+      <c r="B8" s="166"/>
+      <c r="C8" s="169"/>
       <c r="D8" s="16" t="s">
         <v>61</v>
       </c>
@@ -40599,8 +40691,8 @@
       </c>
     </row>
     <row r="9" spans="2:13">
-      <c r="B9" s="165"/>
-      <c r="C9" s="168"/>
+      <c r="B9" s="166"/>
+      <c r="C9" s="169"/>
       <c r="D9" s="16" t="s">
         <v>60</v>
       </c>
@@ -40609,30 +40701,30 @@
       </c>
     </row>
     <row r="10" spans="2:13">
-      <c r="B10" s="165"/>
-      <c r="C10" s="168"/>
+      <c r="B10" s="166"/>
+      <c r="C10" s="169"/>
       <c r="D10" s="16" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="2:13">
-      <c r="B11" s="165"/>
-      <c r="C11" s="168"/>
+      <c r="B11" s="166"/>
+      <c r="C11" s="169"/>
       <c r="D11" s="16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:13">
-      <c r="B12" s="166"/>
-      <c r="C12" s="169"/>
+      <c r="B12" s="167"/>
+      <c r="C12" s="170"/>
       <c r="D12" s="16" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>55</v>
@@ -40667,16 +40759,16 @@
       <c r="C17" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="162" t="s">
+      <c r="D17" s="160" t="s">
         <v>134</v>
       </c>
-      <c r="E17" s="163"/>
+      <c r="E17" s="161"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="160" t="s">
+      <c r="B18" s="162" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="161" t="s">
+      <c r="C18" s="163" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="16" t="s">
@@ -40687,8 +40779,8 @@
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="160"/>
-      <c r="C19" s="161"/>
+      <c r="B19" s="162"/>
+      <c r="C19" s="163"/>
       <c r="D19" s="16" t="s">
         <v>58</v>
       </c>
@@ -40697,8 +40789,8 @@
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="160"/>
-      <c r="C20" s="161"/>
+      <c r="B20" s="162"/>
+      <c r="C20" s="163"/>
       <c r="D20" s="16" t="s">
         <v>59</v>
       </c>
@@ -40707,10 +40799,10 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="160"/>
-      <c r="C21" s="161"/>
+      <c r="B21" s="162"/>
+      <c r="C21" s="163"/>
       <c r="D21" s="16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>55</v>
@@ -40745,16 +40837,16 @@
       <c r="C26" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="162" t="s">
+      <c r="D26" s="160" t="s">
         <v>140</v>
       </c>
-      <c r="E26" s="163"/>
+      <c r="E26" s="161"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="160" t="s">
+      <c r="B27" s="162" t="s">
         <v>138</v>
       </c>
-      <c r="C27" s="161" t="s">
+      <c r="C27" s="163" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="16" t="s">
@@ -40765,8 +40857,8 @@
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="160"/>
-      <c r="C28" s="161"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="163"/>
       <c r="D28" s="16" t="s">
         <v>64</v>
       </c>
@@ -40775,16 +40867,16 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="160"/>
-      <c r="C29" s="161"/>
+      <c r="B29" s="162"/>
+      <c r="C29" s="163"/>
       <c r="D29" s="16" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="160"/>
-      <c r="C30" s="161"/>
+      <c r="B30" s="162"/>
+      <c r="C30" s="163"/>
       <c r="D30" s="16" t="s">
         <v>65</v>
       </c>
@@ -40821,16 +40913,16 @@
       <c r="C34" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D34" s="162" t="s">
+      <c r="D34" s="160" t="s">
         <v>130</v>
       </c>
-      <c r="E34" s="163"/>
+      <c r="E34" s="161"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="160" t="s">
+      <c r="B35" s="162" t="s">
         <v>128</v>
       </c>
-      <c r="C35" s="161" t="s">
+      <c r="C35" s="163" t="s">
         <v>53</v>
       </c>
       <c r="D35" s="16" t="s">
@@ -40841,8 +40933,8 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="160"/>
-      <c r="C36" s="161"/>
+      <c r="B36" s="162"/>
+      <c r="C36" s="163"/>
       <c r="D36" s="16" t="s">
         <v>58</v>
       </c>
@@ -40851,18 +40943,18 @@
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="160"/>
-      <c r="C37" s="161"/>
+      <c r="B37" s="162"/>
+      <c r="C37" s="163"/>
       <c r="D37" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="160"/>
-      <c r="C38" s="161"/>
+      <c r="B38" s="162"/>
+      <c r="C38" s="163"/>
       <c r="D38" s="16" t="s">
         <v>131</v>
       </c>
@@ -40872,18 +40964,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D26:E26"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -40897,6 +40977,18 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="C7:C12"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40949,10 +41041,10 @@
     </row>
     <row r="6" spans="1:5" s="5" customFormat="1" ht="23.25" customHeight="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="164" t="s">
+      <c r="B6" s="165" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="167" t="s">
+      <c r="C6" s="168" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="16" t="s">
@@ -40964,8 +41056,8 @@
     </row>
     <row r="7" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="165"/>
-      <c r="C7" s="168"/>
+      <c r="B7" s="166"/>
+      <c r="C7" s="169"/>
       <c r="D7" s="16" t="s">
         <v>61</v>
       </c>
@@ -40975,8 +41067,8 @@
     </row>
     <row r="8" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="165"/>
-      <c r="C8" s="168"/>
+      <c r="B8" s="166"/>
+      <c r="C8" s="169"/>
       <c r="D8" s="16" t="s">
         <v>60</v>
       </c>
@@ -40986,28 +41078,28 @@
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="165"/>
-      <c r="C9" s="168"/>
+      <c r="B9" s="166"/>
+      <c r="C9" s="169"/>
       <c r="D9" s="16" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="165"/>
-      <c r="C10" s="168"/>
+      <c r="B10" s="166"/>
+      <c r="C10" s="169"/>
       <c r="D10" s="16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="166"/>
-      <c r="C11" s="169"/>
+      <c r="B11" s="167"/>
+      <c r="C11" s="170"/>
       <c r="D11" s="16" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E11" s="19"/>
     </row>
@@ -41125,16 +41217,16 @@
       <c r="C27" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="162" t="s">
+      <c r="D27" s="160" t="s">
         <v>134</v>
       </c>
-      <c r="E27" s="163"/>
+      <c r="E27" s="161"/>
     </row>
     <row r="28" spans="1:5" ht="23.25" customHeight="1">
-      <c r="B28" s="160" t="s">
+      <c r="B28" s="162" t="s">
         <v>132</v>
       </c>
-      <c r="C28" s="161" t="s">
+      <c r="C28" s="163" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="16" t="s">
@@ -41143,42 +41235,42 @@
       <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:5" ht="23.25">
-      <c r="B29" s="160"/>
-      <c r="C29" s="161"/>
+      <c r="B29" s="162"/>
+      <c r="C29" s="163"/>
       <c r="D29" s="16" t="s">
         <v>58</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:5" ht="23.25">
-      <c r="B30" s="160"/>
-      <c r="C30" s="161"/>
+      <c r="B30" s="162"/>
+      <c r="C30" s="163"/>
       <c r="D30" s="16" t="s">
         <v>59</v>
       </c>
       <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5" ht="23.25">
-      <c r="B31" s="160"/>
-      <c r="C31" s="161"/>
+      <c r="B31" s="162"/>
+      <c r="C31" s="163"/>
       <c r="D31" s="16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E31" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="B6:B11"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="C28:C31"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B6:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -41215,46 +41307,46 @@
     </row>
     <row r="3" spans="1:26">
       <c r="S3" s="67"/>
-      <c r="T3" s="172" t="s">
+      <c r="T3" s="173" t="s">
         <v>81</v>
       </c>
-      <c r="U3" s="172"/>
-      <c r="V3" s="172"/>
-      <c r="W3" s="172"/>
-      <c r="X3" s="172"/>
-      <c r="Y3" s="172"/>
+      <c r="U3" s="173"/>
+      <c r="V3" s="173"/>
+      <c r="W3" s="173"/>
+      <c r="X3" s="173"/>
+      <c r="Y3" s="173"/>
       <c r="Z3" s="68"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="173">
+      <c r="A4" s="174">
         <v>1</v>
       </c>
       <c r="S4" s="67"/>
-      <c r="T4" s="172"/>
-      <c r="U4" s="172"/>
-      <c r="V4" s="172"/>
-      <c r="W4" s="172"/>
-      <c r="X4" s="172"/>
-      <c r="Y4" s="172"/>
+      <c r="T4" s="173"/>
+      <c r="U4" s="173"/>
+      <c r="V4" s="173"/>
+      <c r="W4" s="173"/>
+      <c r="X4" s="173"/>
+      <c r="Y4" s="173"/>
       <c r="Z4" s="68"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="173"/>
+      <c r="A5" s="174"/>
       <c r="S5" s="67"/>
-      <c r="T5" s="170" t="s">
+      <c r="T5" s="171" t="s">
         <v>84</v>
       </c>
-      <c r="U5" s="170"/>
-      <c r="V5" s="170"/>
-      <c r="W5" s="171" t="s">
+      <c r="U5" s="171"/>
+      <c r="V5" s="171"/>
+      <c r="W5" s="172" t="s">
         <v>83</v>
       </c>
-      <c r="X5" s="170"/>
-      <c r="Y5" s="170"/>
+      <c r="X5" s="171"/>
+      <c r="Y5" s="171"/>
       <c r="Z5" s="68"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="173"/>
+      <c r="A6" s="174"/>
       <c r="S6" s="67"/>
       <c r="V6" t="s">
         <v>80</v>
@@ -41263,7 +41355,7 @@
       <c r="Z6" s="68"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="173"/>
+      <c r="A7" s="174"/>
       <c r="S7" s="67"/>
       <c r="W7" s="15"/>
       <c r="Y7" t="s">
@@ -41272,13 +41364,13 @@
       <c r="Z7" s="68"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="173"/>
+      <c r="A8" s="174"/>
       <c r="S8" s="67"/>
       <c r="W8" s="15"/>
       <c r="Z8" s="68"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="173"/>
+      <c r="A9" s="174"/>
       <c r="S9" s="67"/>
       <c r="V9" t="s">
         <v>82</v>
@@ -41287,13 +41379,13 @@
       <c r="Z9" s="68"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="173"/>
+      <c r="A10" s="174"/>
       <c r="S10" s="67"/>
       <c r="W10" s="15"/>
       <c r="Z10" s="68"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="173"/>
+      <c r="A11" s="174"/>
       <c r="S11" s="67"/>
       <c r="W11" s="15"/>
       <c r="Z11" s="68"/>
@@ -41379,186 +41471,186 @@
       <c r="Z25" s="71"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="173">
+      <c r="A36" s="174">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="173"/>
+      <c r="A37" s="174"/>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="173"/>
+      <c r="A38" s="174"/>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="173"/>
+      <c r="A39" s="174"/>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="173"/>
+      <c r="A40" s="174"/>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="173"/>
+      <c r="A41" s="174"/>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="173"/>
+      <c r="A42" s="174"/>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="173"/>
+      <c r="A43" s="174"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="173">
+      <c r="A68" s="174">
         <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="173"/>
+      <c r="A69" s="174"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="173"/>
+      <c r="A70" s="174"/>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="173"/>
+      <c r="A71" s="174"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="173"/>
+      <c r="A72" s="174"/>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="173"/>
+      <c r="A73" s="174"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="173"/>
+      <c r="A74" s="174"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="173"/>
+      <c r="A75" s="174"/>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="173">
+      <c r="A100" s="174">
         <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="173"/>
+      <c r="A101" s="174"/>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="173"/>
+      <c r="A102" s="174"/>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="173"/>
+      <c r="A103" s="174"/>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="173"/>
+      <c r="A104" s="174"/>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="173"/>
+      <c r="A105" s="174"/>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="173"/>
+      <c r="A106" s="174"/>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="173"/>
+      <c r="A107" s="174"/>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="173">
+      <c r="A132" s="174">
         <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:1">
-      <c r="A133" s="173"/>
+      <c r="A133" s="174"/>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="173"/>
+      <c r="A134" s="174"/>
     </row>
     <row r="135" spans="1:1">
-      <c r="A135" s="173"/>
+      <c r="A135" s="174"/>
     </row>
     <row r="136" spans="1:1">
-      <c r="A136" s="173"/>
+      <c r="A136" s="174"/>
     </row>
     <row r="137" spans="1:1">
-      <c r="A137" s="173"/>
+      <c r="A137" s="174"/>
     </row>
     <row r="138" spans="1:1">
-      <c r="A138" s="173"/>
+      <c r="A138" s="174"/>
     </row>
     <row r="139" spans="1:1">
-      <c r="A139" s="173"/>
+      <c r="A139" s="174"/>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="173">
+      <c r="A164" s="174">
         <v>6</v>
       </c>
     </row>
     <row r="165" spans="1:1">
-      <c r="A165" s="173"/>
+      <c r="A165" s="174"/>
     </row>
     <row r="166" spans="1:1">
-      <c r="A166" s="173"/>
+      <c r="A166" s="174"/>
     </row>
     <row r="167" spans="1:1">
-      <c r="A167" s="173"/>
+      <c r="A167" s="174"/>
     </row>
     <row r="168" spans="1:1">
-      <c r="A168" s="173"/>
+      <c r="A168" s="174"/>
     </row>
     <row r="169" spans="1:1">
-      <c r="A169" s="173"/>
+      <c r="A169" s="174"/>
     </row>
     <row r="170" spans="1:1">
-      <c r="A170" s="173"/>
+      <c r="A170" s="174"/>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" s="173"/>
+      <c r="A171" s="174"/>
     </row>
     <row r="196" spans="1:1">
-      <c r="A196" s="173">
+      <c r="A196" s="174">
         <v>7</v>
       </c>
     </row>
     <row r="197" spans="1:1">
-      <c r="A197" s="173"/>
+      <c r="A197" s="174"/>
     </row>
     <row r="198" spans="1:1">
-      <c r="A198" s="173"/>
+      <c r="A198" s="174"/>
     </row>
     <row r="199" spans="1:1">
-      <c r="A199" s="173"/>
+      <c r="A199" s="174"/>
     </row>
     <row r="200" spans="1:1">
-      <c r="A200" s="173"/>
+      <c r="A200" s="174"/>
     </row>
     <row r="201" spans="1:1">
-      <c r="A201" s="173"/>
+      <c r="A201" s="174"/>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" s="173"/>
+      <c r="A202" s="174"/>
     </row>
     <row r="203" spans="1:1">
-      <c r="A203" s="173"/>
+      <c r="A203" s="174"/>
     </row>
     <row r="228" spans="1:1">
-      <c r="A228" s="173">
+      <c r="A228" s="174">
         <v>8</v>
       </c>
     </row>
     <row r="229" spans="1:1">
-      <c r="A229" s="173"/>
+      <c r="A229" s="174"/>
     </row>
     <row r="230" spans="1:1">
-      <c r="A230" s="173"/>
+      <c r="A230" s="174"/>
     </row>
     <row r="231" spans="1:1">
-      <c r="A231" s="173"/>
+      <c r="A231" s="174"/>
     </row>
     <row r="232" spans="1:1">
-      <c r="A232" s="173"/>
+      <c r="A232" s="174"/>
     </row>
     <row r="233" spans="1:1">
-      <c r="A233" s="173"/>
+      <c r="A233" s="174"/>
     </row>
     <row r="234" spans="1:1">
-      <c r="A234" s="173"/>
+      <c r="A234" s="174"/>
     </row>
     <row r="235" spans="1:1">
-      <c r="A235" s="173"/>
+      <c r="A235" s="174"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -41605,62 +41697,62 @@
   </cols>
   <sheetData>
     <row r="70" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="C70" s="174" t="s">
-        <v>183</v>
+      <c r="C70" s="175" t="s">
+        <v>179</v>
       </c>
-      <c r="D70" s="174" t="s">
+      <c r="D70" s="175" t="s">
+        <v>164</v>
+      </c>
+      <c r="E70" s="175" t="s">
+        <v>163</v>
+      </c>
+      <c r="F70" s="178" t="s">
+        <v>169</v>
+      </c>
+      <c r="G70" s="175" t="s">
+        <v>162</v>
+      </c>
+      <c r="H70" s="175" t="s">
         <v>168</v>
       </c>
-      <c r="E70" s="174" t="s">
+      <c r="I70" s="175"/>
+      <c r="J70" s="175" t="s">
+        <v>3</v>
+      </c>
+      <c r="K70" s="175"/>
+      <c r="L70" s="175"/>
+      <c r="M70" s="175"/>
+    </row>
+    <row r="71" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
+      <c r="C71" s="175"/>
+      <c r="D71" s="175"/>
+      <c r="E71" s="175"/>
+      <c r="F71" s="175"/>
+      <c r="G71" s="175"/>
+      <c r="H71" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="F70" s="177" t="s">
-        <v>173</v>
+      <c r="I71" s="75" t="s">
+        <v>159</v>
       </c>
-      <c r="G70" s="174" t="s">
+      <c r="J71" s="74" t="s">
         <v>166</v>
       </c>
-      <c r="H70" s="174" t="s">
-        <v>172</v>
-      </c>
-      <c r="I70" s="174"/>
-      <c r="J70" s="174" t="s">
-        <v>3</v>
-      </c>
-      <c r="K70" s="174"/>
-      <c r="L70" s="174"/>
-      <c r="M70" s="174"/>
-    </row>
-    <row r="71" spans="3:13" s="2" customFormat="1" ht="45.75" customHeight="1">
-      <c r="C71" s="174"/>
-      <c r="D71" s="174"/>
-      <c r="E71" s="174"/>
-      <c r="F71" s="174"/>
-      <c r="G71" s="174"/>
-      <c r="H71" s="74" t="s">
-        <v>171</v>
-      </c>
-      <c r="I71" s="75" t="s">
-        <v>163</v>
-      </c>
-      <c r="J71" s="74" t="s">
-        <v>170</v>
-      </c>
       <c r="K71" s="74" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="L71" s="74" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="M71" s="83" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="72" spans="3:13" s="2" customFormat="1" ht="151.5" customHeight="1">
-      <c r="C72" s="175" t="s">
-        <v>199</v>
+      <c r="C72" s="176" t="s">
+        <v>195</v>
       </c>
-      <c r="D72" s="176"/>
+      <c r="D72" s="177"/>
       <c r="E72" s="76"/>
       <c r="F72" s="77"/>
       <c r="G72" s="77"/>
@@ -41671,113 +41763,113 @@
     </row>
     <row r="73" spans="3:13" s="2" customFormat="1" ht="139.5">
       <c r="C73" s="88" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E73" s="76" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F73" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="G73" s="77" t="s">
+        <v>172</v>
+      </c>
+      <c r="H73" s="78" t="s">
+        <v>173</v>
+      </c>
+      <c r="I73" s="79" t="s">
+        <v>174</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L73" s="80" t="s">
         <v>175</v>
       </c>
-      <c r="G73" s="77" t="s">
-        <v>176</v>
-      </c>
-      <c r="H73" s="78" t="s">
-        <v>177</v>
-      </c>
-      <c r="I73" s="79" t="s">
-        <v>178</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="L73" s="80" t="s">
-        <v>179</v>
-      </c>
       <c r="M73" s="84" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="D74" s="81" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G74" s="77" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="L74" s="80" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="M74" s="84" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="75" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C75" s="87" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="M75" s="85"/>
     </row>
     <row r="76" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="D76" s="81" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="M76" s="85"/>
     </row>
     <row r="77" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="D77" s="81" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="M77" s="85"/>
     </row>
     <row r="78" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C78" s="82" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="M78" s="85"/>
     </row>
     <row r="79" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C79" s="82" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="M79" s="85"/>
     </row>
     <row r="80" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C80" s="82" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="M80" s="85"/>
     </row>
     <row r="81" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C81" s="82" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="M81" s="85"/>
     </row>
     <row r="82" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C82" s="82" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="M82" s="85"/>
     </row>
     <row r="83" spans="3:13" s="2" customFormat="1" ht="201" customHeight="1">
       <c r="C83" s="82" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="M83" s="85"/>
     </row>

</xml_diff>

<commit_message>
I used memory hooks to optimize the performance of my app, and added some alerts after the various actions in my app
</commit_message>
<xml_diff>
--- a/Final-React-Project-Design.xlsx
+++ b/Final-React-Project-Design.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basheer\Desktop\בשיר\Full Stack Work\Full Stack Cors - YanivArad\Projects\React-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B93EC7-E3B2-47A9-9A9A-B4EB8CD326BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56C0E93-6794-408C-9044-14A5B843BD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="970" xr2:uid="{6C9ACC65-0954-4C83-9435-0755A94AE81B}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="250">
   <si>
     <t>Num</t>
   </si>
@@ -4929,9 +4929,6 @@
     <t>18/11/23</t>
   </si>
   <si>
-    <t>Improving the efficiency of the application</t>
-  </si>
-  <si>
     <t>28/11/23</t>
   </si>
   <si>
@@ -5183,16 +5180,10 @@
     <t>Improve and Sync between the external DB [Firebase] and the internal DB [redux]</t>
   </si>
   <si>
-    <t>I will add a dashboard page that gives the possibility to manage the necessary data</t>
-  </si>
-  <si>
     <t>5-7/12/2023</t>
   </si>
   <si>
     <t>8-9/12/2023</t>
-  </si>
-  <si>
-    <t>10-11/12/2023</t>
   </si>
   <si>
     <t>Authentication to Firebase with email and password</t>
@@ -5389,7 +5380,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Step 15</t>
+      <t>Step 16</t>
     </r>
     <r>
       <rPr>
@@ -5399,48 +5390,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - Build dashboard page - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Optionally</t>
+      <t xml:space="preserve"> - Tests</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Step 16</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Tests</t>
-    </r>
+    <t>Used memoization hooks for optimizing the performance of my app</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="65">
+  <fonts count="64">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5862,13 +5823,6 @@
       <color rgb="FF6F42C1"/>
       <name val="Courier New"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -6801,95 +6755,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6918,7 +6791,16 @@
     <xf numFmtId="0" fontId="47" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6933,11 +6815,86 @@
     <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6951,19 +6908,16 @@
     <xf numFmtId="0" fontId="25" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -39309,10 +39263,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="B1:F31"/>
+  <dimension ref="B1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15"/>
@@ -39461,7 +39415,7 @@
         <v>143</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>124</v>
@@ -39478,7 +39432,7 @@
         <v>144</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>124</v>
@@ -39495,7 +39449,7 @@
         <v>145</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>124</v>
@@ -39512,7 +39466,7 @@
         <v>142</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>124</v>
@@ -39529,7 +39483,7 @@
         <v>151</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>124</v>
@@ -39546,7 +39500,7 @@
         <v>152</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>124</v>
@@ -39563,7 +39517,7 @@
         <v>153</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>124</v>
@@ -39574,13 +39528,13 @@
         <v>13</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D18" s="46" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>124</v>
@@ -39591,13 +39545,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>124</v>
@@ -39608,13 +39562,13 @@
         <v>15</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D20" s="46" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>124</v>
@@ -39625,13 +39579,13 @@
         <v>16</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>124</v>
@@ -39642,13 +39596,13 @@
         <v>17</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D22" s="46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E22" s="46" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>124</v>
@@ -39659,79 +39613,70 @@
         <v>18</v>
       </c>
       <c r="C23" s="46" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D23" s="46" t="s">
         <v>157</v>
       </c>
       <c r="E23" s="104" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" ht="30">
       <c r="B24" s="46">
         <v>19</v>
       </c>
       <c r="C24" s="46" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D24" s="46" t="s">
-        <v>215</v>
+        <v>249</v>
       </c>
       <c r="E24" s="104" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="25" spans="2:6" ht="30">
+    <row r="25" spans="2:6">
       <c r="B25" s="46">
         <v>20</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D25" s="46" t="s">
-        <v>232</v>
-      </c>
-      <c r="E25" s="104" t="s">
-        <v>235</v>
-      </c>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="B26" s="46">
-        <v>21</v>
-      </c>
-      <c r="C26" s="46" t="s">
-        <v>252</v>
-      </c>
-      <c r="D26" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="E26" s="104">
+      <c r="E25" s="104">
         <v>45272</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="27" spans="2:6" ht="37.5">
-      <c r="C27" s="89" t="s">
+    <row r="26" spans="2:6" ht="37.5">
+      <c r="C26" s="89" t="s">
         <v>196</v>
       </c>
-      <c r="D27" s="105" t="s">
+      <c r="D26" s="105" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="37.5">
-      <c r="C29" s="89" t="s">
+    <row r="28" spans="2:6" ht="37.5">
+      <c r="C28" s="89" t="s">
         <v>198</v>
       </c>
-      <c r="D29" s="105" t="s">
+      <c r="D28" s="105" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="37.5">
-      <c r="D31" s="105" t="s">
+    <row r="30" spans="2:6" ht="37.5">
+      <c r="D30" s="105" t="s">
         <v>200</v>
       </c>
     </row>
@@ -39745,14 +39690,14 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="E4:E5"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6:F26">
+  <conditionalFormatting sqref="F6:F25">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="V">
       <formula>NOT(ISERROR(SEARCH("V",F6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C27" r:id="rId1" xr:uid="{B5AF2755-436A-4008-9BA4-CBBB84CC1736}"/>
-    <hyperlink ref="C29" r:id="rId2" xr:uid="{3D76CBC8-DA15-470A-8E1E-DBBC4061AE14}"/>
+    <hyperlink ref="C26" r:id="rId1" xr:uid="{B5AF2755-436A-4008-9BA4-CBBB84CC1736}"/>
+    <hyperlink ref="C28" r:id="rId2" xr:uid="{3D76CBC8-DA15-470A-8E1E-DBBC4061AE14}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
@@ -39782,36 +39727,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="51.75" customHeight="1">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="110" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" thickBot="1">
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B4" s="125" t="s">
+      <c r="B4" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="118" t="s">
+      <c r="C4" s="149" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="118" t="s">
+      <c r="D4" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="118" t="s">
+      <c r="E4" s="149" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="133"/>
+      <c r="F4" s="150"/>
     </row>
     <row r="5" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B5" s="126"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
+      <c r="B5" s="137"/>
+      <c r="C5" s="152"/>
+      <c r="D5" s="152"/>
       <c r="E5" s="31" t="s">
         <v>9</v>
       </c>
@@ -39820,10 +39765,10 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B6" s="142">
+      <c r="B6" s="115">
         <v>1</v>
       </c>
-      <c r="C6" s="121" t="s">
+      <c r="C6" s="112" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="73" t="s">
@@ -39837,63 +39782,63 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B7" s="143"/>
-      <c r="C7" s="140"/>
-      <c r="D7" s="112" t="s">
+      <c r="B7" s="116"/>
+      <c r="C7" s="113"/>
+      <c r="D7" s="125" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" s="124" t="s">
+        <v>222</v>
+      </c>
+      <c r="F7" s="99" t="s">
         <v>218</v>
       </c>
-      <c r="E7" s="135" t="s">
-        <v>223</v>
-      </c>
-      <c r="F7" s="99" t="s">
+    </row>
+    <row r="8" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B8" s="116"/>
+      <c r="C8" s="113"/>
+      <c r="D8" s="126"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="99" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B8" s="143"/>
-      <c r="C8" s="140"/>
-      <c r="D8" s="150"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="99" t="s">
+    <row r="9" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B9" s="116"/>
+      <c r="C9" s="113"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="99" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B9" s="143"/>
-      <c r="C9" s="140"/>
-      <c r="D9" s="150"/>
-      <c r="E9" s="136"/>
-      <c r="F9" s="99" t="s">
+    <row r="10" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B10" s="116"/>
+      <c r="C10" s="113"/>
+      <c r="D10" s="126"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="100"/>
+    </row>
+    <row r="11" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
+      <c r="B11" s="134"/>
+      <c r="C11" s="133"/>
+      <c r="D11" s="135"/>
+      <c r="E11" s="153"/>
+      <c r="F11" s="101" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B10" s="143"/>
-      <c r="C10" s="140"/>
-      <c r="D10" s="150"/>
-      <c r="E10" s="136"/>
-      <c r="F10" s="100"/>
-    </row>
-    <row r="11" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B11" s="155"/>
-      <c r="C11" s="122"/>
-      <c r="D11" s="124"/>
-      <c r="E11" s="137"/>
-      <c r="F11" s="101" t="s">
-        <v>222</v>
-      </c>
-    </row>
     <row r="12" spans="2:6" ht="22.5">
-      <c r="B12" s="129">
+      <c r="B12" s="130">
         <v>2</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="138" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="110" t="s">
+      <c r="D12" s="146" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="116" t="s">
+      <c r="E12" s="143" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="38" t="s">
@@ -39901,63 +39846,63 @@
       </c>
     </row>
     <row r="13" spans="2:6" ht="22.5">
-      <c r="B13" s="130"/>
-      <c r="C13" s="114"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="117"/>
+      <c r="B13" s="131"/>
+      <c r="C13" s="139"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="144"/>
       <c r="F13" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="22.5">
-      <c r="B14" s="130"/>
-      <c r="C14" s="114"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="117"/>
+      <c r="B14" s="131"/>
+      <c r="C14" s="139"/>
+      <c r="D14" s="147"/>
+      <c r="E14" s="144"/>
       <c r="F14" s="21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="22.5">
-      <c r="B15" s="130"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="111"/>
-      <c r="E15" s="117"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="139"/>
+      <c r="D15" s="147"/>
+      <c r="E15" s="144"/>
       <c r="F15" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="22.5">
-      <c r="B16" s="130"/>
-      <c r="C16" s="114"/>
-      <c r="D16" s="111"/>
-      <c r="E16" s="117"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="139"/>
+      <c r="D16" s="147"/>
+      <c r="E16" s="144"/>
       <c r="F16" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="22.5">
-      <c r="B17" s="130"/>
-      <c r="C17" s="114"/>
-      <c r="D17" s="111"/>
-      <c r="E17" s="117"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="147"/>
+      <c r="E17" s="144"/>
       <c r="F17" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="22.5">
-      <c r="B18" s="130"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="117"/>
+      <c r="B18" s="131"/>
+      <c r="C18" s="139"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="144"/>
       <c r="F18" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B19" s="131"/>
-      <c r="C19" s="115"/>
-      <c r="D19" s="132"/>
+      <c r="B19" s="145"/>
+      <c r="C19" s="140"/>
+      <c r="D19" s="148"/>
       <c r="E19" s="40" t="s">
         <v>13</v>
       </c>
@@ -39966,16 +39911,16 @@
       </c>
     </row>
     <row r="20" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B20" s="129">
+      <c r="B20" s="130">
         <v>3</v>
       </c>
-      <c r="C20" s="113" t="s">
+      <c r="C20" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="110" t="s">
+      <c r="D20" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="116" t="s">
+      <c r="E20" s="143" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="41" t="s">
@@ -39983,45 +39928,45 @@
       </c>
     </row>
     <row r="21" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B21" s="130"/>
-      <c r="C21" s="114"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="117"/>
+      <c r="B21" s="131"/>
+      <c r="C21" s="139"/>
+      <c r="D21" s="147"/>
+      <c r="E21" s="144"/>
       <c r="F21" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B22" s="130"/>
-      <c r="C22" s="114"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="117"/>
+      <c r="B22" s="131"/>
+      <c r="C22" s="139"/>
+      <c r="D22" s="147"/>
+      <c r="E22" s="144"/>
       <c r="F22" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B23" s="130"/>
-      <c r="C23" s="114"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="117"/>
+      <c r="B23" s="131"/>
+      <c r="C23" s="139"/>
+      <c r="D23" s="147"/>
+      <c r="E23" s="144"/>
       <c r="F23" s="26" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B24" s="130"/>
-      <c r="C24" s="114"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="117"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="139"/>
+      <c r="D24" s="147"/>
+      <c r="E24" s="144"/>
       <c r="F24" s="27" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B25" s="131"/>
-      <c r="C25" s="115"/>
-      <c r="D25" s="132"/>
+      <c r="B25" s="145"/>
+      <c r="C25" s="140"/>
+      <c r="D25" s="148"/>
       <c r="E25" s="40" t="s">
         <v>13</v>
       </c>
@@ -40030,16 +39975,16 @@
       </c>
     </row>
     <row r="26" spans="2:6" ht="22.5">
-      <c r="B26" s="129">
+      <c r="B26" s="130">
         <v>4</v>
       </c>
-      <c r="C26" s="113" t="s">
+      <c r="C26" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="110" t="s">
+      <c r="D26" s="146" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="116" t="s">
+      <c r="E26" s="143" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="41" t="s">
@@ -40047,27 +39992,27 @@
       </c>
     </row>
     <row r="27" spans="2:6" ht="22.5">
-      <c r="B27" s="130"/>
-      <c r="C27" s="114"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="117"/>
+      <c r="B27" s="131"/>
+      <c r="C27" s="139"/>
+      <c r="D27" s="147"/>
+      <c r="E27" s="144"/>
       <c r="F27" s="28" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="22.5">
-      <c r="B28" s="130"/>
-      <c r="C28" s="114"/>
-      <c r="D28" s="111"/>
-      <c r="E28" s="117"/>
+      <c r="B28" s="131"/>
+      <c r="C28" s="139"/>
+      <c r="D28" s="147"/>
+      <c r="E28" s="144"/>
       <c r="F28" s="29" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="42" customHeight="1" thickBot="1">
-      <c r="B29" s="154"/>
-      <c r="C29" s="134"/>
-      <c r="D29" s="112"/>
+      <c r="B29" s="132"/>
+      <c r="C29" s="151"/>
+      <c r="D29" s="125"/>
       <c r="E29" s="12" t="s">
         <v>13</v>
       </c>
@@ -40093,16 +40038,16 @@
       </c>
     </row>
     <row r="31" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B31" s="129">
+      <c r="B31" s="130">
         <v>6</v>
       </c>
-      <c r="C31" s="113" t="s">
+      <c r="C31" s="138" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="127" t="s">
+      <c r="D31" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="116" t="s">
+      <c r="E31" s="143" t="s">
         <v>13</v>
       </c>
       <c r="F31" s="41" t="s">
@@ -40110,17 +40055,17 @@
       </c>
     </row>
     <row r="32" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B32" s="130"/>
-      <c r="C32" s="114"/>
-      <c r="D32" s="128"/>
-      <c r="E32" s="117"/>
+      <c r="B32" s="131"/>
+      <c r="C32" s="139"/>
+      <c r="D32" s="142"/>
+      <c r="E32" s="144"/>
       <c r="F32" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="34.5" customHeight="1" thickBot="1">
-      <c r="B33" s="131"/>
-      <c r="C33" s="115"/>
+      <c r="B33" s="145"/>
+      <c r="C33" s="140"/>
       <c r="D33" s="39" t="s">
         <v>39</v>
       </c>
@@ -40164,10 +40109,10 @@
       </c>
     </row>
     <row r="36" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B36" s="142">
+      <c r="B36" s="115">
         <v>9</v>
       </c>
-      <c r="C36" s="121" t="s">
+      <c r="C36" s="112" t="s">
         <v>90</v>
       </c>
       <c r="D36" s="73" t="s">
@@ -40181,12 +40126,12 @@
       </c>
     </row>
     <row r="37" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B37" s="143"/>
-      <c r="C37" s="140"/>
-      <c r="D37" s="112" t="s">
+      <c r="B37" s="116"/>
+      <c r="C37" s="113"/>
+      <c r="D37" s="125" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="135" t="s">
+      <c r="E37" s="124" t="s">
         <v>96</v>
       </c>
       <c r="F37" s="55" t="s">
@@ -40194,37 +40139,37 @@
       </c>
     </row>
     <row r="38" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B38" s="143"/>
-      <c r="C38" s="140"/>
-      <c r="D38" s="150"/>
-      <c r="E38" s="136"/>
+      <c r="B38" s="116"/>
+      <c r="C38" s="113"/>
+      <c r="D38" s="126"/>
+      <c r="E38" s="122"/>
       <c r="F38" s="51" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B39" s="143"/>
-      <c r="C39" s="140"/>
-      <c r="D39" s="150"/>
-      <c r="E39" s="136"/>
+      <c r="B39" s="116"/>
+      <c r="C39" s="113"/>
+      <c r="D39" s="126"/>
+      <c r="E39" s="122"/>
       <c r="F39" s="51" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B40" s="143"/>
-      <c r="C40" s="140"/>
-      <c r="D40" s="150"/>
-      <c r="E40" s="149"/>
+      <c r="B40" s="116"/>
+      <c r="C40" s="113"/>
+      <c r="D40" s="126"/>
+      <c r="E40" s="123"/>
       <c r="F40" s="56" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B41" s="143"/>
-      <c r="C41" s="140"/>
-      <c r="D41" s="150"/>
-      <c r="E41" s="135" t="s">
+      <c r="B41" s="116"/>
+      <c r="C41" s="113"/>
+      <c r="D41" s="126"/>
+      <c r="E41" s="124" t="s">
         <v>98</v>
       </c>
       <c r="F41" s="57" t="s">
@@ -40232,54 +40177,54 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B42" s="143"/>
-      <c r="C42" s="140"/>
-      <c r="D42" s="150"/>
-      <c r="E42" s="136"/>
+      <c r="B42" s="116"/>
+      <c r="C42" s="113"/>
+      <c r="D42" s="126"/>
+      <c r="E42" s="122"/>
       <c r="F42" s="58" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B43" s="143"/>
-      <c r="C43" s="140"/>
-      <c r="D43" s="150"/>
-      <c r="E43" s="136"/>
+      <c r="B43" s="116"/>
+      <c r="C43" s="113"/>
+      <c r="D43" s="126"/>
+      <c r="E43" s="122"/>
       <c r="F43" s="58" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B44" s="143"/>
-      <c r="C44" s="140"/>
-      <c r="D44" s="150"/>
-      <c r="E44" s="136"/>
+      <c r="B44" s="116"/>
+      <c r="C44" s="113"/>
+      <c r="D44" s="126"/>
+      <c r="E44" s="122"/>
       <c r="F44" s="59" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B45" s="143"/>
-      <c r="C45" s="140"/>
-      <c r="D45" s="150"/>
-      <c r="E45" s="136"/>
+      <c r="B45" s="116"/>
+      <c r="C45" s="113"/>
+      <c r="D45" s="126"/>
+      <c r="E45" s="122"/>
       <c r="F45" s="59" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B46" s="143"/>
-      <c r="C46" s="140"/>
-      <c r="D46" s="151"/>
-      <c r="E46" s="149"/>
+      <c r="B46" s="116"/>
+      <c r="C46" s="113"/>
+      <c r="D46" s="127"/>
+      <c r="E46" s="123"/>
       <c r="F46" s="60" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="75">
-      <c r="B47" s="143"/>
-      <c r="C47" s="140"/>
-      <c r="D47" s="112" t="s">
+      <c r="B47" s="116"/>
+      <c r="C47" s="113"/>
+      <c r="D47" s="125" t="s">
         <v>97</v>
       </c>
       <c r="E47" s="10" t="s">
@@ -40290,10 +40235,10 @@
       </c>
     </row>
     <row r="48" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B48" s="143"/>
-      <c r="C48" s="140"/>
-      <c r="D48" s="150"/>
-      <c r="E48" s="152" t="s">
+      <c r="B48" s="116"/>
+      <c r="C48" s="113"/>
+      <c r="D48" s="126"/>
+      <c r="E48" s="128" t="s">
         <v>109</v>
       </c>
       <c r="F48" s="58" t="s">
@@ -40301,28 +40246,28 @@
       </c>
     </row>
     <row r="49" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B49" s="143"/>
-      <c r="C49" s="140"/>
-      <c r="D49" s="150"/>
-      <c r="E49" s="152"/>
+      <c r="B49" s="116"/>
+      <c r="C49" s="113"/>
+      <c r="D49" s="126"/>
+      <c r="E49" s="128"/>
       <c r="F49" s="59" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B50" s="143"/>
-      <c r="C50" s="140"/>
-      <c r="D50" s="150"/>
-      <c r="E50" s="152"/>
+      <c r="B50" s="116"/>
+      <c r="C50" s="113"/>
+      <c r="D50" s="126"/>
+      <c r="E50" s="128"/>
       <c r="F50" s="59" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B51" s="144"/>
-      <c r="C51" s="141"/>
-      <c r="D51" s="151"/>
-      <c r="E51" s="153"/>
+      <c r="B51" s="117"/>
+      <c r="C51" s="114"/>
+      <c r="D51" s="127"/>
+      <c r="E51" s="129"/>
       <c r="F51" s="60" t="s">
         <v>99</v>
       </c>
@@ -40331,7 +40276,7 @@
       <c r="B52" s="94"/>
       <c r="C52" s="95"/>
       <c r="D52" s="96" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E52" s="102" t="s">
         <v>13</v>
@@ -40339,16 +40284,16 @@
       <c r="F52" s="103"/>
     </row>
     <row r="53" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B53" s="143">
+      <c r="B53" s="116">
         <v>10</v>
       </c>
-      <c r="C53" s="147" t="s">
+      <c r="C53" s="120" t="s">
         <v>117</v>
       </c>
-      <c r="D53" s="145" t="s">
+      <c r="D53" s="118" t="s">
         <v>126</v>
       </c>
-      <c r="E53" s="136" t="s">
+      <c r="E53" s="122" t="s">
         <v>118</v>
       </c>
       <c r="F53" s="62" t="s">
@@ -40356,44 +40301,44 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B54" s="143"/>
-      <c r="C54" s="147"/>
-      <c r="D54" s="145"/>
-      <c r="E54" s="136"/>
+      <c r="B54" s="116"/>
+      <c r="C54" s="120"/>
+      <c r="D54" s="118"/>
+      <c r="E54" s="122"/>
       <c r="F54" s="62" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B55" s="143"/>
-      <c r="C55" s="147"/>
-      <c r="D55" s="145"/>
-      <c r="E55" s="136"/>
+      <c r="B55" s="116"/>
+      <c r="C55" s="120"/>
+      <c r="D55" s="118"/>
+      <c r="E55" s="122"/>
       <c r="F55" s="63" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B56" s="143"/>
-      <c r="C56" s="147"/>
-      <c r="D56" s="145"/>
-      <c r="E56" s="136"/>
+      <c r="B56" s="116"/>
+      <c r="C56" s="120"/>
+      <c r="D56" s="118"/>
+      <c r="E56" s="122"/>
       <c r="F56" s="62" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="57" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B57" s="144"/>
-      <c r="C57" s="148"/>
-      <c r="D57" s="146"/>
-      <c r="E57" s="149"/>
+      <c r="B57" s="117"/>
+      <c r="C57" s="121"/>
+      <c r="D57" s="119"/>
+      <c r="E57" s="123"/>
       <c r="F57" s="62" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="58" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B58" s="33"/>
-      <c r="C58" s="121" t="s">
+      <c r="C58" s="112" t="s">
         <v>201</v>
       </c>
       <c r="D58" s="72" t="s">
@@ -40405,13 +40350,13 @@
       <c r="F58" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="G58" s="120" t="s">
+      <c r="G58" s="154" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="59" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B59" s="33"/>
-      <c r="C59" s="122"/>
+      <c r="C59" s="133"/>
       <c r="D59" s="72" t="s">
         <v>203</v>
       </c>
@@ -40421,13 +40366,13 @@
       <c r="F59" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="G59" s="120"/>
+      <c r="G59" s="154"/>
     </row>
     <row r="60" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B60" s="94"/>
       <c r="C60" s="95"/>
       <c r="D60" s="96" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E60" s="97"/>
       <c r="F60" s="14"/>
@@ -40436,24 +40381,24 @@
     <row r="61" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B61" s="94"/>
       <c r="C61" s="95" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
-      <c r="D61" s="123" t="s">
-        <v>226</v>
+      <c r="D61" s="155" t="s">
+        <v>225</v>
       </c>
       <c r="E61" s="97"/>
       <c r="F61" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G61" s="91"/>
     </row>
     <row r="62" spans="2:7" ht="42.75" customHeight="1" thickBot="1">
       <c r="B62" s="94"/>
       <c r="C62" s="95"/>
-      <c r="D62" s="124"/>
+      <c r="D62" s="135"/>
       <c r="E62" s="97"/>
       <c r="F62" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G62" s="91"/>
     </row>
@@ -40481,10 +40426,10 @@
       <c r="F65" s="50"/>
     </row>
     <row r="66" spans="2:7" s="90" customFormat="1" ht="45.75" customHeight="1">
-      <c r="G66" s="120"/>
+      <c r="G66" s="154"/>
     </row>
     <row r="67" spans="2:7" s="90" customFormat="1" ht="45.75" customHeight="1">
-      <c r="G67" s="120"/>
+      <c r="G67" s="154"/>
     </row>
     <row r="68" spans="2:7" s="90" customFormat="1" ht="43.5" customHeight="1">
       <c r="G68" s="91"/>
@@ -40545,6 +40490,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="C12:C19"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="E12:E18"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D12:D19"/>
+    <mergeCell ref="E7:E11"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="C36:C51"/>
     <mergeCell ref="B36:B51"/>
@@ -40561,30 +40530,6 @@
     <mergeCell ref="C6:C11"/>
     <mergeCell ref="B6:B11"/>
     <mergeCell ref="D7:D11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="E20:E24"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="D20:D25"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="E12:E18"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D12:D19"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="C12:C19"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D61:D62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="28" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40614,12 +40559,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="30.75">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -40630,20 +40575,20 @@
       <c r="M2" s="4"/>
     </row>
     <row r="4" spans="2:13">
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="156" t="s">
+      <c r="C4" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="158" t="s">
+      <c r="D4" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="159"/>
+      <c r="E4" s="160"/>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="157"/>
-      <c r="C5" s="157"/>
+      <c r="B5" s="158"/>
+      <c r="C5" s="158"/>
       <c r="D5" s="17" t="s">
         <v>54</v>
       </c>
@@ -40658,10 +40603,10 @@
       <c r="C6" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="160" t="s">
+      <c r="D6" s="163" t="s">
         <v>137</v>
       </c>
-      <c r="E6" s="161"/>
+      <c r="E6" s="164"/>
     </row>
     <row r="7" spans="2:13" ht="23.25" customHeight="1">
       <c r="B7" s="165" t="s">
@@ -40731,20 +40676,20 @@
       </c>
     </row>
     <row r="15" spans="2:13">
-      <c r="B15" s="156" t="s">
+      <c r="B15" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="156" t="s">
+      <c r="C15" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="158" t="s">
+      <c r="D15" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="159"/>
+      <c r="E15" s="160"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
       <c r="D16" s="17" t="s">
         <v>54</v>
       </c>
@@ -40759,16 +40704,16 @@
       <c r="C17" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="160" t="s">
+      <c r="D17" s="163" t="s">
         <v>134</v>
       </c>
-      <c r="E17" s="161"/>
+      <c r="E17" s="164"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="162" t="s">
+      <c r="B18" s="161" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="163" t="s">
+      <c r="C18" s="162" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="16" t="s">
@@ -40779,8 +40724,8 @@
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="162"/>
-      <c r="C19" s="163"/>
+      <c r="B19" s="161"/>
+      <c r="C19" s="162"/>
       <c r="D19" s="16" t="s">
         <v>58</v>
       </c>
@@ -40789,8 +40734,8 @@
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="162"/>
-      <c r="C20" s="163"/>
+      <c r="B20" s="161"/>
+      <c r="C20" s="162"/>
       <c r="D20" s="16" t="s">
         <v>59</v>
       </c>
@@ -40799,8 +40744,8 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="162"/>
-      <c r="C21" s="163"/>
+      <c r="B21" s="161"/>
+      <c r="C21" s="162"/>
       <c r="D21" s="16" t="s">
         <v>210</v>
       </c>
@@ -40809,20 +40754,20 @@
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="156" t="s">
+      <c r="B24" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="156" t="s">
+      <c r="C24" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="158" t="s">
+      <c r="D24" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="159"/>
+      <c r="E24" s="160"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="157"/>
-      <c r="C25" s="157"/>
+      <c r="B25" s="158"/>
+      <c r="C25" s="158"/>
       <c r="D25" s="17" t="s">
         <v>54</v>
       </c>
@@ -40837,16 +40782,16 @@
       <c r="C26" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="160" t="s">
+      <c r="D26" s="163" t="s">
         <v>140</v>
       </c>
-      <c r="E26" s="161"/>
+      <c r="E26" s="164"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="162" t="s">
+      <c r="B27" s="161" t="s">
         <v>138</v>
       </c>
-      <c r="C27" s="163" t="s">
+      <c r="C27" s="162" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="16" t="s">
@@ -40857,8 +40802,8 @@
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
+      <c r="B28" s="161"/>
+      <c r="C28" s="162"/>
       <c r="D28" s="16" t="s">
         <v>64</v>
       </c>
@@ -40867,16 +40812,16 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="162"/>
-      <c r="C29" s="163"/>
+      <c r="B29" s="161"/>
+      <c r="C29" s="162"/>
       <c r="D29" s="16" t="s">
         <v>213</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="162"/>
-      <c r="C30" s="163"/>
+      <c r="B30" s="161"/>
+      <c r="C30" s="162"/>
       <c r="D30" s="16" t="s">
         <v>65</v>
       </c>
@@ -40885,20 +40830,20 @@
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="156" t="s">
+      <c r="B32" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="156" t="s">
+      <c r="C32" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="158" t="s">
+      <c r="D32" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="159"/>
+      <c r="E32" s="160"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="157"/>
-      <c r="C33" s="157"/>
+      <c r="B33" s="158"/>
+      <c r="C33" s="158"/>
       <c r="D33" s="17" t="s">
         <v>54</v>
       </c>
@@ -40913,16 +40858,16 @@
       <c r="C34" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D34" s="160" t="s">
+      <c r="D34" s="163" t="s">
         <v>130</v>
       </c>
-      <c r="E34" s="161"/>
+      <c r="E34" s="164"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="162" t="s">
+      <c r="B35" s="161" t="s">
         <v>128</v>
       </c>
-      <c r="C35" s="163" t="s">
+      <c r="C35" s="162" t="s">
         <v>53</v>
       </c>
       <c r="D35" s="16" t="s">
@@ -40933,8 +40878,8 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="162"/>
-      <c r="C36" s="163"/>
+      <c r="B36" s="161"/>
+      <c r="C36" s="162"/>
       <c r="D36" s="16" t="s">
         <v>58</v>
       </c>
@@ -40943,8 +40888,8 @@
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="162"/>
-      <c r="C37" s="163"/>
+      <c r="B37" s="161"/>
+      <c r="C37" s="162"/>
       <c r="D37" s="16" t="s">
         <v>170</v>
       </c>
@@ -40953,8 +40898,8 @@
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="162"/>
-      <c r="C38" s="163"/>
+      <c r="B38" s="161"/>
+      <c r="C38" s="162"/>
       <c r="D38" s="16" t="s">
         <v>131</v>
       </c>
@@ -40964,6 +40909,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -40977,18 +40934,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="C7:C12"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -41017,21 +40962,21 @@
   <sheetData>
     <row r="4" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="156" t="s">
+      <c r="C4" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="158" t="s">
+      <c r="D4" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="159"/>
+      <c r="E4" s="160"/>
     </row>
     <row r="5" spans="1:5" s="5" customFormat="1" ht="23.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="157"/>
-      <c r="C5" s="157"/>
+      <c r="B5" s="158"/>
+      <c r="C5" s="158"/>
       <c r="D5" s="17" t="s">
         <v>54</v>
       </c>
@@ -41189,20 +41134,20 @@
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" ht="23.25">
-      <c r="B25" s="156" t="s">
+      <c r="B25" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="156" t="s">
+      <c r="C25" s="157" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="158" t="s">
+      <c r="D25" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="159"/>
+      <c r="E25" s="160"/>
     </row>
     <row r="26" spans="1:5" ht="23.25">
-      <c r="B26" s="157"/>
-      <c r="C26" s="157"/>
+      <c r="B26" s="158"/>
+      <c r="C26" s="158"/>
       <c r="D26" s="17" t="s">
         <v>54</v>
       </c>
@@ -41217,16 +41162,16 @@
       <c r="C27" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="160" t="s">
+      <c r="D27" s="163" t="s">
         <v>134</v>
       </c>
-      <c r="E27" s="161"/>
+      <c r="E27" s="164"/>
     </row>
     <row r="28" spans="1:5" ht="23.25" customHeight="1">
-      <c r="B28" s="162" t="s">
+      <c r="B28" s="161" t="s">
         <v>132</v>
       </c>
-      <c r="C28" s="163" t="s">
+      <c r="C28" s="162" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="16" t="s">
@@ -41235,24 +41180,24 @@
       <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:5" ht="23.25">
-      <c r="B29" s="162"/>
-      <c r="C29" s="163"/>
+      <c r="B29" s="161"/>
+      <c r="C29" s="162"/>
       <c r="D29" s="16" t="s">
         <v>58</v>
       </c>
       <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:5" ht="23.25">
-      <c r="B30" s="162"/>
-      <c r="C30" s="163"/>
+      <c r="B30" s="161"/>
+      <c r="C30" s="162"/>
       <c r="D30" s="16" t="s">
         <v>59</v>
       </c>
       <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5" ht="23.25">
-      <c r="B31" s="162"/>
-      <c r="C31" s="163"/>
+      <c r="B31" s="161"/>
+      <c r="C31" s="162"/>
       <c r="D31" s="16" t="s">
         <v>210</v>
       </c>
@@ -41260,17 +41205,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B6:B11"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="C28:C31"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="B6:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>